<commit_message>
Target GUI -> Target GUI Model
</commit_message>
<xml_diff>
--- a/documentation/VD/source/procedures.xlsx
+++ b/documentation/VD/source/procedures.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DF3AA8-E98D-49D8-BF60-4E69F4D9A974}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72B9079-CBFB-42E0-8A7B-DF500BAEF949}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="683" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-48" yWindow="4284" windowWidth="17280" windowHeight="11508" tabRatio="683" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="2" r:id="rId1"/>
@@ -673,9 +673,6 @@
     <t>See @TGUICI_test_02.png .</t>
   </si>
   <si>
-    <t>Click on any component of the **Target GUI**</t>
-  </si>
-  <si>
     <t>API Model Creation</t>
   </si>
   <si>
@@ -962,6 +959,9 @@
   </si>
   <si>
     <t>The verification procedure for SAR4.3.1.6.2 Show Relevant Actions passes.</t>
+  </si>
+  <si>
+    <t>Click on any component of the **Target GUI Model**</t>
   </si>
 </sst>
 </file>
@@ -1317,20 +1317,98 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1359,15 +1437,6 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1377,89 +1446,20 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1747,836 +1747,854 @@
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="3.20703125" customWidth="1"/>
+    <col min="2" max="2" width="3.21875" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="15.89453125" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.3" x14ac:dyDescent="0.7">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="25"/>
-    </row>
-    <row r="2" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="26" t="s">
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="51"/>
+    </row>
+    <row r="2" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="28"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="26"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="28"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="28"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="26"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="28"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="26"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="28"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="26"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="28"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="26"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="28"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="26"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="28"/>
-    </row>
-    <row r="10" spans="1:9" ht="18.3" x14ac:dyDescent="0.7">
-      <c r="A10" s="29" t="s">
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="54"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="52"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="54"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="52"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="54"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="52"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="54"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="52"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="54"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="52"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="54"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="52"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="54"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="52"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="54"/>
+    </row>
+    <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A10" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="31"/>
-    </row>
-    <row r="11" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="32" t="s">
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="57"/>
+    </row>
+    <row r="11" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="34"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="32"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="34"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="32"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="34"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="32"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="34"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="32"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="34"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="32"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="34"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="32"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="34"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="32"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="34"/>
-    </row>
-    <row r="19" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="20">
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="26"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="24"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="26"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="24"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="26"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="24"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="26"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="24"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="26"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="24"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="26"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="24"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="26"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="24"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="26"/>
+    </row>
+    <row r="19" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="63">
         <v>1</v>
       </c>
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="37"/>
-    </row>
-    <row r="20" spans="1:9" ht="20.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="21"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="59"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="60"/>
+    </row>
+    <row r="20" spans="1:9" ht="20.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="64"/>
       <c r="B20" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="38" t="s">
+      <c r="D20" s="62"/>
+      <c r="E20" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="39"/>
-    </row>
-    <row r="21" spans="1:9" ht="23.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="21"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="23"/>
+    </row>
+    <row r="21" spans="1:9" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="64"/>
       <c r="B21" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="38" t="s">
+      <c r="D21" s="62"/>
+      <c r="E21" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="39"/>
-    </row>
-    <row r="22" spans="1:9" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="21"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="23"/>
+    </row>
+    <row r="22" spans="1:9" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="64"/>
       <c r="B22" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="19"/>
-      <c r="E22" s="38" t="s">
+      <c r="D22" s="62"/>
+      <c r="E22" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="39"/>
-    </row>
-    <row r="23" spans="1:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="21"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="23"/>
+    </row>
+    <row r="23" spans="1:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="64"/>
       <c r="B23" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="38" t="s">
+      <c r="D23" s="62"/>
+      <c r="E23" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="39"/>
-    </row>
-    <row r="24" spans="1:9" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="21"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="23"/>
+    </row>
+    <row r="24" spans="1:9" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="64"/>
       <c r="B24" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="19"/>
-      <c r="E24" s="38" t="s">
+      <c r="D24" s="62"/>
+      <c r="E24" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="39"/>
-    </row>
-    <row r="25" spans="1:9" ht="50.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="21"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="23"/>
+    </row>
+    <row r="25" spans="1:9" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="64"/>
       <c r="B25" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="19"/>
-      <c r="E25" s="38" t="s">
+      <c r="D25" s="62"/>
+      <c r="E25" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="39"/>
-    </row>
-    <row r="26" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="21"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="23"/>
+    </row>
+    <row r="26" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="64"/>
       <c r="B26" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="38" t="s">
+      <c r="D26" s="62"/>
+      <c r="E26" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="39"/>
-    </row>
-    <row r="27" spans="1:9" ht="73.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="21"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="23"/>
+    </row>
+    <row r="27" spans="1:9" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="64"/>
       <c r="B27" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="38" t="s">
+      <c r="D27" s="62"/>
+      <c r="E27" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="39"/>
-    </row>
-    <row r="28" spans="1:9" ht="33.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="21"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="23"/>
+    </row>
+    <row r="28" spans="1:9" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="64"/>
       <c r="B28" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="19"/>
-      <c r="E28" s="38" t="s">
+      <c r="D28" s="62"/>
+      <c r="E28" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="F28" s="40"/>
-      <c r="G28" s="40"/>
-      <c r="H28" s="40"/>
-      <c r="I28" s="41"/>
-    </row>
-    <row r="29" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="22"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="46"/>
+    </row>
+    <row r="29" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="65"/>
       <c r="B29" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="19"/>
-      <c r="E29" s="42" t="s">
+      <c r="D29" s="62"/>
+      <c r="E29" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="44"/>
-    </row>
-    <row r="30" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A30" s="45">
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="48"/>
+    </row>
+    <row r="30" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="30">
         <v>2</v>
       </c>
-      <c r="B30" s="49" t="s">
+      <c r="B30" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="49"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="49"/>
-      <c r="H30" s="49"/>
-      <c r="I30" s="50"/>
-    </row>
-    <row r="31" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="46"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="20"/>
+    </row>
+    <row r="31" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="31"/>
       <c r="B31" s="9"/>
-      <c r="C31" s="51" t="s">
+      <c r="C31" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="39"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="46"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="23"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="31"/>
       <c r="B32" s="9"/>
-      <c r="C32" s="32"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="34"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="46"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="26"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="31"/>
       <c r="B33" s="9"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="34"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="46"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="26"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="31"/>
       <c r="B34" s="9"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="33"/>
-      <c r="I34" s="34"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="46"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="26"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="31"/>
       <c r="B35" s="9"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="33"/>
-      <c r="H35" s="33"/>
-      <c r="I35" s="34"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="46"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="25"/>
+      <c r="I35" s="26"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="31"/>
       <c r="B36" s="9"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="33"/>
-      <c r="G36" s="33"/>
-      <c r="H36" s="33"/>
-      <c r="I36" s="34"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="46"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="26"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="31"/>
       <c r="B37" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="63" t="s">
+      <c r="C37" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="64"/>
-      <c r="E37" s="64"/>
-      <c r="F37" s="64"/>
-      <c r="G37" s="64"/>
-      <c r="H37" s="64"/>
-      <c r="I37" s="65"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="46"/>
+      <c r="D37" s="43"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="43"/>
+      <c r="G37" s="43"/>
+      <c r="H37" s="43"/>
+      <c r="I37" s="44"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="31"/>
       <c r="B38" s="11"/>
       <c r="C38" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D38" s="51" t="s">
+      <c r="D38" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="E38" s="38"/>
-      <c r="F38" s="38"/>
-      <c r="G38" s="38"/>
-      <c r="H38" s="38"/>
-      <c r="I38" s="39"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="46"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="23"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="31"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="33"/>
-      <c r="F39" s="33"/>
-      <c r="G39" s="33"/>
-      <c r="H39" s="33"/>
-      <c r="I39" s="34"/>
-    </row>
-    <row r="40" spans="1:9" ht="18.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="46"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="26"/>
+    </row>
+    <row r="40" spans="1:9" ht="18.3" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="31"/>
       <c r="B40" s="11"/>
       <c r="C40" s="14"/>
-      <c r="D40" s="52"/>
-      <c r="E40" s="53"/>
-      <c r="F40" s="53"/>
-      <c r="G40" s="53"/>
-      <c r="H40" s="53"/>
-      <c r="I40" s="54"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="46"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="28"/>
+      <c r="G40" s="28"/>
+      <c r="H40" s="28"/>
+      <c r="I40" s="29"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="31"/>
       <c r="B41" s="11"/>
       <c r="C41" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D41" s="58" t="s">
+      <c r="D41" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="E41" s="42"/>
-      <c r="F41" s="42"/>
-      <c r="G41" s="42"/>
-      <c r="H41" s="42"/>
-      <c r="I41" s="59"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="47"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="37"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="37"/>
+      <c r="I41" s="38"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="32"/>
       <c r="B42" s="14"/>
       <c r="C42" s="14"/>
-      <c r="D42" s="60"/>
-      <c r="E42" s="61"/>
-      <c r="F42" s="61"/>
-      <c r="G42" s="61"/>
-      <c r="H42" s="61"/>
-      <c r="I42" s="62"/>
-    </row>
-    <row r="43" spans="1:9" ht="18.3" x14ac:dyDescent="0.7">
-      <c r="A43" s="45">
+      <c r="D42" s="39"/>
+      <c r="E42" s="40"/>
+      <c r="F42" s="40"/>
+      <c r="G42" s="40"/>
+      <c r="H42" s="40"/>
+      <c r="I42" s="41"/>
+    </row>
+    <row r="43" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A43" s="30">
         <v>3</v>
       </c>
-      <c r="B43" s="48" t="s">
+      <c r="B43" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="C43" s="49"/>
-      <c r="D43" s="49"/>
-      <c r="E43" s="49"/>
-      <c r="F43" s="49"/>
-      <c r="G43" s="49"/>
-      <c r="H43" s="49"/>
-      <c r="I43" s="50"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="46"/>
-      <c r="B44" s="56" t="s">
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="20"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="31"/>
+      <c r="B44" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="C44" s="55" t="s">
+      <c r="C44" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="D44" s="51" t="s">
+      <c r="D44" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="E44" s="38"/>
-      <c r="F44" s="38"/>
-      <c r="G44" s="38"/>
-      <c r="H44" s="38"/>
-      <c r="I44" s="39"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="46"/>
-      <c r="B45" s="56"/>
-      <c r="C45" s="56"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="33"/>
-      <c r="F45" s="33"/>
-      <c r="G45" s="33"/>
-      <c r="H45" s="33"/>
-      <c r="I45" s="34"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="46"/>
-      <c r="B46" s="56"/>
-      <c r="C46" s="57"/>
-      <c r="D46" s="52"/>
-      <c r="E46" s="53"/>
-      <c r="F46" s="53"/>
-      <c r="G46" s="53"/>
-      <c r="H46" s="53"/>
-      <c r="I46" s="54"/>
-    </row>
-    <row r="47" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="46"/>
-      <c r="B47" s="56" t="s">
+      <c r="E44" s="22"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="23"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="31"/>
+      <c r="B45" s="33"/>
+      <c r="C45" s="33"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="25"/>
+      <c r="G45" s="25"/>
+      <c r="H45" s="25"/>
+      <c r="I45" s="26"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="31"/>
+      <c r="B46" s="33"/>
+      <c r="C46" s="34"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="28"/>
+      <c r="G46" s="28"/>
+      <c r="H46" s="28"/>
+      <c r="I46" s="29"/>
+    </row>
+    <row r="47" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="31"/>
+      <c r="B47" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C47" s="55" t="s">
+      <c r="C47" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="D47" s="51" t="s">
+      <c r="D47" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="E47" s="38"/>
-      <c r="F47" s="38"/>
-      <c r="G47" s="38"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="39"/>
-    </row>
-    <row r="48" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="46"/>
-      <c r="B48" s="56"/>
-      <c r="C48" s="56"/>
-      <c r="D48" s="32"/>
-      <c r="E48" s="33"/>
-      <c r="F48" s="33"/>
-      <c r="G48" s="33"/>
-      <c r="H48" s="33"/>
-      <c r="I48" s="34"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="46"/>
-      <c r="B49" s="56"/>
-      <c r="C49" s="57"/>
-      <c r="D49" s="52"/>
-      <c r="E49" s="53"/>
-      <c r="F49" s="53"/>
-      <c r="G49" s="53"/>
-      <c r="H49" s="53"/>
-      <c r="I49" s="54"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="46"/>
-      <c r="B50" s="56" t="s">
+      <c r="E47" s="22"/>
+      <c r="F47" s="22"/>
+      <c r="G47" s="22"/>
+      <c r="H47" s="22"/>
+      <c r="I47" s="23"/>
+    </row>
+    <row r="48" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="31"/>
+      <c r="B48" s="33"/>
+      <c r="C48" s="33"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="25"/>
+      <c r="F48" s="25"/>
+      <c r="G48" s="25"/>
+      <c r="H48" s="25"/>
+      <c r="I48" s="26"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="31"/>
+      <c r="B49" s="33"/>
+      <c r="C49" s="34"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="28"/>
+      <c r="G49" s="28"/>
+      <c r="H49" s="28"/>
+      <c r="I49" s="29"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="31"/>
+      <c r="B50" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="C50" s="56" t="s">
+      <c r="C50" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="D50" s="51" t="s">
+      <c r="D50" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="E50" s="38"/>
-      <c r="F50" s="38"/>
-      <c r="G50" s="38"/>
-      <c r="H50" s="38"/>
-      <c r="I50" s="39"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="46"/>
-      <c r="B51" s="56"/>
-      <c r="C51" s="56"/>
-      <c r="D51" s="32"/>
-      <c r="E51" s="33"/>
-      <c r="F51" s="33"/>
-      <c r="G51" s="33"/>
-      <c r="H51" s="33"/>
-      <c r="I51" s="34"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="47"/>
-      <c r="B52" s="57"/>
-      <c r="C52" s="57"/>
-      <c r="D52" s="52"/>
-      <c r="E52" s="53"/>
-      <c r="F52" s="53"/>
-      <c r="G52" s="53"/>
-      <c r="H52" s="53"/>
-      <c r="I52" s="54"/>
-    </row>
-    <row r="53" spans="1:9" ht="18.3" x14ac:dyDescent="0.7">
-      <c r="A53" s="45">
+      <c r="E50" s="22"/>
+      <c r="F50" s="22"/>
+      <c r="G50" s="22"/>
+      <c r="H50" s="22"/>
+      <c r="I50" s="23"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="31"/>
+      <c r="B51" s="33"/>
+      <c r="C51" s="33"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="25"/>
+      <c r="F51" s="25"/>
+      <c r="G51" s="25"/>
+      <c r="H51" s="25"/>
+      <c r="I51" s="26"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="32"/>
+      <c r="B52" s="34"/>
+      <c r="C52" s="34"/>
+      <c r="D52" s="27"/>
+      <c r="E52" s="28"/>
+      <c r="F52" s="28"/>
+      <c r="G52" s="28"/>
+      <c r="H52" s="28"/>
+      <c r="I52" s="29"/>
+    </row>
+    <row r="53" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A53" s="30">
         <v>4</v>
       </c>
-      <c r="B53" s="48" t="s">
+      <c r="B53" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C53" s="49"/>
-      <c r="D53" s="49"/>
-      <c r="E53" s="49"/>
-      <c r="F53" s="49"/>
-      <c r="G53" s="49"/>
-      <c r="H53" s="49"/>
-      <c r="I53" s="50"/>
-    </row>
-    <row r="54" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="46"/>
-      <c r="B54" s="46" t="s">
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="19"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="19"/>
+      <c r="I53" s="20"/>
+    </row>
+    <row r="54" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="31"/>
+      <c r="B54" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C54" s="51" t="s">
+      <c r="C54" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D54" s="38"/>
-      <c r="E54" s="38"/>
-      <c r="F54" s="38"/>
-      <c r="G54" s="38"/>
-      <c r="H54" s="38"/>
-      <c r="I54" s="39"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="46"/>
-      <c r="B55" s="46"/>
-      <c r="C55" s="32"/>
-      <c r="D55" s="33"/>
-      <c r="E55" s="33"/>
-      <c r="F55" s="33"/>
-      <c r="G55" s="33"/>
-      <c r="H55" s="33"/>
-      <c r="I55" s="34"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" s="46"/>
-      <c r="B56" s="46"/>
-      <c r="C56" s="32"/>
-      <c r="D56" s="33"/>
-      <c r="E56" s="33"/>
-      <c r="F56" s="33"/>
-      <c r="G56" s="33"/>
-      <c r="H56" s="33"/>
-      <c r="I56" s="34"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="46"/>
-      <c r="B57" s="46"/>
-      <c r="C57" s="32"/>
-      <c r="D57" s="33"/>
-      <c r="E57" s="33"/>
-      <c r="F57" s="33"/>
-      <c r="G57" s="33"/>
-      <c r="H57" s="33"/>
-      <c r="I57" s="34"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" s="46"/>
-      <c r="B58" s="46"/>
-      <c r="C58" s="32"/>
-      <c r="D58" s="33"/>
-      <c r="E58" s="33"/>
-      <c r="F58" s="33"/>
-      <c r="G58" s="33"/>
-      <c r="H58" s="33"/>
-      <c r="I58" s="34"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="46"/>
-      <c r="B59" s="46"/>
-      <c r="C59" s="32"/>
-      <c r="D59" s="33"/>
-      <c r="E59" s="33"/>
-      <c r="F59" s="33"/>
-      <c r="G59" s="33"/>
-      <c r="H59" s="33"/>
-      <c r="I59" s="34"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" s="46"/>
-      <c r="B60" s="46"/>
-      <c r="C60" s="32"/>
-      <c r="D60" s="33"/>
-      <c r="E60" s="33"/>
-      <c r="F60" s="33"/>
-      <c r="G60" s="33"/>
-      <c r="H60" s="33"/>
-      <c r="I60" s="34"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61" s="46"/>
-      <c r="B61" s="46"/>
-      <c r="C61" s="32"/>
-      <c r="D61" s="33"/>
-      <c r="E61" s="33"/>
-      <c r="F61" s="33"/>
-      <c r="G61" s="33"/>
-      <c r="H61" s="33"/>
-      <c r="I61" s="34"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="46"/>
-      <c r="B62" s="46"/>
-      <c r="C62" s="32"/>
-      <c r="D62" s="33"/>
-      <c r="E62" s="33"/>
-      <c r="F62" s="33"/>
-      <c r="G62" s="33"/>
-      <c r="H62" s="33"/>
-      <c r="I62" s="34"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" s="47"/>
-      <c r="B63" s="47"/>
-      <c r="C63" s="52"/>
-      <c r="D63" s="53"/>
-      <c r="E63" s="53"/>
-      <c r="F63" s="53"/>
-      <c r="G63" s="53"/>
-      <c r="H63" s="53"/>
-      <c r="I63" s="54"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="22"/>
+      <c r="F54" s="22"/>
+      <c r="G54" s="22"/>
+      <c r="H54" s="22"/>
+      <c r="I54" s="23"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="31"/>
+      <c r="B55" s="31"/>
+      <c r="C55" s="24"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="25"/>
+      <c r="F55" s="25"/>
+      <c r="G55" s="25"/>
+      <c r="H55" s="25"/>
+      <c r="I55" s="26"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="31"/>
+      <c r="B56" s="31"/>
+      <c r="C56" s="24"/>
+      <c r="D56" s="25"/>
+      <c r="E56" s="25"/>
+      <c r="F56" s="25"/>
+      <c r="G56" s="25"/>
+      <c r="H56" s="25"/>
+      <c r="I56" s="26"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="31"/>
+      <c r="B57" s="31"/>
+      <c r="C57" s="24"/>
+      <c r="D57" s="25"/>
+      <c r="E57" s="25"/>
+      <c r="F57" s="25"/>
+      <c r="G57" s="25"/>
+      <c r="H57" s="25"/>
+      <c r="I57" s="26"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="31"/>
+      <c r="B58" s="31"/>
+      <c r="C58" s="24"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="25"/>
+      <c r="F58" s="25"/>
+      <c r="G58" s="25"/>
+      <c r="H58" s="25"/>
+      <c r="I58" s="26"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" s="31"/>
+      <c r="B59" s="31"/>
+      <c r="C59" s="24"/>
+      <c r="D59" s="25"/>
+      <c r="E59" s="25"/>
+      <c r="F59" s="25"/>
+      <c r="G59" s="25"/>
+      <c r="H59" s="25"/>
+      <c r="I59" s="26"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="31"/>
+      <c r="B60" s="31"/>
+      <c r="C60" s="24"/>
+      <c r="D60" s="25"/>
+      <c r="E60" s="25"/>
+      <c r="F60" s="25"/>
+      <c r="G60" s="25"/>
+      <c r="H60" s="25"/>
+      <c r="I60" s="26"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" s="31"/>
+      <c r="B61" s="31"/>
+      <c r="C61" s="24"/>
+      <c r="D61" s="25"/>
+      <c r="E61" s="25"/>
+      <c r="F61" s="25"/>
+      <c r="G61" s="25"/>
+      <c r="H61" s="25"/>
+      <c r="I61" s="26"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" s="31"/>
+      <c r="B62" s="31"/>
+      <c r="C62" s="24"/>
+      <c r="D62" s="25"/>
+      <c r="E62" s="25"/>
+      <c r="F62" s="25"/>
+      <c r="G62" s="25"/>
+      <c r="H62" s="25"/>
+      <c r="I62" s="26"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" s="32"/>
+      <c r="B63" s="32"/>
+      <c r="C63" s="27"/>
+      <c r="D63" s="28"/>
+      <c r="E63" s="28"/>
+      <c r="F63" s="28"/>
+      <c r="G63" s="28"/>
+      <c r="H63" s="28"/>
+      <c r="I63" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="B53:I53"/>
-    <mergeCell ref="C54:I63"/>
-    <mergeCell ref="A53:A63"/>
-    <mergeCell ref="B54:B63"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="A43:A52"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="A19:A29"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I9"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A11:I18"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="E29:I29"/>
     <mergeCell ref="A30:A42"/>
     <mergeCell ref="B43:I43"/>
     <mergeCell ref="D47:I49"/>
@@ -2590,32 +2608,14 @@
     <mergeCell ref="D44:I46"/>
     <mergeCell ref="B30:I30"/>
     <mergeCell ref="C37:I37"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="E28:I28"/>
-    <mergeCell ref="E29:I29"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I9"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A11:I18"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="A19:A29"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="B53:I53"/>
+    <mergeCell ref="C54:I63"/>
+    <mergeCell ref="A53:A63"/>
+    <mergeCell ref="B54:B63"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="A43:A52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2626,25 +2626,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE9DEC4C-0859-492A-9859-A5102CF1C24C}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView topLeftCell="C13" workbookViewId="0">
+    <sheetView topLeftCell="D15" workbookViewId="0">
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.20703125" customWidth="1"/>
-    <col min="2" max="2" width="46.5234375" customWidth="1"/>
-    <col min="3" max="3" width="18.5234375" customWidth="1"/>
-    <col min="4" max="4" width="18.20703125" customWidth="1"/>
-    <col min="5" max="5" width="17.68359375" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="2" max="2" width="46.5546875" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="23.20703125" customWidth="1"/>
-    <col min="8" max="8" width="27.3125" customWidth="1"/>
-    <col min="9" max="9" width="19.20703125" customWidth="1"/>
-    <col min="10" max="10" width="44.3125" customWidth="1"/>
+    <col min="7" max="7" width="23.21875" customWidth="1"/>
+    <col min="8" max="8" width="27.33203125" customWidth="1"/>
+    <col min="9" max="9" width="19.21875" customWidth="1"/>
+    <col min="10" max="10" width="44.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="61.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2676,12 +2676,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="171.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="171.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -2690,25 +2690,25 @@
         <v>10</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>299</v>
-      </c>
       <c r="I2" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2718,19 +2718,19 @@
         <v>13</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>301</v>
-      </c>
       <c r="I3" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2746,13 +2746,13 @@
         <v>183</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2766,13 +2766,13 @@
         <v>70</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2786,13 +2786,13 @@
         <v>84</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="99.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2806,13 +2806,13 @@
         <v>21</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -2828,7 +2828,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2844,7 +2844,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2860,7 +2860,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2876,7 +2876,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2892,7 +2892,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2908,7 +2908,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -2916,132 +2916,132 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>215</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:10" ht="101.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" ht="101.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G15" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="H15" s="2" t="s">
+    </row>
+    <row r="16" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="G16" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="G17" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="18" spans="7:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="G18" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="19" spans="7:8" ht="103.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G19" s="2" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="G16" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="17" spans="7:8" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="G17" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="18" spans="7:8" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="G18" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="19" spans="7:8" ht="103.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="G19" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="H19" s="2" t="s">
+    </row>
+    <row r="20" spans="7:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="G20" s="2" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="20" spans="7:8" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="G20" s="2" t="s">
+      <c r="H20" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="H20" s="2" t="s">
+    </row>
+    <row r="21" spans="7:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="G21" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="22" spans="7:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G22" s="2" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="21" spans="7:8" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="G21" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="22" spans="7:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="G22" s="2" t="s">
-        <v>228</v>
-      </c>
       <c r="H22" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="23" spans="7:8" ht="144" x14ac:dyDescent="0.3">
+      <c r="G23" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="23" spans="7:8" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="G23" s="2" t="s">
+    <row r="24" spans="7:8" ht="144" x14ac:dyDescent="0.3">
+      <c r="G24" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="H23" s="2" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="24" spans="7:8" ht="144" x14ac:dyDescent="0.55000000000000004">
-      <c r="G24" s="2" t="s">
+      <c r="H24" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="25" spans="7:8" ht="144" x14ac:dyDescent="0.3">
+      <c r="G25" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="26" spans="7:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G26" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="27" spans="7:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G27" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="28" spans="7:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="G28" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="29" spans="7:8" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="G29" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="H24" s="2" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="25" spans="7:8" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="G25" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="26" spans="7:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="G26" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="27" spans="7:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="G27" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="28" spans="7:8" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="G28" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="H28" s="2" t="s">
+      <c r="H29" s="2" t="s">
         <v>273</v>
-      </c>
-    </row>
-    <row r="29" spans="7:8" ht="115.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="G29" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -3054,25 +3054,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D9C558-86BD-4789-80C1-D36E81752C81}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView topLeftCell="D12" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.89453125" customWidth="1"/>
-    <col min="2" max="2" width="38.5234375" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="2" max="2" width="38.5546875" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="16.89453125" customWidth="1"/>
-    <col min="5" max="5" width="20.41796875" customWidth="1"/>
-    <col min="6" max="6" width="19.7890625" customWidth="1"/>
-    <col min="7" max="7" width="23.89453125" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" customWidth="1"/>
+    <col min="6" max="6" width="19.77734375" customWidth="1"/>
+    <col min="7" max="7" width="23.88671875" customWidth="1"/>
     <col min="8" max="8" width="27" customWidth="1"/>
-    <col min="9" max="9" width="23.68359375" customWidth="1"/>
-    <col min="10" max="10" width="33.68359375" customWidth="1"/>
+    <col min="9" max="9" width="23.6640625" customWidth="1"/>
+    <col min="10" max="10" width="33.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="57.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3104,12 +3104,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="165" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="165" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -3118,7 +3118,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>12</v>
@@ -3130,13 +3130,13 @@
         <v>183</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="J2" s="8" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="123.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="3" spans="1:10" ht="123.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -3152,13 +3152,13 @@
         <v>70</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -3174,13 +3174,13 @@
         <v>84</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -3196,7 +3196,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -3212,7 +3212,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3228,7 +3228,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -3244,7 +3244,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3260,7 +3260,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -3276,7 +3276,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -3287,12 +3287,12 @@
         <v>82</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -3300,15 +3300,15 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -3316,70 +3316,70 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>223</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="G14" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>217</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:10" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="G15" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="H15" s="2" t="s">
+    </row>
+    <row r="16" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="G16" s="2" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="G16" s="2" t="s">
+      <c r="H16" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="H16" s="16" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="17" spans="7:8" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="17" spans="7:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="G17" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="H17" s="2" t="s">
+    </row>
+    <row r="18" spans="7:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="G18" s="2" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="18" spans="7:8" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="G18" s="2" t="s">
+      <c r="H18" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="H18" s="2" t="s">
+    </row>
+    <row r="19" spans="7:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="G19" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="20" spans="7:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="G20" s="2" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="19" spans="7:8" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="G19" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="20" spans="7:8" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="G20" s="2" t="s">
-        <v>228</v>
-      </c>
       <c r="H20" s="16" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -3391,25 +3391,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE0C746B-3182-4B37-8AF4-A9D404711DCD}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView topLeftCell="B16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F16" workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.1015625" customWidth="1"/>
-    <col min="2" max="2" width="34.7890625" customWidth="1"/>
-    <col min="3" max="3" width="18.89453125" customWidth="1"/>
-    <col min="4" max="4" width="15.41796875" customWidth="1"/>
-    <col min="5" max="5" width="21.68359375" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="34.77734375" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="7" width="17.41796875" customWidth="1"/>
-    <col min="8" max="8" width="16.41796875" customWidth="1"/>
-    <col min="9" max="9" width="27.41796875" customWidth="1"/>
-    <col min="10" max="10" width="17.68359375" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" customWidth="1"/>
+    <col min="9" max="9" width="27.44140625" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3441,12 +3441,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="225" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="225" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -3455,7 +3455,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>12</v>
@@ -3467,13 +3467,13 @@
         <v>183</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="J2" s="8" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -3491,7 +3491,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -3509,7 +3509,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -3525,7 +3525,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -3541,7 +3541,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3557,7 +3557,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -3573,7 +3573,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3589,7 +3589,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -3605,7 +3605,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -3616,12 +3616,12 @@
         <v>82</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -3629,15 +3629,15 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -3645,60 +3645,60 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>223</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="G14" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="H14" s="2" t="s">
+    </row>
+    <row r="15" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="G15" s="2" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="G15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="H15" s="2" t="s">
+    </row>
+    <row r="16" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="G16" s="2" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="G16" s="2" t="s">
-        <v>220</v>
-      </c>
       <c r="H16" s="16" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="G17" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="18" spans="7:8" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="G18" s="2" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="17" spans="7:8" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="G17" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="18" spans="7:8" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="G18" s="2" t="s">
-        <v>234</v>
-      </c>
       <c r="H18" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="19" spans="7:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="G19" s="2" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="19" spans="7:8" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="G19" s="2" t="s">
-        <v>228</v>
-      </c>
       <c r="H19" s="16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -3714,21 +3714,21 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.41796875" customWidth="1"/>
-    <col min="2" max="2" width="28.68359375" customWidth="1"/>
-    <col min="3" max="3" width="17.89453125" customWidth="1"/>
-    <col min="4" max="4" width="17.41796875" customWidth="1"/>
-    <col min="5" max="5" width="20.5234375" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="20.5546875" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="7" width="15.20703125" customWidth="1"/>
-    <col min="8" max="8" width="16.41796875" customWidth="1"/>
-    <col min="9" max="9" width="18.89453125" customWidth="1"/>
-    <col min="10" max="10" width="17.41796875" customWidth="1"/>
+    <col min="7" max="7" width="15.21875" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" customWidth="1"/>
+    <col min="10" max="10" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="61.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3760,12 +3760,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="295.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="295.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -3774,7 +3774,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>12</v>
@@ -3786,13 +3786,13 @@
         <v>183</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="J2" s="8" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="3" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -3810,7 +3810,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -3828,7 +3828,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -3844,7 +3844,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -3860,7 +3860,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3876,7 +3876,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -3892,7 +3892,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3908,7 +3908,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -3924,7 +3924,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -3935,12 +3935,12 @@
         <v>82</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -3948,15 +3948,15 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -3968,7 +3968,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
@@ -3985,21 +3985,21 @@
       <selection activeCell="I4" sqref="I4:J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.5234375" customWidth="1"/>
-    <col min="2" max="2" width="55.3125" customWidth="1"/>
-    <col min="3" max="3" width="25.89453125" customWidth="1"/>
-    <col min="4" max="4" width="26.7890625" customWidth="1"/>
+    <col min="1" max="1" width="39.5546875" customWidth="1"/>
+    <col min="2" max="2" width="55.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" customWidth="1"/>
+    <col min="4" max="4" width="26.77734375" customWidth="1"/>
     <col min="5" max="5" width="33" customWidth="1"/>
-    <col min="6" max="6" width="32.41796875" customWidth="1"/>
-    <col min="7" max="7" width="24.3125" customWidth="1"/>
-    <col min="8" max="8" width="25.1015625" customWidth="1"/>
-    <col min="9" max="9" width="18.89453125" customWidth="1"/>
-    <col min="10" max="10" width="21.68359375" customWidth="1"/>
+    <col min="6" max="6" width="32.44140625" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" customWidth="1"/>
+    <col min="8" max="8" width="25.109375" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" customWidth="1"/>
+    <col min="10" max="10" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="37.200000000000003" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="55.8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4031,7 +4031,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="216" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="216" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>149</v>
       </c>
@@ -4063,7 +4063,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4085,7 +4085,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -4105,7 +4105,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -4121,7 +4121,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -4137,7 +4137,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4153,7 +4153,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -4169,7 +4169,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -4185,7 +4185,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="216" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -4201,7 +4201,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -4212,12 +4212,12 @@
         <v>150</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -4229,7 +4229,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -4241,13 +4241,13 @@
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="6"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I15" s="6"/>
       <c r="J15" s="8"/>
     </row>
@@ -4264,20 +4264,20 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.68359375" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="29.89453125" customWidth="1"/>
-    <col min="4" max="4" width="24.68359375" customWidth="1"/>
-    <col min="5" max="5" width="28.3125" customWidth="1"/>
-    <col min="6" max="6" width="26.89453125" customWidth="1"/>
-    <col min="7" max="7" width="24.1015625" customWidth="1"/>
-    <col min="8" max="8" width="21.1015625" customWidth="1"/>
-    <col min="9" max="10" width="26.1015625" customWidth="1"/>
+    <col min="3" max="3" width="29.88671875" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" customWidth="1"/>
+    <col min="6" max="6" width="26.88671875" customWidth="1"/>
+    <col min="7" max="7" width="24.109375" customWidth="1"/>
+    <col min="8" max="8" width="21.109375" customWidth="1"/>
+    <col min="9" max="10" width="26.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="55.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="55.8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4309,7 +4309,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="225.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="234.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>154</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="144" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4363,7 +4363,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -4383,7 +4383,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -4403,7 +4403,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -4419,7 +4419,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4435,7 +4435,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -4451,7 +4451,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -4467,7 +4467,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="216" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -4478,12 +4478,12 @@
         <v>80</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="144" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -4499,7 +4499,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -4515,7 +4515,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -4527,13 +4527,13 @@
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="6"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I15" s="6"/>
       <c r="J15" s="8"/>
     </row>
@@ -4547,25 +4547,25 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="77" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5234375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="69.20703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="36.20703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="34.1015625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="69.21875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="36.21875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="34.109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="40" style="2" customWidth="1"/>
-    <col min="6" max="6" width="32.5234375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="46.20703125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="43.68359375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="32.5546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="46.21875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="43.6640625" style="2" customWidth="1"/>
     <col min="9" max="9" width="29" style="2" customWidth="1"/>
-    <col min="10" max="10" width="29.3125" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="8.89453125" style="2"/>
+    <col min="10" max="10" width="29.33203125" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="18.600000000000001" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4597,7 +4597,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="93" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="93" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -4629,7 +4629,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4651,7 +4651,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="48.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -4667,7 +4667,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -4683,7 +4683,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -4699,7 +4699,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4715,7 +4715,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -4731,27 +4731,27 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I14" s="8"/>
     </row>
   </sheetData>
@@ -4765,24 +4765,24 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.3125" customWidth="1"/>
-    <col min="2" max="2" width="68.7890625" customWidth="1"/>
-    <col min="3" max="3" width="16.1015625" customWidth="1"/>
-    <col min="4" max="4" width="19.20703125" customWidth="1"/>
-    <col min="5" max="5" width="38.3125" customWidth="1"/>
-    <col min="6" max="6" width="17.7890625" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="68.77734375" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" customWidth="1"/>
+    <col min="4" max="4" width="19.21875" customWidth="1"/>
+    <col min="5" max="5" width="38.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" customWidth="1"/>
     <col min="7" max="7" width="26" customWidth="1"/>
-    <col min="8" max="8" width="19.5234375" customWidth="1"/>
-    <col min="9" max="9" width="18.7890625" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" customWidth="1"/>
+    <col min="9" max="9" width="18.77734375" customWidth="1"/>
     <col min="10" max="10" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="55.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="55.8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4814,7 +4814,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>74</v>
       </c>
@@ -4846,7 +4846,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4868,7 +4868,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -4884,7 +4884,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -4900,7 +4900,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -4916,7 +4916,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="109.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="109.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4932,7 +4932,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -4948,7 +4948,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -4964,7 +4964,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -4980,7 +4980,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -4996,7 +4996,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -5008,7 +5008,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -5029,25 +5029,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B71E50-493D-4640-A992-202C8A3B64C0}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="F3" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.20703125" customWidth="1"/>
-    <col min="2" max="2" width="53.89453125" customWidth="1"/>
-    <col min="3" max="3" width="28.3125" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="2" max="2" width="53.88671875" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="21.1015625" customWidth="1"/>
-    <col min="6" max="6" width="19.20703125" customWidth="1"/>
-    <col min="7" max="7" width="34.20703125" customWidth="1"/>
-    <col min="8" max="8" width="45.1015625" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" customWidth="1"/>
+    <col min="7" max="7" width="34.21875" customWidth="1"/>
+    <col min="8" max="8" width="45.109375" customWidth="1"/>
     <col min="9" max="9" width="24" customWidth="1"/>
-    <col min="10" max="10" width="22.3125" customWidth="1"/>
+    <col min="10" max="10" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="37.200000000000003" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="37.200000000000003" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -5079,12 +5079,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="207" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="207" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -5099,15 +5099,15 @@
         <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>285</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="8"/>
     </row>
-    <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -5117,15 +5117,15 @@
         <v>13</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>286</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>287</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -5133,15 +5133,15 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>289</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="62.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="62.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -5149,15 +5149,15 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>290</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>291</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="59.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -5165,15 +5165,15 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>292</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="58.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -5181,15 +5181,15 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>295</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="55.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -5197,15 +5197,15 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>296</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>297</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -5217,7 +5217,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -5229,7 +5229,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -5241,7 +5241,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -5253,7 +5253,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -5265,7 +5265,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
@@ -5279,25 +5279,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E612745-E32A-4DF6-8B6E-CDF906DFB81F}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView topLeftCell="P3" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView topLeftCell="C8" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.68359375" customWidth="1"/>
-    <col min="2" max="2" width="52.7890625" customWidth="1"/>
-    <col min="3" max="3" width="18.3125" customWidth="1"/>
-    <col min="4" max="4" width="16.89453125" customWidth="1"/>
-    <col min="5" max="5" width="19.1015625" customWidth="1"/>
-    <col min="6" max="6" width="18.3125" customWidth="1"/>
-    <col min="7" max="7" width="28.41796875" customWidth="1"/>
-    <col min="8" max="8" width="39.41796875" customWidth="1"/>
-    <col min="9" max="9" width="29.5234375" customWidth="1"/>
-    <col min="10" max="10" width="26.20703125" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="52.77734375" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="28.44140625" customWidth="1"/>
+    <col min="8" max="8" width="39.44140625" customWidth="1"/>
+    <col min="9" max="9" width="29.5546875" customWidth="1"/>
+    <col min="10" max="10" width="26.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="37.200000000000003" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="37.200000000000003" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -5329,7 +5329,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="144" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>91</v>
       </c>
@@ -5361,7 +5361,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -5383,7 +5383,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -5401,7 +5401,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -5417,7 +5417,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -5433,7 +5433,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -5449,7 +5449,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -5465,7 +5465,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -5481,7 +5481,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -5497,7 +5497,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -5513,7 +5513,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -5521,7 +5521,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>205</v>
+        <v>301</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>204</v>
@@ -5529,7 +5529,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -5545,7 +5545,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
@@ -5562,21 +5562,21 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.1015625" customWidth="1"/>
-    <col min="2" max="2" width="67.3125" customWidth="1"/>
-    <col min="3" max="3" width="39.7890625" customWidth="1"/>
-    <col min="4" max="4" width="39.89453125" customWidth="1"/>
-    <col min="5" max="5" width="32.41796875" customWidth="1"/>
-    <col min="6" max="6" width="26.1015625" customWidth="1"/>
-    <col min="7" max="7" width="28.20703125" customWidth="1"/>
-    <col min="8" max="8" width="30.1015625" customWidth="1"/>
-    <col min="9" max="9" width="24.68359375" customWidth="1"/>
-    <col min="10" max="10" width="23.7890625" customWidth="1"/>
+    <col min="1" max="1" width="32.109375" customWidth="1"/>
+    <col min="2" max="2" width="67.33203125" customWidth="1"/>
+    <col min="3" max="3" width="39.77734375" customWidth="1"/>
+    <col min="4" max="4" width="39.88671875" customWidth="1"/>
+    <col min="5" max="5" width="32.44140625" customWidth="1"/>
+    <col min="6" max="6" width="26.109375" customWidth="1"/>
+    <col min="7" max="7" width="28.21875" customWidth="1"/>
+    <col min="8" max="8" width="30.109375" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" customWidth="1"/>
+    <col min="10" max="10" width="23.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="37.200000000000003" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="37.200000000000003" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -5608,7 +5608,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="187.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="187.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>100</v>
       </c>
@@ -5640,7 +5640,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -5662,7 +5662,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -5680,7 +5680,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -5696,7 +5696,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -5712,7 +5712,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -5728,7 +5728,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -5744,7 +5744,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -5760,7 +5760,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -5776,7 +5776,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -5792,7 +5792,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -5808,7 +5808,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -5824,7 +5824,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="G14" s="2" t="s">
         <v>103</v>
       </c>
@@ -5832,7 +5832,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="G15" s="2" t="s">
         <v>104</v>
       </c>
@@ -5840,7 +5840,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="G16" s="2" t="s">
         <v>105</v>
       </c>
@@ -5848,7 +5848,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="17" spans="7:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="7:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="G17" s="2" t="s">
         <v>106</v>
       </c>
@@ -5856,7 +5856,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="7:8" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="7:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="G18" s="2" t="s">
         <v>107</v>
       </c>
@@ -5877,21 +5877,21 @@
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.68359375" customWidth="1"/>
-    <col min="2" max="2" width="49.20703125" customWidth="1"/>
-    <col min="3" max="3" width="31.20703125" customWidth="1"/>
-    <col min="4" max="4" width="31.1015625" customWidth="1"/>
-    <col min="5" max="5" width="22.68359375" customWidth="1"/>
-    <col min="6" max="6" width="23.7890625" customWidth="1"/>
-    <col min="7" max="7" width="19.7890625" customWidth="1"/>
-    <col min="8" max="8" width="23.41796875" customWidth="1"/>
-    <col min="9" max="9" width="28.20703125" customWidth="1"/>
-    <col min="10" max="10" width="32.5234375" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="2" max="2" width="49.21875" customWidth="1"/>
+    <col min="3" max="3" width="31.21875" customWidth="1"/>
+    <col min="4" max="4" width="31.109375" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23.77734375" customWidth="1"/>
+    <col min="7" max="7" width="19.77734375" customWidth="1"/>
+    <col min="8" max="8" width="23.44140625" customWidth="1"/>
+    <col min="9" max="9" width="28.21875" customWidth="1"/>
+    <col min="10" max="10" width="32.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -5923,7 +5923,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="141" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="151.80000000000001" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>120</v>
       </c>
@@ -5955,7 +5955,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -5977,7 +5977,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -5993,7 +5993,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -6009,7 +6009,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -6025,7 +6025,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -6041,7 +6041,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -6057,7 +6057,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -6073,7 +6073,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="230.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -6089,7 +6089,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -6105,7 +6105,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -6121,7 +6121,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -6137,7 +6137,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
@@ -6154,21 +6154,21 @@
       <selection activeCell="G10" sqref="G10:H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.68359375" customWidth="1"/>
-    <col min="2" max="2" width="63.5234375" customWidth="1"/>
-    <col min="3" max="3" width="33.3125" customWidth="1"/>
-    <col min="4" max="4" width="31.1015625" customWidth="1"/>
-    <col min="5" max="5" width="37.1015625" customWidth="1"/>
-    <col min="6" max="6" width="30.1015625" customWidth="1"/>
+    <col min="1" max="1" width="37.6640625" customWidth="1"/>
+    <col min="2" max="2" width="63.5546875" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" customWidth="1"/>
+    <col min="4" max="4" width="31.109375" customWidth="1"/>
+    <col min="5" max="5" width="37.109375" customWidth="1"/>
+    <col min="6" max="6" width="30.109375" customWidth="1"/>
     <col min="7" max="7" width="30" customWidth="1"/>
-    <col min="8" max="8" width="28.7890625" customWidth="1"/>
-    <col min="9" max="9" width="24.20703125" customWidth="1"/>
-    <col min="10" max="10" width="25.89453125" customWidth="1"/>
+    <col min="8" max="8" width="28.77734375" customWidth="1"/>
+    <col min="9" max="9" width="24.21875" customWidth="1"/>
+    <col min="10" max="10" width="25.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="37.200000000000003" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="37.200000000000003" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -6200,7 +6200,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="188.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="188.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>125</v>
       </c>
@@ -6232,7 +6232,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -6250,7 +6250,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -6268,7 +6268,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -6284,7 +6284,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -6300,7 +6300,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -6316,7 +6316,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -6332,7 +6332,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -6348,7 +6348,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -6364,7 +6364,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -6380,7 +6380,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -6396,7 +6396,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -6412,7 +6412,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="G14" s="2" t="s">
         <v>131</v>
       </c>
@@ -6420,7 +6420,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="G15" s="2" t="s">
         <v>135</v>
       </c>
@@ -6428,15 +6428,15 @@
         <v>198</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G16" s="2"/>
       <c r="H16" s="16"/>
     </row>
-    <row r="17" spans="7:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G17" s="2"/>
       <c r="H17" s="16"/>
     </row>
-    <row r="18" spans="7:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G18" s="2"/>
       <c r="H18" s="16"/>
     </row>
@@ -6453,21 +6453,21 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.89453125" customWidth="1"/>
-    <col min="2" max="2" width="50.68359375" customWidth="1"/>
+    <col min="1" max="1" width="30.88671875" customWidth="1"/>
+    <col min="2" max="2" width="50.6640625" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="24.7890625" customWidth="1"/>
-    <col min="5" max="5" width="23.5234375" customWidth="1"/>
-    <col min="6" max="6" width="24.5234375" customWidth="1"/>
+    <col min="4" max="4" width="24.77734375" customWidth="1"/>
+    <col min="5" max="5" width="23.5546875" customWidth="1"/>
+    <col min="6" max="6" width="24.5546875" customWidth="1"/>
     <col min="7" max="7" width="22" customWidth="1"/>
-    <col min="8" max="8" width="24.3125" customWidth="1"/>
-    <col min="9" max="9" width="22.41796875" customWidth="1"/>
-    <col min="10" max="10" width="23.41796875" customWidth="1"/>
+    <col min="8" max="8" width="24.33203125" customWidth="1"/>
+    <col min="9" max="9" width="22.44140625" customWidth="1"/>
+    <col min="10" max="10" width="23.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="37.200000000000003" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="55.8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -6499,7 +6499,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="221.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="221.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>136</v>
       </c>
@@ -6531,7 +6531,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -6549,7 +6549,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -6567,7 +6567,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -6583,7 +6583,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -6599,7 +6599,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -6615,7 +6615,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -6631,7 +6631,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -6647,7 +6647,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -6663,7 +6663,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -6679,7 +6679,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -6695,7 +6695,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -6711,7 +6711,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="G14" s="2" t="s">
         <v>144</v>
       </c>
@@ -6719,7 +6719,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>

</xml_diff>

<commit_message>
Made some changes to the new test cases.
</commit_message>
<xml_diff>
--- a/documentation/VD/source/procedures.xlsx
+++ b/documentation/VD/source/procedures.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72B9079-CBFB-42E0-8A7B-DF500BAEF949}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2D9F6F-3A60-4D88-863F-3AA00011CC83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-48" yWindow="4284" windowWidth="17280" windowHeight="11508" tabRatio="683" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13572" yWindow="7572" windowWidth="17280" windowHeight="11508" tabRatio="683" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="307">
   <si>
     <t>Title</t>
   </si>
@@ -748,18 +748,9 @@
     <t>Validator_test_01.png</t>
   </si>
   <si>
-    <t>A snippit of the Facile software system that shows 200 messages of the TGUIM and API being validated for errors, warning, and info.</t>
-  </si>
-  <si>
     <t>A variety of files are shown. The main file is the name of your project with the *.fcl* extension. Refer to @extension_test_01.png Test case is completed.</t>
   </si>
   <si>
-    <t>Value of input port is updated.</t>
-  </si>
-  <si>
-    <t>Click on **NoneType** under **Output Ports** and add the type of data structure.</t>
-  </si>
-  <si>
     <t>ShowRelevantActions_test_01.png</t>
   </si>
   <si>
@@ -895,12 +886,6 @@
     <t>A action pipeline creation dialog is shown in a new window. Refer to @ActionPipelineCreation_test_01.png</t>
   </si>
   <si>
-    <t>Refer to @ShowRelevantActions_test_01.png Test Case is completed.</t>
-  </si>
-  <si>
-    <t>Refer to @Validator_test_01.png  Test case is completed</t>
-  </si>
-  <si>
     <t xml:space="preserve">Project is saved with the *.fcl* extension in the selected folder. Refer to @GUI_test_02.png </t>
   </si>
   <si>
@@ -962,6 +947,36 @@
   </si>
   <si>
     <t>Click on any component of the **Target GUI Model**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on a component in the **Target GUI Model**. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All actions that can be performed on that component appear in the Action Menu view. Refer to @ShowRelevantActions_test_01.png Test case is complete. </t>
+  </si>
+  <si>
+    <t>Validator_test_02.png</t>
+  </si>
+  <si>
+    <t>Validator_test_03.png</t>
+  </si>
+  <si>
+    <t>A snippit of the Facile software system that shows a message of thevalidator being run and warning message coming up.</t>
+  </si>
+  <si>
+    <t>A snippit of the Facile software system that shows a message of thevalidator being run and validated message coming up.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refer to @Validator_test_01.png  error message comes up for not having an action pipeline. </t>
+  </si>
+  <si>
+    <t>Refer to @Validator_test_02.png  warning message comes up for not using the input port of the action pipeline.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on a input port at the top level of that action pipeline and draw a wire from it to an top level output port or a child input port with the same data type. </t>
+  </si>
+  <si>
+    <t>Refer to @Validator_test_03.png  a green message comes up validating the **APIM**. Test case is completed.</t>
   </si>
 </sst>
 </file>
@@ -1317,98 +1332,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1437,6 +1374,15 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1446,20 +1392,89 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1755,846 +1770,828 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="51"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="25"/>
     </row>
     <row r="2" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="54"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="28"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="52"/>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="54"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="28"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="52"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="54"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="28"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="52"/>
-      <c r="B5" s="53"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="54"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="28"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="52"/>
-      <c r="B6" s="53"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="54"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="28"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="52"/>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="54"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="28"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="52"/>
-      <c r="B8" s="53"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="54"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="28"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="52"/>
-      <c r="B9" s="53"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="54"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="28"/>
     </row>
     <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="55" t="s">
+      <c r="A10" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="57"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="31"/>
     </row>
     <row r="11" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="26"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="34"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="24"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="26"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="34"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="24"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="26"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="34"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="24"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="26"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="34"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="24"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="26"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="34"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="24"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="26"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="34"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="24"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="26"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="34"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="24"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="26"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="34"/>
     </row>
     <row r="19" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="63">
+      <c r="A19" s="20">
         <v>1</v>
       </c>
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="59"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="59"/>
-      <c r="H19" s="59"/>
-      <c r="I19" s="60"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="37"/>
     </row>
     <row r="20" spans="1:9" ht="20.7" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="64"/>
+      <c r="A20" s="21"/>
       <c r="B20" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="61" t="s">
+      <c r="C20" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="62"/>
-      <c r="E20" s="22" t="s">
+      <c r="D20" s="19"/>
+      <c r="E20" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="23"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="39"/>
     </row>
     <row r="21" spans="1:9" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="64"/>
+      <c r="A21" s="21"/>
       <c r="B21" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="61" t="s">
+      <c r="C21" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="62"/>
-      <c r="E21" s="22" t="s">
+      <c r="D21" s="19"/>
+      <c r="E21" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="23"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="39"/>
     </row>
     <row r="22" spans="1:9" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="64"/>
+      <c r="A22" s="21"/>
       <c r="B22" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="61" t="s">
+      <c r="C22" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="62"/>
-      <c r="E22" s="22" t="s">
+      <c r="D22" s="19"/>
+      <c r="E22" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="23"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="39"/>
     </row>
     <row r="23" spans="1:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="64"/>
+      <c r="A23" s="21"/>
       <c r="B23" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="61" t="s">
+      <c r="C23" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="62"/>
-      <c r="E23" s="22" t="s">
+      <c r="D23" s="19"/>
+      <c r="E23" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="23"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="39"/>
     </row>
     <row r="24" spans="1:9" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="64"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="61" t="s">
+      <c r="C24" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="62"/>
-      <c r="E24" s="22" t="s">
+      <c r="D24" s="19"/>
+      <c r="E24" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="23"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="39"/>
     </row>
     <row r="25" spans="1:9" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="64"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="61" t="s">
+      <c r="C25" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="62"/>
-      <c r="E25" s="22" t="s">
+      <c r="D25" s="19"/>
+      <c r="E25" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="23"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="39"/>
     </row>
     <row r="26" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="64"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="61" t="s">
+      <c r="C26" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="62"/>
-      <c r="E26" s="22" t="s">
+      <c r="D26" s="19"/>
+      <c r="E26" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="23"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="39"/>
     </row>
     <row r="27" spans="1:9" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="64"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="61" t="s">
+      <c r="C27" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="62"/>
-      <c r="E27" s="22" t="s">
+      <c r="D27" s="19"/>
+      <c r="E27" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="23"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="39"/>
     </row>
     <row r="28" spans="1:9" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="64"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="61" t="s">
+      <c r="C28" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="62"/>
-      <c r="E28" s="22" t="s">
+      <c r="D28" s="19"/>
+      <c r="E28" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="46"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="40"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="41"/>
     </row>
     <row r="29" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="65"/>
+      <c r="A29" s="22"/>
       <c r="B29" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="61" t="s">
+      <c r="C29" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="62"/>
-      <c r="E29" s="37" t="s">
+      <c r="D29" s="19"/>
+      <c r="E29" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="F29" s="47"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="48"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="44"/>
     </row>
     <row r="30" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="30">
+      <c r="A30" s="45">
         <v>2</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="20"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="49"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="50"/>
     </row>
     <row r="31" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="31"/>
+      <c r="A31" s="46"/>
       <c r="B31" s="9"/>
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="23"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="39"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="31"/>
+      <c r="A32" s="46"/>
       <c r="B32" s="9"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="26"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="34"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="31"/>
+      <c r="A33" s="46"/>
       <c r="B33" s="9"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="26"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="34"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="31"/>
+      <c r="A34" s="46"/>
       <c r="B34" s="9"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="26"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="33"/>
+      <c r="H34" s="33"/>
+      <c r="I34" s="34"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="31"/>
+      <c r="A35" s="46"/>
       <c r="B35" s="9"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="26"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="33"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="34"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="31"/>
+      <c r="A36" s="46"/>
       <c r="B36" s="9"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="26"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="33"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="34"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="31"/>
+      <c r="A37" s="46"/>
       <c r="B37" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="42" t="s">
+      <c r="C37" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="43"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="43"/>
-      <c r="H37" s="43"/>
-      <c r="I37" s="44"/>
+      <c r="D37" s="64"/>
+      <c r="E37" s="64"/>
+      <c r="F37" s="64"/>
+      <c r="G37" s="64"/>
+      <c r="H37" s="64"/>
+      <c r="I37" s="65"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="31"/>
+      <c r="A38" s="46"/>
       <c r="B38" s="11"/>
       <c r="C38" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D38" s="21" t="s">
+      <c r="D38" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="23"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="39"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="31"/>
+      <c r="A39" s="46"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="25"/>
-      <c r="H39" s="25"/>
-      <c r="I39" s="26"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="33"/>
+      <c r="I39" s="34"/>
     </row>
     <row r="40" spans="1:9" ht="18.3" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="31"/>
+      <c r="A40" s="46"/>
       <c r="B40" s="11"/>
       <c r="C40" s="14"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="28"/>
-      <c r="F40" s="28"/>
-      <c r="G40" s="28"/>
-      <c r="H40" s="28"/>
-      <c r="I40" s="29"/>
+      <c r="D40" s="52"/>
+      <c r="E40" s="53"/>
+      <c r="F40" s="53"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="53"/>
+      <c r="I40" s="54"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="31"/>
+      <c r="A41" s="46"/>
       <c r="B41" s="11"/>
       <c r="C41" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D41" s="36" t="s">
+      <c r="D41" s="58" t="s">
         <v>57</v>
       </c>
-      <c r="E41" s="37"/>
-      <c r="F41" s="37"/>
-      <c r="G41" s="37"/>
-      <c r="H41" s="37"/>
-      <c r="I41" s="38"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="42"/>
+      <c r="H41" s="42"/>
+      <c r="I41" s="59"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="32"/>
+      <c r="A42" s="47"/>
       <c r="B42" s="14"/>
       <c r="C42" s="14"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="40"/>
-      <c r="F42" s="40"/>
-      <c r="G42" s="40"/>
-      <c r="H42" s="40"/>
-      <c r="I42" s="41"/>
+      <c r="D42" s="60"/>
+      <c r="E42" s="61"/>
+      <c r="F42" s="61"/>
+      <c r="G42" s="61"/>
+      <c r="H42" s="61"/>
+      <c r="I42" s="62"/>
     </row>
     <row r="43" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A43" s="30">
+      <c r="A43" s="45">
         <v>3</v>
       </c>
-      <c r="B43" s="18" t="s">
+      <c r="B43" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="20"/>
+      <c r="C43" s="49"/>
+      <c r="D43" s="49"/>
+      <c r="E43" s="49"/>
+      <c r="F43" s="49"/>
+      <c r="G43" s="49"/>
+      <c r="H43" s="49"/>
+      <c r="I43" s="50"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="31"/>
-      <c r="B44" s="33" t="s">
+      <c r="A44" s="46"/>
+      <c r="B44" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="C44" s="35" t="s">
+      <c r="C44" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="D44" s="21" t="s">
+      <c r="D44" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="E44" s="22"/>
-      <c r="F44" s="22"/>
-      <c r="G44" s="22"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="23"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="39"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="31"/>
-      <c r="B45" s="33"/>
-      <c r="C45" s="33"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="25"/>
-      <c r="H45" s="25"/>
-      <c r="I45" s="26"/>
+      <c r="A45" s="46"/>
+      <c r="B45" s="56"/>
+      <c r="C45" s="56"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="33"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="33"/>
+      <c r="H45" s="33"/>
+      <c r="I45" s="34"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="31"/>
-      <c r="B46" s="33"/>
-      <c r="C46" s="34"/>
-      <c r="D46" s="27"/>
-      <c r="E46" s="28"/>
-      <c r="F46" s="28"/>
-      <c r="G46" s="28"/>
-      <c r="H46" s="28"/>
-      <c r="I46" s="29"/>
+      <c r="A46" s="46"/>
+      <c r="B46" s="56"/>
+      <c r="C46" s="57"/>
+      <c r="D46" s="52"/>
+      <c r="E46" s="53"/>
+      <c r="F46" s="53"/>
+      <c r="G46" s="53"/>
+      <c r="H46" s="53"/>
+      <c r="I46" s="54"/>
     </row>
     <row r="47" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="31"/>
-      <c r="B47" s="33" t="s">
+      <c r="A47" s="46"/>
+      <c r="B47" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="C47" s="35" t="s">
+      <c r="C47" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="D47" s="21" t="s">
+      <c r="D47" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="E47" s="22"/>
-      <c r="F47" s="22"/>
-      <c r="G47" s="22"/>
-      <c r="H47" s="22"/>
-      <c r="I47" s="23"/>
+      <c r="E47" s="38"/>
+      <c r="F47" s="38"/>
+      <c r="G47" s="38"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="39"/>
     </row>
     <row r="48" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="31"/>
-      <c r="B48" s="33"/>
-      <c r="C48" s="33"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="25"/>
-      <c r="H48" s="25"/>
-      <c r="I48" s="26"/>
+      <c r="A48" s="46"/>
+      <c r="B48" s="56"/>
+      <c r="C48" s="56"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="33"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="33"/>
+      <c r="H48" s="33"/>
+      <c r="I48" s="34"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="31"/>
-      <c r="B49" s="33"/>
-      <c r="C49" s="34"/>
-      <c r="D49" s="27"/>
-      <c r="E49" s="28"/>
-      <c r="F49" s="28"/>
-      <c r="G49" s="28"/>
-      <c r="H49" s="28"/>
-      <c r="I49" s="29"/>
+      <c r="A49" s="46"/>
+      <c r="B49" s="56"/>
+      <c r="C49" s="57"/>
+      <c r="D49" s="52"/>
+      <c r="E49" s="53"/>
+      <c r="F49" s="53"/>
+      <c r="G49" s="53"/>
+      <c r="H49" s="53"/>
+      <c r="I49" s="54"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="31"/>
-      <c r="B50" s="33" t="s">
+      <c r="A50" s="46"/>
+      <c r="B50" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="C50" s="33" t="s">
+      <c r="C50" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="D50" s="21" t="s">
+      <c r="D50" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="E50" s="22"/>
-      <c r="F50" s="22"/>
-      <c r="G50" s="22"/>
-      <c r="H50" s="22"/>
-      <c r="I50" s="23"/>
+      <c r="E50" s="38"/>
+      <c r="F50" s="38"/>
+      <c r="G50" s="38"/>
+      <c r="H50" s="38"/>
+      <c r="I50" s="39"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="31"/>
-      <c r="B51" s="33"/>
-      <c r="C51" s="33"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="25"/>
-      <c r="F51" s="25"/>
-      <c r="G51" s="25"/>
-      <c r="H51" s="25"/>
-      <c r="I51" s="26"/>
+      <c r="A51" s="46"/>
+      <c r="B51" s="56"/>
+      <c r="C51" s="56"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="33"/>
+      <c r="F51" s="33"/>
+      <c r="G51" s="33"/>
+      <c r="H51" s="33"/>
+      <c r="I51" s="34"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="32"/>
-      <c r="B52" s="34"/>
-      <c r="C52" s="34"/>
-      <c r="D52" s="27"/>
-      <c r="E52" s="28"/>
-      <c r="F52" s="28"/>
-      <c r="G52" s="28"/>
-      <c r="H52" s="28"/>
-      <c r="I52" s="29"/>
+      <c r="A52" s="47"/>
+      <c r="B52" s="57"/>
+      <c r="C52" s="57"/>
+      <c r="D52" s="52"/>
+      <c r="E52" s="53"/>
+      <c r="F52" s="53"/>
+      <c r="G52" s="53"/>
+      <c r="H52" s="53"/>
+      <c r="I52" s="54"/>
     </row>
     <row r="53" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A53" s="30">
+      <c r="A53" s="45">
         <v>4</v>
       </c>
-      <c r="B53" s="18" t="s">
+      <c r="B53" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19"/>
-      <c r="G53" s="19"/>
-      <c r="H53" s="19"/>
-      <c r="I53" s="20"/>
+      <c r="C53" s="49"/>
+      <c r="D53" s="49"/>
+      <c r="E53" s="49"/>
+      <c r="F53" s="49"/>
+      <c r="G53" s="49"/>
+      <c r="H53" s="49"/>
+      <c r="I53" s="50"/>
     </row>
     <row r="54" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="31"/>
-      <c r="B54" s="31" t="s">
+      <c r="A54" s="46"/>
+      <c r="B54" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="C54" s="21" t="s">
+      <c r="C54" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="D54" s="22"/>
-      <c r="E54" s="22"/>
-      <c r="F54" s="22"/>
-      <c r="G54" s="22"/>
-      <c r="H54" s="22"/>
-      <c r="I54" s="23"/>
+      <c r="D54" s="38"/>
+      <c r="E54" s="38"/>
+      <c r="F54" s="38"/>
+      <c r="G54" s="38"/>
+      <c r="H54" s="38"/>
+      <c r="I54" s="39"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="31"/>
-      <c r="B55" s="31"/>
-      <c r="C55" s="24"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="25"/>
-      <c r="F55" s="25"/>
-      <c r="G55" s="25"/>
-      <c r="H55" s="25"/>
-      <c r="I55" s="26"/>
+      <c r="A55" s="46"/>
+      <c r="B55" s="46"/>
+      <c r="C55" s="32"/>
+      <c r="D55" s="33"/>
+      <c r="E55" s="33"/>
+      <c r="F55" s="33"/>
+      <c r="G55" s="33"/>
+      <c r="H55" s="33"/>
+      <c r="I55" s="34"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="31"/>
-      <c r="B56" s="31"/>
-      <c r="C56" s="24"/>
-      <c r="D56" s="25"/>
-      <c r="E56" s="25"/>
-      <c r="F56" s="25"/>
-      <c r="G56" s="25"/>
-      <c r="H56" s="25"/>
-      <c r="I56" s="26"/>
+      <c r="A56" s="46"/>
+      <c r="B56" s="46"/>
+      <c r="C56" s="32"/>
+      <c r="D56" s="33"/>
+      <c r="E56" s="33"/>
+      <c r="F56" s="33"/>
+      <c r="G56" s="33"/>
+      <c r="H56" s="33"/>
+      <c r="I56" s="34"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="31"/>
-      <c r="B57" s="31"/>
-      <c r="C57" s="24"/>
-      <c r="D57" s="25"/>
-      <c r="E57" s="25"/>
-      <c r="F57" s="25"/>
-      <c r="G57" s="25"/>
-      <c r="H57" s="25"/>
-      <c r="I57" s="26"/>
+      <c r="A57" s="46"/>
+      <c r="B57" s="46"/>
+      <c r="C57" s="32"/>
+      <c r="D57" s="33"/>
+      <c r="E57" s="33"/>
+      <c r="F57" s="33"/>
+      <c r="G57" s="33"/>
+      <c r="H57" s="33"/>
+      <c r="I57" s="34"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="31"/>
-      <c r="B58" s="31"/>
-      <c r="C58" s="24"/>
-      <c r="D58" s="25"/>
-      <c r="E58" s="25"/>
-      <c r="F58" s="25"/>
-      <c r="G58" s="25"/>
-      <c r="H58" s="25"/>
-      <c r="I58" s="26"/>
+      <c r="A58" s="46"/>
+      <c r="B58" s="46"/>
+      <c r="C58" s="32"/>
+      <c r="D58" s="33"/>
+      <c r="E58" s="33"/>
+      <c r="F58" s="33"/>
+      <c r="G58" s="33"/>
+      <c r="H58" s="33"/>
+      <c r="I58" s="34"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="31"/>
-      <c r="B59" s="31"/>
-      <c r="C59" s="24"/>
-      <c r="D59" s="25"/>
-      <c r="E59" s="25"/>
-      <c r="F59" s="25"/>
-      <c r="G59" s="25"/>
-      <c r="H59" s="25"/>
-      <c r="I59" s="26"/>
+      <c r="A59" s="46"/>
+      <c r="B59" s="46"/>
+      <c r="C59" s="32"/>
+      <c r="D59" s="33"/>
+      <c r="E59" s="33"/>
+      <c r="F59" s="33"/>
+      <c r="G59" s="33"/>
+      <c r="H59" s="33"/>
+      <c r="I59" s="34"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="31"/>
-      <c r="B60" s="31"/>
-      <c r="C60" s="24"/>
-      <c r="D60" s="25"/>
-      <c r="E60" s="25"/>
-      <c r="F60" s="25"/>
-      <c r="G60" s="25"/>
-      <c r="H60" s="25"/>
-      <c r="I60" s="26"/>
+      <c r="A60" s="46"/>
+      <c r="B60" s="46"/>
+      <c r="C60" s="32"/>
+      <c r="D60" s="33"/>
+      <c r="E60" s="33"/>
+      <c r="F60" s="33"/>
+      <c r="G60" s="33"/>
+      <c r="H60" s="33"/>
+      <c r="I60" s="34"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="31"/>
-      <c r="B61" s="31"/>
-      <c r="C61" s="24"/>
-      <c r="D61" s="25"/>
-      <c r="E61" s="25"/>
-      <c r="F61" s="25"/>
-      <c r="G61" s="25"/>
-      <c r="H61" s="25"/>
-      <c r="I61" s="26"/>
+      <c r="A61" s="46"/>
+      <c r="B61" s="46"/>
+      <c r="C61" s="32"/>
+      <c r="D61" s="33"/>
+      <c r="E61" s="33"/>
+      <c r="F61" s="33"/>
+      <c r="G61" s="33"/>
+      <c r="H61" s="33"/>
+      <c r="I61" s="34"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="31"/>
-      <c r="B62" s="31"/>
-      <c r="C62" s="24"/>
-      <c r="D62" s="25"/>
-      <c r="E62" s="25"/>
-      <c r="F62" s="25"/>
-      <c r="G62" s="25"/>
-      <c r="H62" s="25"/>
-      <c r="I62" s="26"/>
+      <c r="A62" s="46"/>
+      <c r="B62" s="46"/>
+      <c r="C62" s="32"/>
+      <c r="D62" s="33"/>
+      <c r="E62" s="33"/>
+      <c r="F62" s="33"/>
+      <c r="G62" s="33"/>
+      <c r="H62" s="33"/>
+      <c r="I62" s="34"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="32"/>
-      <c r="B63" s="32"/>
-      <c r="C63" s="27"/>
-      <c r="D63" s="28"/>
-      <c r="E63" s="28"/>
-      <c r="F63" s="28"/>
-      <c r="G63" s="28"/>
-      <c r="H63" s="28"/>
-      <c r="I63" s="29"/>
+      <c r="A63" s="47"/>
+      <c r="B63" s="47"/>
+      <c r="C63" s="52"/>
+      <c r="D63" s="53"/>
+      <c r="E63" s="53"/>
+      <c r="F63" s="53"/>
+      <c r="G63" s="53"/>
+      <c r="H63" s="53"/>
+      <c r="I63" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="A19:A29"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I9"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A11:I18"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="E28:I28"/>
-    <mergeCell ref="E29:I29"/>
+    <mergeCell ref="B53:I53"/>
+    <mergeCell ref="C54:I63"/>
+    <mergeCell ref="A53:A63"/>
+    <mergeCell ref="B54:B63"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="A43:A52"/>
     <mergeCell ref="A30:A42"/>
     <mergeCell ref="B43:I43"/>
     <mergeCell ref="D47:I49"/>
@@ -2608,14 +2605,32 @@
     <mergeCell ref="D44:I46"/>
     <mergeCell ref="B30:I30"/>
     <mergeCell ref="C37:I37"/>
-    <mergeCell ref="B53:I53"/>
-    <mergeCell ref="C54:I63"/>
-    <mergeCell ref="A53:A63"/>
-    <mergeCell ref="B54:B63"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="A43:A52"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="E29:I29"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I9"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A11:I18"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="A19:A29"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2626,8 +2641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE9DEC4C-0859-492A-9859-A5102CF1C24C}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView topLeftCell="D15" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView topLeftCell="H3" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2681,7 +2696,7 @@
         <v>205</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -2696,16 +2711,16 @@
         <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2718,16 +2733,16 @@
         <v>13</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
@@ -2746,10 +2761,10 @@
         <v>183</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -2766,10 +2781,10 @@
         <v>70</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
@@ -2786,10 +2801,10 @@
         <v>84</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2806,10 +2821,10 @@
         <v>21</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -2974,10 +2989,10 @@
     </row>
     <row r="21" spans="7:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="G21" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="22" spans="7:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2985,63 +3000,63 @@
         <v>227</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="23" spans="7:8" ht="144" x14ac:dyDescent="0.3">
       <c r="G23" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="24" spans="7:8" ht="144" x14ac:dyDescent="0.3">
       <c r="G24" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="25" spans="7:8" ht="144" x14ac:dyDescent="0.3">
       <c r="G25" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="26" spans="7:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="G26" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="27" spans="7:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="G27" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="28" spans="7:8" ht="72" x14ac:dyDescent="0.3">
       <c r="G28" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="29" spans="7:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="G29" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -3054,8 +3069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D9C558-86BD-4789-80C1-D36E81752C81}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="H3" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3109,7 +3124,7 @@
         <v>207</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -3130,10 +3145,10 @@
         <v>183</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="123.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -3152,10 +3167,10 @@
         <v>70</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
@@ -3174,10 +3189,10 @@
         <v>84</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -3287,7 +3302,7 @@
         <v>82</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
@@ -3300,10 +3315,10 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
@@ -3368,10 +3383,10 @@
     </row>
     <row r="19" spans="7:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="G19" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="20" spans="7:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -3379,7 +3394,7 @@
         <v>227</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -3391,8 +3406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE0C746B-3182-4B37-8AF4-A9D404711DCD}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F16" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView topLeftCell="O3" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3404,7 +3419,7 @@
     <col min="5" max="5" width="21.6640625" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
     <col min="7" max="7" width="17.44140625" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" customWidth="1"/>
+    <col min="8" max="8" width="20.21875" customWidth="1"/>
     <col min="9" max="9" width="27.44140625" customWidth="1"/>
     <col min="10" max="10" width="17.6640625" customWidth="1"/>
   </cols>
@@ -3446,7 +3461,7 @@
         <v>209</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -3467,10 +3482,10 @@
         <v>183</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -3616,12 +3631,12 @@
         <v>82</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -3629,77 +3644,49 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>249</v>
+        <v>297</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>214</v>
+        <v>298</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>222</v>
-      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="G14" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="G15" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="G16" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="17" spans="7:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="G17" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="18" spans="7:8" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="G18" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="19" spans="7:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="G19" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="H19" s="16" t="s">
-        <v>279</v>
-      </c>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G16" s="2"/>
+      <c r="H16" s="16"/>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G19" s="2"/>
+      <c r="H19" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3708,10 +3695,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D9410B-47BB-4E45-80F2-F71FCE9008EE}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="D6" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3765,7 +3752,7 @@
         <v>211</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -3789,10 +3776,10 @@
         <v>229</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -3807,10 +3794,14 @@
       <c r="H3" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="8"/>
-    </row>
-    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="I3" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -3825,10 +3816,14 @@
       <c r="H4" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="8"/>
-    </row>
-    <row r="5" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="I4" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -3841,8 +3836,12 @@
       <c r="H5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="8"/>
+      <c r="I5" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
@@ -3935,12 +3934,12 @@
         <v>82</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -3951,26 +3950,106 @@
         <v>228</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>280</v>
+        <v>303</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="144" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>275</v>
+      </c>
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+    <row r="14" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="G14" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="G15" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="G16" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="G17" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="18" spans="7:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="G18" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="19" spans="7:8" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="G19" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="20" spans="7:8" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="G20" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="21" spans="7:8" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="G21" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="22" spans="7:8" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="G22" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="23" spans="7:8" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="G23" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>306</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4212,7 +4291,7 @@
         <v>150</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
@@ -4478,7 +4557,7 @@
         <v>80</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
@@ -5084,7 +5163,7 @@
         <v>75</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -5099,10 +5178,10 @@
         <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="8"/>
@@ -5117,10 +5196,10 @@
         <v>13</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="8"/>
@@ -5133,10 +5212,10 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
@@ -5149,10 +5228,10 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
@@ -5165,10 +5244,10 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
@@ -5181,10 +5260,10 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
@@ -5197,10 +5276,10 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
@@ -5521,7 +5600,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>204</v>

</xml_diff>

<commit_message>
Changed where the images were located.
</commit_message>
<xml_diff>
--- a/documentation/VD/source/procedures.xlsx
+++ b/documentation/VD/source/procedures.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2D9F6F-3A60-4D88-863F-3AA00011CC83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F05D8B-DAAA-44FC-B881-791FB6A0453C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13572" yWindow="7572" windowWidth="17280" windowHeight="11508" tabRatio="683" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="852" windowWidth="17280" windowHeight="11508" tabRatio="683" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="2" r:id="rId1"/>
@@ -1332,20 +1332,98 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1374,15 +1452,6 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1392,89 +1461,20 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1770,828 +1770,846 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="25"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="51"/>
     </row>
     <row r="2" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="28"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="54"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="26"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="28"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="54"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="28"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="54"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="26"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="28"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="54"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="26"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="28"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="54"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="26"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="28"/>
+      <c r="A7" s="52"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="54"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="26"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="28"/>
+      <c r="A8" s="52"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="54"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="26"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="28"/>
+      <c r="A9" s="52"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="54"/>
     </row>
     <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="31"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="57"/>
     </row>
     <row r="11" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="34"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="26"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="32"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="34"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="26"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="32"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="34"/>
+      <c r="A13" s="24"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="26"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="32"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="34"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="26"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="32"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="34"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="26"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="32"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="34"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="26"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="32"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="34"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="26"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="32"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="34"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="26"/>
     </row>
     <row r="19" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="20">
+      <c r="A19" s="63">
         <v>1</v>
       </c>
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="37"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="59"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="60"/>
     </row>
     <row r="20" spans="1:9" ht="20.7" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="21"/>
+      <c r="A20" s="64"/>
       <c r="B20" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="38" t="s">
+      <c r="D20" s="62"/>
+      <c r="E20" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="39"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="23"/>
     </row>
     <row r="21" spans="1:9" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="21"/>
+      <c r="A21" s="64"/>
       <c r="B21" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="38" t="s">
+      <c r="D21" s="62"/>
+      <c r="E21" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="39"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="23"/>
     </row>
     <row r="22" spans="1:9" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="21"/>
+      <c r="A22" s="64"/>
       <c r="B22" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="19"/>
-      <c r="E22" s="38" t="s">
+      <c r="D22" s="62"/>
+      <c r="E22" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="39"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="23"/>
     </row>
     <row r="23" spans="1:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="21"/>
+      <c r="A23" s="64"/>
       <c r="B23" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="38" t="s">
+      <c r="D23" s="62"/>
+      <c r="E23" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="39"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="23"/>
     </row>
     <row r="24" spans="1:9" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="21"/>
+      <c r="A24" s="64"/>
       <c r="B24" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="19"/>
-      <c r="E24" s="38" t="s">
+      <c r="D24" s="62"/>
+      <c r="E24" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="39"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="23"/>
     </row>
     <row r="25" spans="1:9" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="21"/>
+      <c r="A25" s="64"/>
       <c r="B25" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="19"/>
-      <c r="E25" s="38" t="s">
+      <c r="D25" s="62"/>
+      <c r="E25" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="39"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="23"/>
     </row>
     <row r="26" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="21"/>
+      <c r="A26" s="64"/>
       <c r="B26" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="38" t="s">
+      <c r="D26" s="62"/>
+      <c r="E26" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="39"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="23"/>
     </row>
     <row r="27" spans="1:9" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="21"/>
+      <c r="A27" s="64"/>
       <c r="B27" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="38" t="s">
+      <c r="D27" s="62"/>
+      <c r="E27" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="39"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="23"/>
     </row>
     <row r="28" spans="1:9" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="21"/>
+      <c r="A28" s="64"/>
       <c r="B28" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="19"/>
-      <c r="E28" s="38" t="s">
+      <c r="D28" s="62"/>
+      <c r="E28" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="F28" s="40"/>
-      <c r="G28" s="40"/>
-      <c r="H28" s="40"/>
-      <c r="I28" s="41"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="46"/>
     </row>
     <row r="29" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="22"/>
+      <c r="A29" s="65"/>
       <c r="B29" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="19"/>
-      <c r="E29" s="42" t="s">
+      <c r="D29" s="62"/>
+      <c r="E29" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="44"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="48"/>
     </row>
     <row r="30" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="45">
+      <c r="A30" s="30">
         <v>2</v>
       </c>
-      <c r="B30" s="49" t="s">
+      <c r="B30" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="49"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="49"/>
-      <c r="H30" s="49"/>
-      <c r="I30" s="50"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="20"/>
     </row>
     <row r="31" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="46"/>
+      <c r="A31" s="31"/>
       <c r="B31" s="9"/>
-      <c r="C31" s="51" t="s">
+      <c r="C31" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="39"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="23"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="46"/>
+      <c r="A32" s="31"/>
       <c r="B32" s="9"/>
-      <c r="C32" s="32"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="34"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="26"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="46"/>
+      <c r="A33" s="31"/>
       <c r="B33" s="9"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="34"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="26"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="46"/>
+      <c r="A34" s="31"/>
       <c r="B34" s="9"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="33"/>
-      <c r="I34" s="34"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="26"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="46"/>
+      <c r="A35" s="31"/>
       <c r="B35" s="9"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="33"/>
-      <c r="H35" s="33"/>
-      <c r="I35" s="34"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="25"/>
+      <c r="I35" s="26"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="46"/>
+      <c r="A36" s="31"/>
       <c r="B36" s="9"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="33"/>
-      <c r="G36" s="33"/>
-      <c r="H36" s="33"/>
-      <c r="I36" s="34"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="26"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="46"/>
+      <c r="A37" s="31"/>
       <c r="B37" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="63" t="s">
+      <c r="C37" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="64"/>
-      <c r="E37" s="64"/>
-      <c r="F37" s="64"/>
-      <c r="G37" s="64"/>
-      <c r="H37" s="64"/>
-      <c r="I37" s="65"/>
+      <c r="D37" s="43"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="43"/>
+      <c r="G37" s="43"/>
+      <c r="H37" s="43"/>
+      <c r="I37" s="44"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="46"/>
+      <c r="A38" s="31"/>
       <c r="B38" s="11"/>
       <c r="C38" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D38" s="51" t="s">
+      <c r="D38" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="E38" s="38"/>
-      <c r="F38" s="38"/>
-      <c r="G38" s="38"/>
-      <c r="H38" s="38"/>
-      <c r="I38" s="39"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="23"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="46"/>
+      <c r="A39" s="31"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="33"/>
-      <c r="F39" s="33"/>
-      <c r="G39" s="33"/>
-      <c r="H39" s="33"/>
-      <c r="I39" s="34"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="26"/>
     </row>
     <row r="40" spans="1:9" ht="18.3" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="46"/>
+      <c r="A40" s="31"/>
       <c r="B40" s="11"/>
       <c r="C40" s="14"/>
-      <c r="D40" s="52"/>
-      <c r="E40" s="53"/>
-      <c r="F40" s="53"/>
-      <c r="G40" s="53"/>
-      <c r="H40" s="53"/>
-      <c r="I40" s="54"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="28"/>
+      <c r="G40" s="28"/>
+      <c r="H40" s="28"/>
+      <c r="I40" s="29"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="46"/>
+      <c r="A41" s="31"/>
       <c r="B41" s="11"/>
       <c r="C41" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D41" s="58" t="s">
+      <c r="D41" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="E41" s="42"/>
-      <c r="F41" s="42"/>
-      <c r="G41" s="42"/>
-      <c r="H41" s="42"/>
-      <c r="I41" s="59"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="37"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="37"/>
+      <c r="I41" s="38"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="47"/>
+      <c r="A42" s="32"/>
       <c r="B42" s="14"/>
       <c r="C42" s="14"/>
-      <c r="D42" s="60"/>
-      <c r="E42" s="61"/>
-      <c r="F42" s="61"/>
-      <c r="G42" s="61"/>
-      <c r="H42" s="61"/>
-      <c r="I42" s="62"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="40"/>
+      <c r="F42" s="40"/>
+      <c r="G42" s="40"/>
+      <c r="H42" s="40"/>
+      <c r="I42" s="41"/>
     </row>
     <row r="43" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A43" s="45">
+      <c r="A43" s="30">
         <v>3</v>
       </c>
-      <c r="B43" s="48" t="s">
+      <c r="B43" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="C43" s="49"/>
-      <c r="D43" s="49"/>
-      <c r="E43" s="49"/>
-      <c r="F43" s="49"/>
-      <c r="G43" s="49"/>
-      <c r="H43" s="49"/>
-      <c r="I43" s="50"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="20"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="46"/>
-      <c r="B44" s="56" t="s">
+      <c r="A44" s="31"/>
+      <c r="B44" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="C44" s="55" t="s">
+      <c r="C44" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="D44" s="51" t="s">
+      <c r="D44" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="E44" s="38"/>
-      <c r="F44" s="38"/>
-      <c r="G44" s="38"/>
-      <c r="H44" s="38"/>
-      <c r="I44" s="39"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="23"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="46"/>
-      <c r="B45" s="56"/>
-      <c r="C45" s="56"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="33"/>
-      <c r="F45" s="33"/>
-      <c r="G45" s="33"/>
-      <c r="H45" s="33"/>
-      <c r="I45" s="34"/>
+      <c r="A45" s="31"/>
+      <c r="B45" s="33"/>
+      <c r="C45" s="33"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="25"/>
+      <c r="G45" s="25"/>
+      <c r="H45" s="25"/>
+      <c r="I45" s="26"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="46"/>
-      <c r="B46" s="56"/>
-      <c r="C46" s="57"/>
-      <c r="D46" s="52"/>
-      <c r="E46" s="53"/>
-      <c r="F46" s="53"/>
-      <c r="G46" s="53"/>
-      <c r="H46" s="53"/>
-      <c r="I46" s="54"/>
+      <c r="A46" s="31"/>
+      <c r="B46" s="33"/>
+      <c r="C46" s="34"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="28"/>
+      <c r="G46" s="28"/>
+      <c r="H46" s="28"/>
+      <c r="I46" s="29"/>
     </row>
     <row r="47" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="46"/>
-      <c r="B47" s="56" t="s">
+      <c r="A47" s="31"/>
+      <c r="B47" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C47" s="55" t="s">
+      <c r="C47" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="D47" s="51" t="s">
+      <c r="D47" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="E47" s="38"/>
-      <c r="F47" s="38"/>
-      <c r="G47" s="38"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="39"/>
+      <c r="E47" s="22"/>
+      <c r="F47" s="22"/>
+      <c r="G47" s="22"/>
+      <c r="H47" s="22"/>
+      <c r="I47" s="23"/>
     </row>
     <row r="48" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="46"/>
-      <c r="B48" s="56"/>
-      <c r="C48" s="56"/>
-      <c r="D48" s="32"/>
-      <c r="E48" s="33"/>
-      <c r="F48" s="33"/>
-      <c r="G48" s="33"/>
-      <c r="H48" s="33"/>
-      <c r="I48" s="34"/>
+      <c r="A48" s="31"/>
+      <c r="B48" s="33"/>
+      <c r="C48" s="33"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="25"/>
+      <c r="F48" s="25"/>
+      <c r="G48" s="25"/>
+      <c r="H48" s="25"/>
+      <c r="I48" s="26"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="46"/>
-      <c r="B49" s="56"/>
-      <c r="C49" s="57"/>
-      <c r="D49" s="52"/>
-      <c r="E49" s="53"/>
-      <c r="F49" s="53"/>
-      <c r="G49" s="53"/>
-      <c r="H49" s="53"/>
-      <c r="I49" s="54"/>
+      <c r="A49" s="31"/>
+      <c r="B49" s="33"/>
+      <c r="C49" s="34"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="28"/>
+      <c r="G49" s="28"/>
+      <c r="H49" s="28"/>
+      <c r="I49" s="29"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="46"/>
-      <c r="B50" s="56" t="s">
+      <c r="A50" s="31"/>
+      <c r="B50" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="C50" s="56" t="s">
+      <c r="C50" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="D50" s="51" t="s">
+      <c r="D50" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="E50" s="38"/>
-      <c r="F50" s="38"/>
-      <c r="G50" s="38"/>
-      <c r="H50" s="38"/>
-      <c r="I50" s="39"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="22"/>
+      <c r="G50" s="22"/>
+      <c r="H50" s="22"/>
+      <c r="I50" s="23"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="46"/>
-      <c r="B51" s="56"/>
-      <c r="C51" s="56"/>
-      <c r="D51" s="32"/>
-      <c r="E51" s="33"/>
-      <c r="F51" s="33"/>
-      <c r="G51" s="33"/>
-      <c r="H51" s="33"/>
-      <c r="I51" s="34"/>
+      <c r="A51" s="31"/>
+      <c r="B51" s="33"/>
+      <c r="C51" s="33"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="25"/>
+      <c r="F51" s="25"/>
+      <c r="G51" s="25"/>
+      <c r="H51" s="25"/>
+      <c r="I51" s="26"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="47"/>
-      <c r="B52" s="57"/>
-      <c r="C52" s="57"/>
-      <c r="D52" s="52"/>
-      <c r="E52" s="53"/>
-      <c r="F52" s="53"/>
-      <c r="G52" s="53"/>
-      <c r="H52" s="53"/>
-      <c r="I52" s="54"/>
+      <c r="A52" s="32"/>
+      <c r="B52" s="34"/>
+      <c r="C52" s="34"/>
+      <c r="D52" s="27"/>
+      <c r="E52" s="28"/>
+      <c r="F52" s="28"/>
+      <c r="G52" s="28"/>
+      <c r="H52" s="28"/>
+      <c r="I52" s="29"/>
     </row>
     <row r="53" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A53" s="45">
+      <c r="A53" s="30">
         <v>4</v>
       </c>
-      <c r="B53" s="48" t="s">
+      <c r="B53" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C53" s="49"/>
-      <c r="D53" s="49"/>
-      <c r="E53" s="49"/>
-      <c r="F53" s="49"/>
-      <c r="G53" s="49"/>
-      <c r="H53" s="49"/>
-      <c r="I53" s="50"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="19"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="19"/>
+      <c r="I53" s="20"/>
     </row>
     <row r="54" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="46"/>
-      <c r="B54" s="46" t="s">
+      <c r="A54" s="31"/>
+      <c r="B54" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C54" s="51" t="s">
+      <c r="C54" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D54" s="38"/>
-      <c r="E54" s="38"/>
-      <c r="F54" s="38"/>
-      <c r="G54" s="38"/>
-      <c r="H54" s="38"/>
-      <c r="I54" s="39"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="22"/>
+      <c r="F54" s="22"/>
+      <c r="G54" s="22"/>
+      <c r="H54" s="22"/>
+      <c r="I54" s="23"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="46"/>
-      <c r="B55" s="46"/>
-      <c r="C55" s="32"/>
-      <c r="D55" s="33"/>
-      <c r="E55" s="33"/>
-      <c r="F55" s="33"/>
-      <c r="G55" s="33"/>
-      <c r="H55" s="33"/>
-      <c r="I55" s="34"/>
+      <c r="A55" s="31"/>
+      <c r="B55" s="31"/>
+      <c r="C55" s="24"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="25"/>
+      <c r="F55" s="25"/>
+      <c r="G55" s="25"/>
+      <c r="H55" s="25"/>
+      <c r="I55" s="26"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="46"/>
-      <c r="B56" s="46"/>
-      <c r="C56" s="32"/>
-      <c r="D56" s="33"/>
-      <c r="E56" s="33"/>
-      <c r="F56" s="33"/>
-      <c r="G56" s="33"/>
-      <c r="H56" s="33"/>
-      <c r="I56" s="34"/>
+      <c r="A56" s="31"/>
+      <c r="B56" s="31"/>
+      <c r="C56" s="24"/>
+      <c r="D56" s="25"/>
+      <c r="E56" s="25"/>
+      <c r="F56" s="25"/>
+      <c r="G56" s="25"/>
+      <c r="H56" s="25"/>
+      <c r="I56" s="26"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="46"/>
-      <c r="B57" s="46"/>
-      <c r="C57" s="32"/>
-      <c r="D57" s="33"/>
-      <c r="E57" s="33"/>
-      <c r="F57" s="33"/>
-      <c r="G57" s="33"/>
-      <c r="H57" s="33"/>
-      <c r="I57" s="34"/>
+      <c r="A57" s="31"/>
+      <c r="B57" s="31"/>
+      <c r="C57" s="24"/>
+      <c r="D57" s="25"/>
+      <c r="E57" s="25"/>
+      <c r="F57" s="25"/>
+      <c r="G57" s="25"/>
+      <c r="H57" s="25"/>
+      <c r="I57" s="26"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="46"/>
-      <c r="B58" s="46"/>
-      <c r="C58" s="32"/>
-      <c r="D58" s="33"/>
-      <c r="E58" s="33"/>
-      <c r="F58" s="33"/>
-      <c r="G58" s="33"/>
-      <c r="H58" s="33"/>
-      <c r="I58" s="34"/>
+      <c r="A58" s="31"/>
+      <c r="B58" s="31"/>
+      <c r="C58" s="24"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="25"/>
+      <c r="F58" s="25"/>
+      <c r="G58" s="25"/>
+      <c r="H58" s="25"/>
+      <c r="I58" s="26"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="46"/>
-      <c r="B59" s="46"/>
-      <c r="C59" s="32"/>
-      <c r="D59" s="33"/>
-      <c r="E59" s="33"/>
-      <c r="F59" s="33"/>
-      <c r="G59" s="33"/>
-      <c r="H59" s="33"/>
-      <c r="I59" s="34"/>
+      <c r="A59" s="31"/>
+      <c r="B59" s="31"/>
+      <c r="C59" s="24"/>
+      <c r="D59" s="25"/>
+      <c r="E59" s="25"/>
+      <c r="F59" s="25"/>
+      <c r="G59" s="25"/>
+      <c r="H59" s="25"/>
+      <c r="I59" s="26"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="46"/>
-      <c r="B60" s="46"/>
-      <c r="C60" s="32"/>
-      <c r="D60" s="33"/>
-      <c r="E60" s="33"/>
-      <c r="F60" s="33"/>
-      <c r="G60" s="33"/>
-      <c r="H60" s="33"/>
-      <c r="I60" s="34"/>
+      <c r="A60" s="31"/>
+      <c r="B60" s="31"/>
+      <c r="C60" s="24"/>
+      <c r="D60" s="25"/>
+      <c r="E60" s="25"/>
+      <c r="F60" s="25"/>
+      <c r="G60" s="25"/>
+      <c r="H60" s="25"/>
+      <c r="I60" s="26"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="46"/>
-      <c r="B61" s="46"/>
-      <c r="C61" s="32"/>
-      <c r="D61" s="33"/>
-      <c r="E61" s="33"/>
-      <c r="F61" s="33"/>
-      <c r="G61" s="33"/>
-      <c r="H61" s="33"/>
-      <c r="I61" s="34"/>
+      <c r="A61" s="31"/>
+      <c r="B61" s="31"/>
+      <c r="C61" s="24"/>
+      <c r="D61" s="25"/>
+      <c r="E61" s="25"/>
+      <c r="F61" s="25"/>
+      <c r="G61" s="25"/>
+      <c r="H61" s="25"/>
+      <c r="I61" s="26"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="46"/>
-      <c r="B62" s="46"/>
-      <c r="C62" s="32"/>
-      <c r="D62" s="33"/>
-      <c r="E62" s="33"/>
-      <c r="F62" s="33"/>
-      <c r="G62" s="33"/>
-      <c r="H62" s="33"/>
-      <c r="I62" s="34"/>
+      <c r="A62" s="31"/>
+      <c r="B62" s="31"/>
+      <c r="C62" s="24"/>
+      <c r="D62" s="25"/>
+      <c r="E62" s="25"/>
+      <c r="F62" s="25"/>
+      <c r="G62" s="25"/>
+      <c r="H62" s="25"/>
+      <c r="I62" s="26"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="47"/>
-      <c r="B63" s="47"/>
-      <c r="C63" s="52"/>
-      <c r="D63" s="53"/>
-      <c r="E63" s="53"/>
-      <c r="F63" s="53"/>
-      <c r="G63" s="53"/>
-      <c r="H63" s="53"/>
-      <c r="I63" s="54"/>
+      <c r="A63" s="32"/>
+      <c r="B63" s="32"/>
+      <c r="C63" s="27"/>
+      <c r="D63" s="28"/>
+      <c r="E63" s="28"/>
+      <c r="F63" s="28"/>
+      <c r="G63" s="28"/>
+      <c r="H63" s="28"/>
+      <c r="I63" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="B53:I53"/>
-    <mergeCell ref="C54:I63"/>
-    <mergeCell ref="A53:A63"/>
-    <mergeCell ref="B54:B63"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="A43:A52"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="A19:A29"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I9"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A11:I18"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="E29:I29"/>
     <mergeCell ref="A30:A42"/>
     <mergeCell ref="B43:I43"/>
     <mergeCell ref="D47:I49"/>
@@ -2605,32 +2623,14 @@
     <mergeCell ref="D44:I46"/>
     <mergeCell ref="B30:I30"/>
     <mergeCell ref="C37:I37"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="E28:I28"/>
-    <mergeCell ref="E29:I29"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I9"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A11:I18"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="A19:A29"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="B53:I53"/>
+    <mergeCell ref="C54:I63"/>
+    <mergeCell ref="A53:A63"/>
+    <mergeCell ref="B54:B63"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="A43:A52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -3697,8 +3697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D9410B-47BB-4E45-80F2-F71FCE9008EE}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D6" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Nothing really changed. I have to commit though.
</commit_message>
<xml_diff>
--- a/documentation/VD/source/procedures.xlsx
+++ b/documentation/VD/source/procedures.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462964C0-51D8-4273-BFA3-B7F2B2ECA507}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D35A4B-CE70-40D9-B03E-497B7448F0E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10248" yWindow="3948" windowWidth="17280" windowHeight="11508" tabRatio="1000" firstSheet="20" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="1000" firstSheet="20" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="2" r:id="rId1"/>
@@ -1908,150 +1908,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2111,6 +1967,150 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2406,846 +2406,828 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="49" t="s">
         <v>306</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="57"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="51"/>
     </row>
     <row r="2" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="60"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="54"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="58"/>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="60"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="54"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="58"/>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="60"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="54"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="58"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="60"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="54"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="58"/>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="60"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="54"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="58"/>
-      <c r="B7" s="59"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="59"/>
-      <c r="H7" s="59"/>
-      <c r="I7" s="60"/>
+      <c r="A7" s="52"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="54"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="58"/>
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="59"/>
-      <c r="I8" s="60"/>
+      <c r="A8" s="52"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="54"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="58"/>
-      <c r="B9" s="59"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="59"/>
-      <c r="H9" s="59"/>
-      <c r="I9" s="60"/>
+      <c r="A9" s="52"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="54"/>
     </row>
     <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="61" t="s">
+      <c r="A10" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="62"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="63"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="57"/>
     </row>
     <row r="11" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="32"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="60"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="30"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="32"/>
+      <c r="A12" s="58"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="60"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="30"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="32"/>
+      <c r="A13" s="58"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="60"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="30"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="32"/>
+      <c r="A14" s="58"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="59"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="60"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="30"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="32"/>
+      <c r="A15" s="58"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="60"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="30"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="32"/>
+      <c r="A16" s="58"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="59"/>
+      <c r="H16" s="59"/>
+      <c r="I16" s="60"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="30"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="32"/>
+      <c r="A17" s="58"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="60"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="30"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="32"/>
+      <c r="A18" s="58"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="59"/>
+      <c r="H18" s="59"/>
+      <c r="I18" s="60"/>
     </row>
     <row r="19" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="69">
+      <c r="A19" s="46">
         <v>1</v>
       </c>
-      <c r="B19" s="64" t="s">
+      <c r="B19" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="65"/>
-      <c r="D19" s="65"/>
-      <c r="E19" s="65"/>
-      <c r="F19" s="65"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="65"/>
-      <c r="I19" s="66"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="62"/>
+      <c r="I19" s="63"/>
     </row>
     <row r="20" spans="1:9" ht="20.7" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="70"/>
+      <c r="A20" s="47"/>
       <c r="B20" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="67" t="s">
+      <c r="C20" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="68"/>
-      <c r="E20" s="28" t="s">
+      <c r="D20" s="45"/>
+      <c r="E20" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="29"/>
+      <c r="F20" s="64"/>
+      <c r="G20" s="64"/>
+      <c r="H20" s="64"/>
+      <c r="I20" s="65"/>
     </row>
     <row r="21" spans="1:9" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="70"/>
+      <c r="A21" s="47"/>
       <c r="B21" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="67" t="s">
+      <c r="C21" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="68"/>
-      <c r="E21" s="28" t="s">
+      <c r="D21" s="45"/>
+      <c r="E21" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="29"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="64"/>
+      <c r="H21" s="64"/>
+      <c r="I21" s="65"/>
     </row>
     <row r="22" spans="1:9" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="70"/>
+      <c r="A22" s="47"/>
       <c r="B22" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="67" t="s">
+      <c r="C22" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="68"/>
-      <c r="E22" s="28" t="s">
+      <c r="D22" s="45"/>
+      <c r="E22" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="29"/>
+      <c r="F22" s="64"/>
+      <c r="G22" s="64"/>
+      <c r="H22" s="64"/>
+      <c r="I22" s="65"/>
     </row>
     <row r="23" spans="1:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="70"/>
+      <c r="A23" s="47"/>
       <c r="B23" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="67" t="s">
+      <c r="C23" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="68"/>
-      <c r="E23" s="28" t="s">
+      <c r="D23" s="45"/>
+      <c r="E23" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="29"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="64"/>
+      <c r="H23" s="64"/>
+      <c r="I23" s="65"/>
     </row>
     <row r="24" spans="1:9" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="70"/>
+      <c r="A24" s="47"/>
       <c r="B24" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="67" t="s">
+      <c r="C24" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="68"/>
-      <c r="E24" s="28" t="s">
+      <c r="D24" s="45"/>
+      <c r="E24" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="29"/>
+      <c r="F24" s="64"/>
+      <c r="G24" s="64"/>
+      <c r="H24" s="64"/>
+      <c r="I24" s="65"/>
     </row>
     <row r="25" spans="1:9" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="70"/>
+      <c r="A25" s="47"/>
       <c r="B25" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="67" t="s">
+      <c r="C25" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="68"/>
-      <c r="E25" s="28" t="s">
+      <c r="D25" s="45"/>
+      <c r="E25" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="29"/>
+      <c r="F25" s="64"/>
+      <c r="G25" s="64"/>
+      <c r="H25" s="64"/>
+      <c r="I25" s="65"/>
     </row>
     <row r="26" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="70"/>
+      <c r="A26" s="47"/>
       <c r="B26" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C26" s="67" t="s">
+      <c r="C26" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="68"/>
-      <c r="E26" s="28" t="s">
+      <c r="D26" s="45"/>
+      <c r="E26" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="29"/>
+      <c r="F26" s="64"/>
+      <c r="G26" s="64"/>
+      <c r="H26" s="64"/>
+      <c r="I26" s="65"/>
     </row>
     <row r="27" spans="1:9" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="70"/>
+      <c r="A27" s="47"/>
       <c r="B27" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="67" t="s">
+      <c r="C27" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="68"/>
-      <c r="E27" s="28" t="s">
+      <c r="D27" s="45"/>
+      <c r="E27" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="29"/>
+      <c r="F27" s="64"/>
+      <c r="G27" s="64"/>
+      <c r="H27" s="64"/>
+      <c r="I27" s="65"/>
     </row>
     <row r="28" spans="1:9" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="70"/>
+      <c r="A28" s="47"/>
       <c r="B28" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="67" t="s">
+      <c r="C28" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="68"/>
-      <c r="E28" s="28" t="s">
+      <c r="D28" s="45"/>
+      <c r="E28" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="F28" s="51"/>
-      <c r="G28" s="51"/>
-      <c r="H28" s="51"/>
-      <c r="I28" s="52"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="66"/>
+      <c r="H28" s="66"/>
+      <c r="I28" s="67"/>
     </row>
     <row r="29" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="71"/>
+      <c r="A29" s="48"/>
       <c r="B29" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="67" t="s">
+      <c r="C29" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="68"/>
-      <c r="E29" s="43" t="s">
+      <c r="D29" s="45"/>
+      <c r="E29" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="F29" s="53"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="54"/>
+      <c r="F29" s="69"/>
+      <c r="G29" s="69"/>
+      <c r="H29" s="69"/>
+      <c r="I29" s="70"/>
     </row>
     <row r="30" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="36">
+      <c r="A30" s="71">
         <v>2</v>
       </c>
-      <c r="B30" s="25" t="s">
+      <c r="B30" s="75" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="26"/>
+      <c r="C30" s="75"/>
+      <c r="D30" s="75"/>
+      <c r="E30" s="75"/>
+      <c r="F30" s="75"/>
+      <c r="G30" s="75"/>
+      <c r="H30" s="75"/>
+      <c r="I30" s="76"/>
     </row>
     <row r="31" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="37"/>
+      <c r="A31" s="72"/>
       <c r="B31" s="9"/>
-      <c r="C31" s="27" t="s">
+      <c r="C31" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="28"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="29"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="64"/>
+      <c r="H31" s="64"/>
+      <c r="I31" s="65"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="37"/>
+      <c r="A32" s="72"/>
       <c r="B32" s="9"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="32"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="59"/>
+      <c r="F32" s="59"/>
+      <c r="G32" s="59"/>
+      <c r="H32" s="59"/>
+      <c r="I32" s="60"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="37"/>
+      <c r="A33" s="72"/>
       <c r="B33" s="9"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="32"/>
+      <c r="C33" s="58"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="59"/>
+      <c r="H33" s="59"/>
+      <c r="I33" s="60"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="37"/>
+      <c r="A34" s="72"/>
       <c r="B34" s="9"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="32"/>
+      <c r="C34" s="58"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="59"/>
+      <c r="F34" s="59"/>
+      <c r="G34" s="59"/>
+      <c r="H34" s="59"/>
+      <c r="I34" s="60"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="37"/>
+      <c r="A35" s="72"/>
       <c r="B35" s="9"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="31"/>
-      <c r="I35" s="32"/>
+      <c r="C35" s="58"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="59"/>
+      <c r="H35" s="59"/>
+      <c r="I35" s="60"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="37"/>
+      <c r="A36" s="72"/>
       <c r="B36" s="9"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="31"/>
-      <c r="H36" s="31"/>
-      <c r="I36" s="32"/>
+      <c r="C36" s="58"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="59"/>
+      <c r="F36" s="59"/>
+      <c r="G36" s="59"/>
+      <c r="H36" s="59"/>
+      <c r="I36" s="60"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="37"/>
+      <c r="A37" s="72"/>
       <c r="B37" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="48" t="s">
+      <c r="C37" s="89" t="s">
         <v>53</v>
       </c>
-      <c r="D37" s="49"/>
-      <c r="E37" s="49"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="49"/>
-      <c r="H37" s="49"/>
-      <c r="I37" s="50"/>
+      <c r="D37" s="90"/>
+      <c r="E37" s="90"/>
+      <c r="F37" s="90"/>
+      <c r="G37" s="90"/>
+      <c r="H37" s="90"/>
+      <c r="I37" s="91"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="37"/>
+      <c r="A38" s="72"/>
       <c r="B38" s="11"/>
       <c r="C38" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D38" s="27" t="s">
+      <c r="D38" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="28"/>
-      <c r="H38" s="28"/>
-      <c r="I38" s="29"/>
+      <c r="E38" s="64"/>
+      <c r="F38" s="64"/>
+      <c r="G38" s="64"/>
+      <c r="H38" s="64"/>
+      <c r="I38" s="65"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="37"/>
+      <c r="A39" s="72"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="31"/>
-      <c r="H39" s="31"/>
-      <c r="I39" s="32"/>
+      <c r="D39" s="58"/>
+      <c r="E39" s="59"/>
+      <c r="F39" s="59"/>
+      <c r="G39" s="59"/>
+      <c r="H39" s="59"/>
+      <c r="I39" s="60"/>
     </row>
     <row r="40" spans="1:9" ht="18.3" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="37"/>
+      <c r="A40" s="72"/>
       <c r="B40" s="11"/>
       <c r="C40" s="14"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="34"/>
-      <c r="G40" s="34"/>
-      <c r="H40" s="34"/>
-      <c r="I40" s="35"/>
+      <c r="D40" s="78"/>
+      <c r="E40" s="79"/>
+      <c r="F40" s="79"/>
+      <c r="G40" s="79"/>
+      <c r="H40" s="79"/>
+      <c r="I40" s="80"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="37"/>
+      <c r="A41" s="72"/>
       <c r="B41" s="11"/>
       <c r="C41" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D41" s="42" t="s">
+      <c r="D41" s="84" t="s">
         <v>56</v>
       </c>
-      <c r="E41" s="43"/>
-      <c r="F41" s="43"/>
-      <c r="G41" s="43"/>
-      <c r="H41" s="43"/>
-      <c r="I41" s="44"/>
+      <c r="E41" s="68"/>
+      <c r="F41" s="68"/>
+      <c r="G41" s="68"/>
+      <c r="H41" s="68"/>
+      <c r="I41" s="85"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="38"/>
+      <c r="A42" s="73"/>
       <c r="B42" s="14"/>
       <c r="C42" s="14"/>
-      <c r="D42" s="45"/>
-      <c r="E42" s="46"/>
-      <c r="F42" s="46"/>
-      <c r="G42" s="46"/>
-      <c r="H42" s="46"/>
-      <c r="I42" s="47"/>
+      <c r="D42" s="86"/>
+      <c r="E42" s="87"/>
+      <c r="F42" s="87"/>
+      <c r="G42" s="87"/>
+      <c r="H42" s="87"/>
+      <c r="I42" s="88"/>
     </row>
     <row r="43" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A43" s="36">
+      <c r="A43" s="71">
         <v>3</v>
       </c>
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="74" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="25"/>
-      <c r="I43" s="26"/>
+      <c r="C43" s="75"/>
+      <c r="D43" s="75"/>
+      <c r="E43" s="75"/>
+      <c r="F43" s="75"/>
+      <c r="G43" s="75"/>
+      <c r="H43" s="75"/>
+      <c r="I43" s="76"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="37"/>
-      <c r="B44" s="39" t="s">
+      <c r="A44" s="72"/>
+      <c r="B44" s="82" t="s">
         <v>31</v>
       </c>
-      <c r="C44" s="41" t="s">
+      <c r="C44" s="81" t="s">
         <v>57</v>
       </c>
-      <c r="D44" s="27" t="s">
+      <c r="D44" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="E44" s="28"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="28"/>
-      <c r="H44" s="28"/>
-      <c r="I44" s="29"/>
+      <c r="E44" s="64"/>
+      <c r="F44" s="64"/>
+      <c r="G44" s="64"/>
+      <c r="H44" s="64"/>
+      <c r="I44" s="65"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="37"/>
-      <c r="B45" s="39"/>
-      <c r="C45" s="39"/>
-      <c r="D45" s="30"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="31"/>
-      <c r="H45" s="31"/>
-      <c r="I45" s="32"/>
+      <c r="A45" s="72"/>
+      <c r="B45" s="82"/>
+      <c r="C45" s="82"/>
+      <c r="D45" s="58"/>
+      <c r="E45" s="59"/>
+      <c r="F45" s="59"/>
+      <c r="G45" s="59"/>
+      <c r="H45" s="59"/>
+      <c r="I45" s="60"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="37"/>
-      <c r="B46" s="39"/>
-      <c r="C46" s="40"/>
-      <c r="D46" s="33"/>
-      <c r="E46" s="34"/>
-      <c r="F46" s="34"/>
-      <c r="G46" s="34"/>
-      <c r="H46" s="34"/>
-      <c r="I46" s="35"/>
+      <c r="A46" s="72"/>
+      <c r="B46" s="82"/>
+      <c r="C46" s="83"/>
+      <c r="D46" s="78"/>
+      <c r="E46" s="79"/>
+      <c r="F46" s="79"/>
+      <c r="G46" s="79"/>
+      <c r="H46" s="79"/>
+      <c r="I46" s="80"/>
     </row>
     <row r="47" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="37"/>
-      <c r="B47" s="39" t="s">
+      <c r="A47" s="72"/>
+      <c r="B47" s="82" t="s">
         <v>32</v>
       </c>
-      <c r="C47" s="41" t="s">
+      <c r="C47" s="81" t="s">
         <v>58</v>
       </c>
-      <c r="D47" s="27" t="s">
+      <c r="D47" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="E47" s="28"/>
-      <c r="F47" s="28"/>
-      <c r="G47" s="28"/>
-      <c r="H47" s="28"/>
-      <c r="I47" s="29"/>
+      <c r="E47" s="64"/>
+      <c r="F47" s="64"/>
+      <c r="G47" s="64"/>
+      <c r="H47" s="64"/>
+      <c r="I47" s="65"/>
     </row>
     <row r="48" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="37"/>
-      <c r="B48" s="39"/>
-      <c r="C48" s="39"/>
-      <c r="D48" s="30"/>
-      <c r="E48" s="31"/>
-      <c r="F48" s="31"/>
-      <c r="G48" s="31"/>
-      <c r="H48" s="31"/>
-      <c r="I48" s="32"/>
+      <c r="A48" s="72"/>
+      <c r="B48" s="82"/>
+      <c r="C48" s="82"/>
+      <c r="D48" s="58"/>
+      <c r="E48" s="59"/>
+      <c r="F48" s="59"/>
+      <c r="G48" s="59"/>
+      <c r="H48" s="59"/>
+      <c r="I48" s="60"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="37"/>
-      <c r="B49" s="39"/>
-      <c r="C49" s="40"/>
-      <c r="D49" s="33"/>
-      <c r="E49" s="34"/>
-      <c r="F49" s="34"/>
-      <c r="G49" s="34"/>
-      <c r="H49" s="34"/>
-      <c r="I49" s="35"/>
+      <c r="A49" s="72"/>
+      <c r="B49" s="82"/>
+      <c r="C49" s="83"/>
+      <c r="D49" s="78"/>
+      <c r="E49" s="79"/>
+      <c r="F49" s="79"/>
+      <c r="G49" s="79"/>
+      <c r="H49" s="79"/>
+      <c r="I49" s="80"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="37"/>
-      <c r="B50" s="39" t="s">
+      <c r="A50" s="72"/>
+      <c r="B50" s="82" t="s">
         <v>33</v>
       </c>
-      <c r="C50" s="39" t="s">
+      <c r="C50" s="82" t="s">
         <v>62</v>
       </c>
-      <c r="D50" s="27" t="s">
+      <c r="D50" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="E50" s="28"/>
-      <c r="F50" s="28"/>
-      <c r="G50" s="28"/>
-      <c r="H50" s="28"/>
-      <c r="I50" s="29"/>
+      <c r="E50" s="64"/>
+      <c r="F50" s="64"/>
+      <c r="G50" s="64"/>
+      <c r="H50" s="64"/>
+      <c r="I50" s="65"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="37"/>
-      <c r="B51" s="39"/>
-      <c r="C51" s="39"/>
-      <c r="D51" s="30"/>
-      <c r="E51" s="31"/>
-      <c r="F51" s="31"/>
-      <c r="G51" s="31"/>
-      <c r="H51" s="31"/>
-      <c r="I51" s="32"/>
+      <c r="A51" s="72"/>
+      <c r="B51" s="82"/>
+      <c r="C51" s="82"/>
+      <c r="D51" s="58"/>
+      <c r="E51" s="59"/>
+      <c r="F51" s="59"/>
+      <c r="G51" s="59"/>
+      <c r="H51" s="59"/>
+      <c r="I51" s="60"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="38"/>
-      <c r="B52" s="40"/>
-      <c r="C52" s="40"/>
-      <c r="D52" s="33"/>
-      <c r="E52" s="34"/>
-      <c r="F52" s="34"/>
-      <c r="G52" s="34"/>
-      <c r="H52" s="34"/>
-      <c r="I52" s="35"/>
+      <c r="A52" s="73"/>
+      <c r="B52" s="83"/>
+      <c r="C52" s="83"/>
+      <c r="D52" s="78"/>
+      <c r="E52" s="79"/>
+      <c r="F52" s="79"/>
+      <c r="G52" s="79"/>
+      <c r="H52" s="79"/>
+      <c r="I52" s="80"/>
     </row>
     <row r="53" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A53" s="36">
+      <c r="A53" s="71">
         <v>4</v>
       </c>
-      <c r="B53" s="24" t="s">
+      <c r="B53" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="25"/>
-      <c r="G53" s="25"/>
-      <c r="H53" s="25"/>
-      <c r="I53" s="26"/>
+      <c r="C53" s="75"/>
+      <c r="D53" s="75"/>
+      <c r="E53" s="75"/>
+      <c r="F53" s="75"/>
+      <c r="G53" s="75"/>
+      <c r="H53" s="75"/>
+      <c r="I53" s="76"/>
     </row>
     <row r="54" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="37"/>
-      <c r="B54" s="37" t="s">
+      <c r="A54" s="72"/>
+      <c r="B54" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="C54" s="27" t="s">
+      <c r="C54" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="D54" s="28"/>
-      <c r="E54" s="28"/>
-      <c r="F54" s="28"/>
-      <c r="G54" s="28"/>
-      <c r="H54" s="28"/>
-      <c r="I54" s="29"/>
+      <c r="D54" s="64"/>
+      <c r="E54" s="64"/>
+      <c r="F54" s="64"/>
+      <c r="G54" s="64"/>
+      <c r="H54" s="64"/>
+      <c r="I54" s="65"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="37"/>
-      <c r="B55" s="37"/>
-      <c r="C55" s="30"/>
-      <c r="D55" s="31"/>
-      <c r="E55" s="31"/>
-      <c r="F55" s="31"/>
-      <c r="G55" s="31"/>
-      <c r="H55" s="31"/>
-      <c r="I55" s="32"/>
+      <c r="A55" s="72"/>
+      <c r="B55" s="72"/>
+      <c r="C55" s="58"/>
+      <c r="D55" s="59"/>
+      <c r="E55" s="59"/>
+      <c r="F55" s="59"/>
+      <c r="G55" s="59"/>
+      <c r="H55" s="59"/>
+      <c r="I55" s="60"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="37"/>
-      <c r="B56" s="37"/>
-      <c r="C56" s="30"/>
-      <c r="D56" s="31"/>
-      <c r="E56" s="31"/>
-      <c r="F56" s="31"/>
-      <c r="G56" s="31"/>
-      <c r="H56" s="31"/>
-      <c r="I56" s="32"/>
+      <c r="A56" s="72"/>
+      <c r="B56" s="72"/>
+      <c r="C56" s="58"/>
+      <c r="D56" s="59"/>
+      <c r="E56" s="59"/>
+      <c r="F56" s="59"/>
+      <c r="G56" s="59"/>
+      <c r="H56" s="59"/>
+      <c r="I56" s="60"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="37"/>
-      <c r="B57" s="37"/>
-      <c r="C57" s="30"/>
-      <c r="D57" s="31"/>
-      <c r="E57" s="31"/>
-      <c r="F57" s="31"/>
-      <c r="G57" s="31"/>
-      <c r="H57" s="31"/>
-      <c r="I57" s="32"/>
+      <c r="A57" s="72"/>
+      <c r="B57" s="72"/>
+      <c r="C57" s="58"/>
+      <c r="D57" s="59"/>
+      <c r="E57" s="59"/>
+      <c r="F57" s="59"/>
+      <c r="G57" s="59"/>
+      <c r="H57" s="59"/>
+      <c r="I57" s="60"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="37"/>
-      <c r="B58" s="37"/>
-      <c r="C58" s="30"/>
-      <c r="D58" s="31"/>
-      <c r="E58" s="31"/>
-      <c r="F58" s="31"/>
-      <c r="G58" s="31"/>
-      <c r="H58" s="31"/>
-      <c r="I58" s="32"/>
+      <c r="A58" s="72"/>
+      <c r="B58" s="72"/>
+      <c r="C58" s="58"/>
+      <c r="D58" s="59"/>
+      <c r="E58" s="59"/>
+      <c r="F58" s="59"/>
+      <c r="G58" s="59"/>
+      <c r="H58" s="59"/>
+      <c r="I58" s="60"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="37"/>
-      <c r="B59" s="37"/>
-      <c r="C59" s="30"/>
-      <c r="D59" s="31"/>
-      <c r="E59" s="31"/>
-      <c r="F59" s="31"/>
-      <c r="G59" s="31"/>
-      <c r="H59" s="31"/>
-      <c r="I59" s="32"/>
+      <c r="A59" s="72"/>
+      <c r="B59" s="72"/>
+      <c r="C59" s="58"/>
+      <c r="D59" s="59"/>
+      <c r="E59" s="59"/>
+      <c r="F59" s="59"/>
+      <c r="G59" s="59"/>
+      <c r="H59" s="59"/>
+      <c r="I59" s="60"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="37"/>
-      <c r="B60" s="37"/>
-      <c r="C60" s="30"/>
-      <c r="D60" s="31"/>
-      <c r="E60" s="31"/>
-      <c r="F60" s="31"/>
-      <c r="G60" s="31"/>
-      <c r="H60" s="31"/>
-      <c r="I60" s="32"/>
+      <c r="A60" s="72"/>
+      <c r="B60" s="72"/>
+      <c r="C60" s="58"/>
+      <c r="D60" s="59"/>
+      <c r="E60" s="59"/>
+      <c r="F60" s="59"/>
+      <c r="G60" s="59"/>
+      <c r="H60" s="59"/>
+      <c r="I60" s="60"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="37"/>
-      <c r="B61" s="37"/>
-      <c r="C61" s="30"/>
-      <c r="D61" s="31"/>
-      <c r="E61" s="31"/>
-      <c r="F61" s="31"/>
-      <c r="G61" s="31"/>
-      <c r="H61" s="31"/>
-      <c r="I61" s="32"/>
+      <c r="A61" s="72"/>
+      <c r="B61" s="72"/>
+      <c r="C61" s="58"/>
+      <c r="D61" s="59"/>
+      <c r="E61" s="59"/>
+      <c r="F61" s="59"/>
+      <c r="G61" s="59"/>
+      <c r="H61" s="59"/>
+      <c r="I61" s="60"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="37"/>
-      <c r="B62" s="37"/>
-      <c r="C62" s="30"/>
-      <c r="D62" s="31"/>
-      <c r="E62" s="31"/>
-      <c r="F62" s="31"/>
-      <c r="G62" s="31"/>
-      <c r="H62" s="31"/>
-      <c r="I62" s="32"/>
+      <c r="A62" s="72"/>
+      <c r="B62" s="72"/>
+      <c r="C62" s="58"/>
+      <c r="D62" s="59"/>
+      <c r="E62" s="59"/>
+      <c r="F62" s="59"/>
+      <c r="G62" s="59"/>
+      <c r="H62" s="59"/>
+      <c r="I62" s="60"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="38"/>
-      <c r="B63" s="38"/>
-      <c r="C63" s="33"/>
-      <c r="D63" s="34"/>
-      <c r="E63" s="34"/>
-      <c r="F63" s="34"/>
-      <c r="G63" s="34"/>
-      <c r="H63" s="34"/>
-      <c r="I63" s="35"/>
+      <c r="A63" s="73"/>
+      <c r="B63" s="73"/>
+      <c r="C63" s="78"/>
+      <c r="D63" s="79"/>
+      <c r="E63" s="79"/>
+      <c r="F63" s="79"/>
+      <c r="G63" s="79"/>
+      <c r="H63" s="79"/>
+      <c r="I63" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="A19:A29"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I9"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A11:I18"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="E28:I28"/>
-    <mergeCell ref="E29:I29"/>
+    <mergeCell ref="B53:I53"/>
+    <mergeCell ref="C54:I63"/>
+    <mergeCell ref="A53:A63"/>
+    <mergeCell ref="B54:B63"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="A43:A52"/>
     <mergeCell ref="A30:A42"/>
     <mergeCell ref="B43:I43"/>
     <mergeCell ref="D47:I49"/>
@@ -3259,14 +3241,32 @@
     <mergeCell ref="D44:I46"/>
     <mergeCell ref="B30:I30"/>
     <mergeCell ref="C37:I37"/>
-    <mergeCell ref="B53:I53"/>
-    <mergeCell ref="C54:I63"/>
-    <mergeCell ref="A53:A63"/>
-    <mergeCell ref="B54:B63"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="A43:A52"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="E29:I29"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I9"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A11:I18"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="A19:A29"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -5501,595 +5501,595 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.109375" style="76" customWidth="1"/>
-    <col min="2" max="2" width="34.77734375" style="76" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" style="76" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" style="76" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" style="76" customWidth="1"/>
-    <col min="6" max="6" width="19" style="76" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" style="76" customWidth="1"/>
-    <col min="8" max="8" width="20.21875" style="76" customWidth="1"/>
-    <col min="9" max="9" width="27.44140625" style="76" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" style="76" customWidth="1"/>
-    <col min="11" max="13" width="8.88671875" style="76"/>
-    <col min="14" max="14" width="18" style="76" customWidth="1"/>
-    <col min="15" max="15" width="35.6640625" style="76" customWidth="1"/>
-    <col min="16" max="16" width="15.6640625" style="76" customWidth="1"/>
-    <col min="17" max="17" width="18.6640625" style="76" customWidth="1"/>
-    <col min="18" max="18" width="16.77734375" style="76" customWidth="1"/>
-    <col min="19" max="19" width="19.44140625" style="76" customWidth="1"/>
-    <col min="20" max="20" width="17.77734375" style="76" customWidth="1"/>
-    <col min="21" max="21" width="17.109375" style="76" customWidth="1"/>
-    <col min="22" max="22" width="17.5546875" style="76" customWidth="1"/>
-    <col min="23" max="23" width="17.109375" style="76" customWidth="1"/>
-    <col min="24" max="16384" width="8.88671875" style="76"/>
+    <col min="1" max="1" width="15.109375" style="28" customWidth="1"/>
+    <col min="2" max="2" width="34.77734375" style="28" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" style="28" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" style="28" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" style="28" customWidth="1"/>
+    <col min="6" max="6" width="19" style="28" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" style="28" customWidth="1"/>
+    <col min="8" max="8" width="20.21875" style="28" customWidth="1"/>
+    <col min="9" max="9" width="27.44140625" style="28" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" style="28" customWidth="1"/>
+    <col min="11" max="13" width="8.88671875" style="28"/>
+    <col min="14" max="14" width="18" style="28" customWidth="1"/>
+    <col min="15" max="15" width="35.6640625" style="28" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" style="28" customWidth="1"/>
+    <col min="17" max="17" width="18.6640625" style="28" customWidth="1"/>
+    <col min="18" max="18" width="16.77734375" style="28" customWidth="1"/>
+    <col min="19" max="19" width="19.44140625" style="28" customWidth="1"/>
+    <col min="20" max="20" width="17.77734375" style="28" customWidth="1"/>
+    <col min="21" max="21" width="17.109375" style="28" customWidth="1"/>
+    <col min="22" max="22" width="17.5546875" style="28" customWidth="1"/>
+    <col min="23" max="23" width="17.109375" style="28" customWidth="1"/>
+    <col min="24" max="16384" width="8.88671875" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="25" t="s">
         <v>306</v>
       </c>
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="73" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="73" t="s">
+      <c r="D1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="73" t="s">
+      <c r="E1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="73" t="s">
+      <c r="F1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="73" t="s">
+      <c r="G1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="73" t="s">
+      <c r="H1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="74" t="s">
+      <c r="I1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="75" t="s">
+      <c r="J1" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="84" t="s">
+      <c r="N1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="O1" s="84" t="s">
+      <c r="O1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="84" t="s">
+      <c r="P1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="84" t="s">
+      <c r="Q1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="R1" s="84" t="s">
+      <c r="R1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="84" t="s">
+      <c r="S1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="84" t="s">
+      <c r="T1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="U1" s="84" t="s">
+      <c r="U1" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="V1" s="84" t="s">
+      <c r="V1" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="W1" s="84" t="s">
+      <c r="W1" s="36" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="225" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="29" t="s">
         <v>207</v>
       </c>
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="30" t="s">
         <v>236</v>
       </c>
-      <c r="C2" s="77" t="s">
+      <c r="C2" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="77" t="s">
+      <c r="D2" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="78" t="s">
+      <c r="E2" s="30" t="s">
         <v>208</v>
       </c>
-      <c r="F2" s="79" t="s">
+      <c r="F2" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="77" t="s">
+      <c r="G2" s="29" t="s">
         <v>174</v>
       </c>
-      <c r="H2" s="77" t="s">
+      <c r="H2" s="29" t="s">
         <v>181</v>
       </c>
-      <c r="I2" s="80" t="s">
+      <c r="I2" s="32" t="s">
         <v>229</v>
       </c>
-      <c r="J2" s="81" t="s">
+      <c r="J2" s="33" t="s">
         <v>230</v>
       </c>
-      <c r="N2" s="78" t="s">
+      <c r="N2" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="O2" s="78" t="s">
+      <c r="O2" s="30" t="s">
         <v>236</v>
       </c>
-      <c r="P2" s="78" t="s">
+      <c r="P2" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="78" t="s">
+      <c r="Q2" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="78" t="s">
+      <c r="R2" s="30" t="s">
         <v>208</v>
       </c>
-      <c r="S2" s="78" t="s">
+      <c r="S2" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="T2" s="78" t="s">
+      <c r="T2" s="30" t="s">
         <v>174</v>
       </c>
-      <c r="U2" s="78" t="s">
+      <c r="U2" s="30" t="s">
         <v>181</v>
       </c>
-      <c r="V2" s="78" t="s">
+      <c r="V2" s="30" t="s">
         <v>229</v>
       </c>
-      <c r="W2" s="78" t="s">
+      <c r="W2" s="30" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="77"/>
-      <c r="B3" s="77"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="79" t="s">
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="77" t="s">
+      <c r="G3" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="H3" s="77" t="s">
+      <c r="H3" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="I3" s="80"/>
-      <c r="J3" s="81"/>
-      <c r="N3" s="78"/>
-      <c r="O3" s="78"/>
-      <c r="P3" s="78"/>
-      <c r="Q3" s="78"/>
-      <c r="R3" s="78"/>
-      <c r="S3" s="78" t="s">
+      <c r="I3" s="32"/>
+      <c r="J3" s="33"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
+      <c r="P3" s="30"/>
+      <c r="Q3" s="30"/>
+      <c r="R3" s="30"/>
+      <c r="S3" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="T3" s="78" t="s">
+      <c r="T3" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="U3" s="78" t="s">
+      <c r="U3" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="V3" s="78"/>
-      <c r="W3" s="78"/>
+      <c r="V3" s="30"/>
+      <c r="W3" s="30"/>
     </row>
     <row r="4" spans="1:23" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="77"/>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77" t="s">
+      <c r="A4" s="29"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="G4" s="77" t="s">
+      <c r="G4" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="H4" s="77" t="s">
+      <c r="H4" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="I4" s="80"/>
-      <c r="J4" s="81"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="78"/>
-      <c r="P4" s="78"/>
-      <c r="Q4" s="78"/>
-      <c r="R4" s="78"/>
-      <c r="S4" s="78" t="s">
+      <c r="I4" s="32"/>
+      <c r="J4" s="33"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="T4" s="78" t="s">
+      <c r="T4" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="U4" s="78" t="s">
+      <c r="U4" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="V4" s="78"/>
-      <c r="W4" s="78"/>
+      <c r="V4" s="30"/>
+      <c r="W4" s="30"/>
     </row>
     <row r="5" spans="1:23" ht="78" x14ac:dyDescent="0.3">
-      <c r="A5" s="77"/>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77" t="s">
+      <c r="A5" s="29"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="77" t="s">
+      <c r="H5" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="80"/>
-      <c r="J5" s="81"/>
-      <c r="N5" s="78"/>
-      <c r="O5" s="78"/>
-      <c r="P5" s="78"/>
-      <c r="Q5" s="78"/>
-      <c r="R5" s="78"/>
-      <c r="S5" s="78"/>
-      <c r="T5" s="78" t="s">
+      <c r="I5" s="32"/>
+      <c r="J5" s="33"/>
+      <c r="N5" s="30"/>
+      <c r="O5" s="30"/>
+      <c r="P5" s="30"/>
+      <c r="Q5" s="30"/>
+      <c r="R5" s="30"/>
+      <c r="S5" s="30"/>
+      <c r="T5" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="U5" s="78" t="s">
+      <c r="U5" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="V5" s="78"/>
-      <c r="W5" s="78"/>
+      <c r="V5" s="30"/>
+      <c r="W5" s="30"/>
     </row>
     <row r="6" spans="1:23" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="77"/>
-      <c r="B6" s="77"/>
-      <c r="C6" s="77"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="77"/>
-      <c r="G6" s="77" t="s">
+      <c r="A6" s="29"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29" t="s">
         <v>179</v>
       </c>
-      <c r="H6" s="77" t="s">
+      <c r="H6" s="29" t="s">
         <v>180</v>
       </c>
-      <c r="I6" s="80"/>
-      <c r="J6" s="81"/>
-      <c r="N6" s="78"/>
-      <c r="O6" s="78"/>
-      <c r="P6" s="78"/>
-      <c r="Q6" s="78"/>
-      <c r="R6" s="78"/>
-      <c r="S6" s="78"/>
-      <c r="T6" s="78" t="s">
+      <c r="I6" s="32"/>
+      <c r="J6" s="33"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="30"/>
+      <c r="T6" s="30" t="s">
         <v>179</v>
       </c>
-      <c r="U6" s="78" t="s">
+      <c r="U6" s="30" t="s">
         <v>180</v>
       </c>
-      <c r="V6" s="78"/>
-      <c r="W6" s="78"/>
+      <c r="V6" s="30"/>
+      <c r="W6" s="30"/>
     </row>
     <row r="7" spans="1:23" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="77"/>
-      <c r="B7" s="77"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="77"/>
-      <c r="G7" s="77" t="s">
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="H7" s="77" t="s">
+      <c r="H7" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="I7" s="80"/>
-      <c r="J7" s="81"/>
-      <c r="N7" s="78"/>
-      <c r="O7" s="78"/>
-      <c r="P7" s="78"/>
-      <c r="Q7" s="78"/>
-      <c r="R7" s="78"/>
-      <c r="S7" s="78"/>
-      <c r="T7" s="78" t="s">
+      <c r="I7" s="32"/>
+      <c r="J7" s="33"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="30"/>
+      <c r="P7" s="30"/>
+      <c r="Q7" s="30"/>
+      <c r="R7" s="30"/>
+      <c r="S7" s="30"/>
+      <c r="T7" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="U7" s="78" t="s">
+      <c r="U7" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="V7" s="78"/>
-      <c r="W7" s="78"/>
+      <c r="V7" s="30"/>
+      <c r="W7" s="30"/>
     </row>
     <row r="8" spans="1:23" ht="78" x14ac:dyDescent="0.3">
-      <c r="A8" s="77"/>
-      <c r="B8" s="77"/>
-      <c r="C8" s="77"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="77" t="s">
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="H8" s="77" t="s">
+      <c r="H8" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="I8" s="80"/>
-      <c r="J8" s="81"/>
-      <c r="N8" s="78"/>
-      <c r="O8" s="78"/>
-      <c r="P8" s="78"/>
-      <c r="Q8" s="78"/>
-      <c r="R8" s="78"/>
-      <c r="S8" s="78"/>
-      <c r="T8" s="78" t="s">
+      <c r="I8" s="32"/>
+      <c r="J8" s="33"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="30"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="30"/>
+      <c r="R8" s="30"/>
+      <c r="S8" s="30"/>
+      <c r="T8" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="U8" s="78" t="s">
+      <c r="U8" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="V8" s="78"/>
-      <c r="W8" s="78"/>
+      <c r="V8" s="30"/>
+      <c r="W8" s="30"/>
     </row>
     <row r="9" spans="1:23" ht="78" x14ac:dyDescent="0.3">
-      <c r="A9" s="82"/>
-      <c r="B9" s="82"/>
-      <c r="C9" s="82"/>
-      <c r="D9" s="82"/>
-      <c r="E9" s="82"/>
-      <c r="F9" s="82"/>
-      <c r="G9" s="77" t="s">
+      <c r="A9" s="34"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="H9" s="77" t="s">
+      <c r="H9" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="I9" s="80"/>
-      <c r="J9" s="81"/>
-      <c r="N9" s="78"/>
-      <c r="O9" s="78"/>
-      <c r="P9" s="78"/>
-      <c r="Q9" s="78"/>
-      <c r="R9" s="78"/>
-      <c r="S9" s="78"/>
-      <c r="T9" s="78" t="s">
+      <c r="I9" s="32"/>
+      <c r="J9" s="33"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="30"/>
+      <c r="R9" s="30"/>
+      <c r="S9" s="30"/>
+      <c r="T9" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="U9" s="78" t="s">
+      <c r="U9" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="V9" s="78"/>
-      <c r="W9" s="78"/>
+      <c r="V9" s="30"/>
+      <c r="W9" s="30"/>
     </row>
     <row r="10" spans="1:23" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="82"/>
-      <c r="B10" s="82"/>
-      <c r="C10" s="82"/>
-      <c r="D10" s="82"/>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="82" t="s">
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="H10" s="82" t="s">
+      <c r="H10" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="I10" s="80"/>
-      <c r="J10" s="81"/>
-      <c r="N10" s="78"/>
-      <c r="O10" s="78"/>
-      <c r="P10" s="78"/>
-      <c r="Q10" s="78"/>
-      <c r="R10" s="78"/>
-      <c r="S10" s="78"/>
-      <c r="T10" s="78" t="s">
+      <c r="I10" s="32"/>
+      <c r="J10" s="33"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="30"/>
+      <c r="R10" s="30"/>
+      <c r="S10" s="30"/>
+      <c r="T10" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="U10" s="78" t="s">
+      <c r="U10" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="V10" s="78"/>
-      <c r="W10" s="78"/>
+      <c r="V10" s="30"/>
+      <c r="W10" s="30"/>
     </row>
     <row r="11" spans="1:23" ht="78" x14ac:dyDescent="0.3">
-      <c r="A11" s="82"/>
-      <c r="B11" s="82"/>
-      <c r="C11" s="82"/>
-      <c r="D11" s="82"/>
-      <c r="E11" s="82"/>
-      <c r="F11" s="82"/>
-      <c r="G11" s="82" t="s">
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="H11" s="82" t="s">
+      <c r="H11" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="I11" s="80"/>
-      <c r="J11" s="81"/>
-      <c r="N11" s="78"/>
-      <c r="O11" s="78"/>
-      <c r="P11" s="78"/>
-      <c r="Q11" s="78"/>
-      <c r="R11" s="78"/>
-      <c r="S11" s="78"/>
-      <c r="T11" s="78" t="s">
+      <c r="I11" s="32"/>
+      <c r="J11" s="33"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="30"/>
+      <c r="R11" s="30"/>
+      <c r="S11" s="30"/>
+      <c r="T11" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="U11" s="78" t="s">
+      <c r="U11" s="30" t="s">
         <v>243</v>
       </c>
-      <c r="V11" s="78"/>
-      <c r="W11" s="78"/>
+      <c r="V11" s="30"/>
+      <c r="W11" s="30"/>
     </row>
     <row r="12" spans="1:23" ht="171.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="82"/>
-      <c r="B12" s="82"/>
-      <c r="C12" s="82"/>
-      <c r="D12" s="82"/>
-      <c r="E12" s="82"/>
-      <c r="F12" s="82"/>
-      <c r="G12" s="82" t="s">
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34" t="s">
         <v>295</v>
       </c>
-      <c r="H12" s="82" t="s">
+      <c r="H12" s="34" t="s">
         <v>296</v>
       </c>
-      <c r="I12" s="80"/>
-      <c r="J12" s="81"/>
-      <c r="N12" s="78"/>
-      <c r="O12" s="78"/>
-      <c r="P12" s="78"/>
-      <c r="Q12" s="78"/>
-      <c r="R12" s="78"/>
-      <c r="S12" s="78"/>
-      <c r="T12" s="78" t="s">
+      <c r="I12" s="32"/>
+      <c r="J12" s="33"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="30"/>
+      <c r="R12" s="30"/>
+      <c r="S12" s="30"/>
+      <c r="T12" s="30" t="s">
         <v>244</v>
       </c>
-      <c r="U12" s="78" t="s">
+      <c r="U12" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="V12" s="78"/>
-      <c r="W12" s="78"/>
+      <c r="V12" s="30"/>
+      <c r="W12" s="30"/>
     </row>
     <row r="13" spans="1:23" ht="78" x14ac:dyDescent="0.3">
-      <c r="A13" s="82"/>
-      <c r="B13" s="82"/>
-      <c r="C13" s="82"/>
-      <c r="D13" s="82"/>
-      <c r="E13" s="82"/>
-      <c r="F13" s="82"/>
-      <c r="G13" s="82"/>
-      <c r="H13" s="82"/>
-      <c r="I13" s="80"/>
-      <c r="J13" s="81"/>
-      <c r="N13" s="78"/>
-      <c r="O13" s="78"/>
-      <c r="P13" s="78"/>
-      <c r="Q13" s="78"/>
-      <c r="R13" s="78"/>
-      <c r="S13" s="78"/>
-      <c r="T13" s="78" t="s">
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="33"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="30"/>
+      <c r="R13" s="30"/>
+      <c r="S13" s="30"/>
+      <c r="T13" s="30" t="s">
         <v>219</v>
       </c>
-      <c r="U13" s="78" t="s">
+      <c r="U13" s="30" t="s">
         <v>220</v>
       </c>
-      <c r="V13" s="78"/>
-      <c r="W13" s="78"/>
+      <c r="V13" s="30"/>
+      <c r="W13" s="30"/>
     </row>
     <row r="14" spans="1:23" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="G14" s="82"/>
-      <c r="H14" s="82"/>
-      <c r="N14" s="78"/>
-      <c r="O14" s="78"/>
-      <c r="P14" s="78"/>
-      <c r="Q14" s="78"/>
-      <c r="R14" s="78"/>
-      <c r="S14" s="78"/>
-      <c r="T14" s="78" t="s">
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="30"/>
+      <c r="R14" s="30"/>
+      <c r="S14" s="30"/>
+      <c r="T14" s="30" t="s">
         <v>213</v>
       </c>
-      <c r="U14" s="78" t="s">
+      <c r="U14" s="30" t="s">
         <v>214</v>
       </c>
-      <c r="V14" s="78"/>
-      <c r="W14" s="78"/>
+      <c r="V14" s="30"/>
+      <c r="W14" s="30"/>
     </row>
     <row r="15" spans="1:23" ht="124.8" x14ac:dyDescent="0.3">
-      <c r="G15" s="82"/>
-      <c r="H15" s="82"/>
-      <c r="N15" s="78"/>
-      <c r="O15" s="78"/>
-      <c r="P15" s="78"/>
-      <c r="Q15" s="78"/>
-      <c r="R15" s="78"/>
-      <c r="S15" s="78"/>
-      <c r="T15" s="78" t="s">
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="30"/>
+      <c r="R15" s="30"/>
+      <c r="S15" s="30"/>
+      <c r="T15" s="30" t="s">
         <v>215</v>
       </c>
-      <c r="U15" s="78" t="s">
+      <c r="U15" s="30" t="s">
         <v>216</v>
       </c>
-      <c r="V15" s="78"/>
-      <c r="W15" s="78"/>
+      <c r="V15" s="30"/>
+      <c r="W15" s="30"/>
     </row>
     <row r="16" spans="1:23" ht="109.2" x14ac:dyDescent="0.3">
-      <c r="G16" s="82"/>
-      <c r="H16" s="83"/>
-      <c r="N16" s="78"/>
-      <c r="O16" s="78"/>
-      <c r="P16" s="78"/>
-      <c r="Q16" s="78"/>
-      <c r="R16" s="78"/>
-      <c r="S16" s="78"/>
-      <c r="T16" s="78" t="s">
+      <c r="G16" s="34"/>
+      <c r="H16" s="35"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="30"/>
+      <c r="R16" s="30"/>
+      <c r="S16" s="30"/>
+      <c r="T16" s="30" t="s">
         <v>217</v>
       </c>
-      <c r="U16" s="78" t="s">
+      <c r="U16" s="30" t="s">
         <v>365</v>
       </c>
-      <c r="V16" s="78"/>
-      <c r="W16" s="78"/>
+      <c r="V16" s="30"/>
+      <c r="W16" s="30"/>
     </row>
     <row r="17" spans="7:23" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="G17" s="82"/>
-      <c r="H17" s="82"/>
-      <c r="N17" s="78"/>
-      <c r="O17" s="78"/>
-      <c r="P17" s="78"/>
-      <c r="Q17" s="78"/>
-      <c r="R17" s="78"/>
-      <c r="S17" s="78"/>
-      <c r="T17" s="78" t="s">
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="30"/>
+      <c r="P17" s="30"/>
+      <c r="Q17" s="30"/>
+      <c r="R17" s="30"/>
+      <c r="S17" s="30"/>
+      <c r="T17" s="30" t="s">
         <v>221</v>
       </c>
-      <c r="U17" s="78" t="s">
+      <c r="U17" s="30" t="s">
         <v>222</v>
       </c>
-      <c r="V17" s="78"/>
-      <c r="W17" s="78"/>
+      <c r="V17" s="30"/>
+      <c r="W17" s="30"/>
     </row>
     <row r="18" spans="7:23" ht="124.8" x14ac:dyDescent="0.3">
-      <c r="G18" s="82"/>
-      <c r="H18" s="82"/>
-      <c r="N18" s="78"/>
-      <c r="O18" s="78"/>
-      <c r="P18" s="78"/>
-      <c r="Q18" s="78"/>
-      <c r="R18" s="78"/>
-      <c r="S18" s="78"/>
-      <c r="T18" s="78" t="s">
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="30"/>
+      <c r="P18" s="30"/>
+      <c r="Q18" s="30"/>
+      <c r="R18" s="30"/>
+      <c r="S18" s="30"/>
+      <c r="T18" s="30" t="s">
         <v>366</v>
       </c>
-      <c r="U18" s="78" t="s">
+      <c r="U18" s="30" t="s">
         <v>224</v>
       </c>
-      <c r="V18" s="78"/>
-      <c r="W18" s="78"/>
+      <c r="V18" s="30"/>
+      <c r="W18" s="30"/>
     </row>
     <row r="19" spans="7:23" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="G19" s="82"/>
-      <c r="H19" s="83"/>
-      <c r="N19" s="78"/>
-      <c r="O19" s="78"/>
-      <c r="P19" s="78"/>
-      <c r="Q19" s="78"/>
-      <c r="R19" s="78"/>
-      <c r="S19" s="78"/>
-      <c r="T19" s="78" t="s">
+      <c r="G19" s="34"/>
+      <c r="H19" s="35"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="30"/>
+      <c r="P19" s="30"/>
+      <c r="Q19" s="30"/>
+      <c r="R19" s="30"/>
+      <c r="S19" s="30"/>
+      <c r="T19" s="30" t="s">
         <v>225</v>
       </c>
-      <c r="U19" s="78" t="s">
+      <c r="U19" s="30" t="s">
         <v>367</v>
       </c>
-      <c r="V19" s="78"/>
-      <c r="W19" s="78"/>
+      <c r="V19" s="30"/>
+      <c r="W19" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6532,10 +6532,10 @@
       <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="90" t="s">
+      <c r="G2" s="42" t="s">
         <v>395</v>
       </c>
-      <c r="H2" s="91" t="s">
+      <c r="H2" s="43" t="s">
         <v>394</v>
       </c>
       <c r="I2" s="8"/>
@@ -6551,7 +6551,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="1"/>
-      <c r="H3" s="85"/>
+      <c r="H3" s="37"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
     </row>
@@ -6563,7 +6563,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="85"/>
+      <c r="H4" s="37"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
     </row>
@@ -6575,7 +6575,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="85"/>
+      <c r="H5" s="37"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
     </row>
@@ -6587,7 +6587,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="85"/>
+      <c r="H6" s="37"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
     </row>
@@ -6599,7 +6599,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="85"/>
+      <c r="H7" s="37"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
     </row>
@@ -6611,7 +6611,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="85"/>
+      <c r="H8" s="37"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
     </row>
@@ -6623,7 +6623,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="85"/>
+      <c r="H9" s="37"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
     </row>
@@ -6635,7 +6635,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="85"/>
+      <c r="H10" s="37"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
     </row>
@@ -6752,10 +6752,10 @@
       <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="85" t="s">
+      <c r="G2" s="37" t="s">
         <v>409</v>
       </c>
-      <c r="H2" s="85" t="s">
+      <c r="H2" s="37" t="s">
         <v>410</v>
       </c>
       <c r="I2" s="8"/>
@@ -6770,10 +6770,10 @@
       <c r="F3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="85" t="s">
+      <c r="G3" s="37" t="s">
         <v>416</v>
       </c>
-      <c r="H3" s="85" t="s">
+      <c r="H3" s="37" t="s">
         <v>417</v>
       </c>
       <c r="I3" s="8"/>
@@ -6788,10 +6788,10 @@
       <c r="F4" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="G4" s="85" t="s">
+      <c r="G4" s="37" t="s">
         <v>418</v>
       </c>
-      <c r="H4" s="85" t="s">
+      <c r="H4" s="37" t="s">
         <v>419</v>
       </c>
       <c r="I4" s="8"/>
@@ -6804,10 +6804,10 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="85" t="s">
+      <c r="G5" s="37" t="s">
         <v>420</v>
       </c>
-      <c r="H5" s="85" t="s">
+      <c r="H5" s="37" t="s">
         <v>421</v>
       </c>
       <c r="I5" s="8"/>
@@ -6820,10 +6820,10 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="85" t="s">
+      <c r="G6" s="37" t="s">
         <v>422</v>
       </c>
-      <c r="H6" s="85" t="s">
+      <c r="H6" s="37" t="s">
         <v>423</v>
       </c>
       <c r="I6" s="8"/>
@@ -6836,10 +6836,10 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="85" t="s">
+      <c r="G7" s="37" t="s">
         <v>424</v>
       </c>
-      <c r="H7" s="85" t="s">
+      <c r="H7" s="37" t="s">
         <v>425</v>
       </c>
       <c r="I7" s="8"/>
@@ -6852,10 +6852,10 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="85" t="s">
+      <c r="G8" s="37" t="s">
         <v>426</v>
       </c>
-      <c r="H8" s="85" t="s">
+      <c r="H8" s="37" t="s">
         <v>428</v>
       </c>
       <c r="I8" s="8"/>
@@ -6868,8 +6868,8 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="85"/>
-      <c r="H9" s="85"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
     </row>
@@ -6881,7 +6881,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="8"/>
-      <c r="H10" s="85"/>
+      <c r="H10" s="37"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
     </row>
@@ -7229,10 +7229,10 @@
       <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="85" t="s">
+      <c r="G2" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="H2" s="85" t="s">
+      <c r="H2" s="37" t="s">
         <v>69</v>
       </c>
       <c r="I2" s="8" t="s">
@@ -7251,10 +7251,10 @@
       <c r="F3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="85" t="s">
+      <c r="G3" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="H3" s="85" t="s">
+      <c r="H3" s="37" t="s">
         <v>83</v>
       </c>
       <c r="I3" s="8" t="s">
@@ -7273,26 +7273,26 @@
       <c r="F4" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="G4" s="85" t="s">
+      <c r="G4" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="85" t="s">
+      <c r="H4" s="37" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="85" t="s">
+      <c r="G5" s="37" t="s">
         <v>179</v>
       </c>
-      <c r="H5" s="85" t="s">
+      <c r="H5" s="37" t="s">
         <v>180</v>
       </c>
       <c r="I5" s="8"/>
@@ -7305,10 +7305,10 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="85" t="s">
+      <c r="G6" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="H6" s="85" t="s">
+      <c r="H6" s="37" t="s">
         <v>112</v>
       </c>
       <c r="I6" s="8"/>
@@ -7321,10 +7321,10 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="85" t="s">
+      <c r="G7" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="H7" s="85" t="s">
+      <c r="H7" s="37" t="s">
         <v>113</v>
       </c>
       <c r="I7" s="8"/>
@@ -7337,10 +7337,10 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="85" t="s">
+      <c r="G8" s="37" t="s">
         <v>374</v>
       </c>
-      <c r="H8" s="85" t="s">
+      <c r="H8" s="37" t="s">
         <v>376</v>
       </c>
       <c r="I8" s="8"/>
@@ -7410,7 +7410,7 @@
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -7426,7 +7426,7 @@
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="G14" s="2" t="s">
         <v>213</v>
       </c>
@@ -7434,7 +7434,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="G15" s="2" t="s">
         <v>354</v>
       </c>
@@ -7442,7 +7442,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="G16" s="2" t="s">
         <v>355</v>
       </c>
@@ -7450,7 +7450,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="17" spans="7:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="7:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="G17" s="2" t="s">
         <v>354</v>
       </c>
@@ -7458,7 +7458,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="18" spans="7:8" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="7:8" ht="72" x14ac:dyDescent="0.3">
       <c r="G18" s="2" t="s">
         <v>356</v>
       </c>
@@ -7466,7 +7466,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="19" spans="7:8" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="7:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="G19" s="2" t="s">
         <v>357</v>
       </c>
@@ -7490,7 +7490,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="22" spans="7:8" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="7:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="G22" s="2" t="s">
         <v>361</v>
       </c>
@@ -7514,7 +7514,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="25" spans="7:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="7:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="G25" s="2" t="s">
         <v>371</v>
       </c>
@@ -7522,7 +7522,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="26" spans="7:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="7:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="G26" s="2" t="s">
         <v>370</v>
       </c>
@@ -7647,10 +7647,10 @@
       <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="85" t="s">
+      <c r="G2" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="H2" s="85" t="s">
+      <c r="H2" s="37" t="s">
         <v>69</v>
       </c>
       <c r="I2" s="8" t="s">
@@ -7669,10 +7669,10 @@
       <c r="F3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="85" t="s">
+      <c r="G3" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="H3" s="85" t="s">
+      <c r="H3" s="37" t="s">
         <v>83</v>
       </c>
       <c r="I3" s="8" t="s">
@@ -7691,10 +7691,10 @@
       <c r="F4" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="G4" s="85" t="s">
+      <c r="G4" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="85" t="s">
+      <c r="H4" s="37" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="8" t="s">
@@ -7713,10 +7713,10 @@
       <c r="F5" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="G5" s="85" t="s">
+      <c r="G5" s="37" t="s">
         <v>179</v>
       </c>
-      <c r="H5" s="85" t="s">
+      <c r="H5" s="37" t="s">
         <v>180</v>
       </c>
       <c r="I5" s="8" t="s">
@@ -7733,10 +7733,10 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="85" t="s">
+      <c r="G6" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="H6" s="85" t="s">
+      <c r="H6" s="37" t="s">
         <v>112</v>
       </c>
       <c r="I6" s="8" t="s">
@@ -7753,10 +7753,10 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="85" t="s">
+      <c r="G7" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="H7" s="85" t="s">
+      <c r="H7" s="37" t="s">
         <v>113</v>
       </c>
       <c r="I7" s="8"/>
@@ -7769,10 +7769,10 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="85" t="s">
+      <c r="G8" s="37" t="s">
         <v>374</v>
       </c>
-      <c r="H8" s="85" t="s">
+      <c r="H8" s="37" t="s">
         <v>376</v>
       </c>
       <c r="I8" s="8"/>
@@ -8083,8 +8083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF3FB38F-39BD-477F-A58E-198477386216}">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F9" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8152,10 +8152,10 @@
       <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="85" t="s">
+      <c r="G2" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="H2" s="85" t="s">
+      <c r="H2" s="37" t="s">
         <v>69</v>
       </c>
       <c r="I2" s="8" t="s">
@@ -8174,10 +8174,10 @@
       <c r="F3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="85" t="s">
+      <c r="G3" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="H3" s="85" t="s">
+      <c r="H3" s="37" t="s">
         <v>83</v>
       </c>
       <c r="I3" s="8" t="s">
@@ -8196,10 +8196,10 @@
       <c r="F4" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="G4" s="85" t="s">
+      <c r="G4" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="85" t="s">
+      <c r="H4" s="37" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="8" t="s">
@@ -8218,10 +8218,10 @@
       <c r="F5" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="G5" s="85" t="s">
+      <c r="G5" s="37" t="s">
         <v>179</v>
       </c>
-      <c r="H5" s="85" t="s">
+      <c r="H5" s="37" t="s">
         <v>180</v>
       </c>
       <c r="I5" s="8" t="s">
@@ -8238,10 +8238,10 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="85" t="s">
+      <c r="G6" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="H6" s="85" t="s">
+      <c r="H6" s="37" t="s">
         <v>112</v>
       </c>
       <c r="I6" s="8" t="s">
@@ -8258,10 +8258,10 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="85" t="s">
+      <c r="G7" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="H7" s="85" t="s">
+      <c r="H7" s="37" t="s">
         <v>113</v>
       </c>
       <c r="I7" s="8"/>
@@ -8274,10 +8274,10 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="85" t="s">
+      <c r="G8" s="37" t="s">
         <v>456</v>
       </c>
-      <c r="H8" s="85" t="s">
+      <c r="H8" s="37" t="s">
         <v>457</v>
       </c>
       <c r="I8" s="8"/>
@@ -8338,10 +8338,10 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="86" t="s">
+      <c r="G12" s="38" t="s">
         <v>460</v>
       </c>
-      <c r="H12" s="86" t="s">
+      <c r="H12" s="38" t="s">
         <v>394</v>
       </c>
       <c r="I12" s="8"/>
@@ -8690,10 +8690,10 @@
       <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="85" t="s">
+      <c r="G2" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="H2" s="85" t="s">
+      <c r="H2" s="37" t="s">
         <v>69</v>
       </c>
       <c r="I2" s="8" t="s">
@@ -8712,10 +8712,10 @@
       <c r="F3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="85" t="s">
+      <c r="G3" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="H3" s="85" t="s">
+      <c r="H3" s="37" t="s">
         <v>83</v>
       </c>
       <c r="I3" s="8" t="s">
@@ -8734,10 +8734,10 @@
       <c r="F4" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="G4" s="85" t="s">
+      <c r="G4" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="85" t="s">
+      <c r="H4" s="37" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="8" t="s">
@@ -8754,10 +8754,10 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="85" t="s">
+      <c r="G5" s="37" t="s">
         <v>179</v>
       </c>
-      <c r="H5" s="85" t="s">
+      <c r="H5" s="37" t="s">
         <v>180</v>
       </c>
       <c r="I5" s="8"/>
@@ -8770,10 +8770,10 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="85" t="s">
+      <c r="G6" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="H6" s="85" t="s">
+      <c r="H6" s="37" t="s">
         <v>112</v>
       </c>
       <c r="I6" s="8"/>
@@ -8786,10 +8786,10 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="85" t="s">
+      <c r="G7" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="H7" s="85" t="s">
+      <c r="H7" s="37" t="s">
         <v>113</v>
       </c>
       <c r="I7" s="8"/>
@@ -8802,10 +8802,10 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="85" t="s">
+      <c r="G8" s="37" t="s">
         <v>374</v>
       </c>
-      <c r="H8" s="85" t="s">
+      <c r="H8" s="37" t="s">
         <v>376</v>
       </c>
       <c r="I8" s="8"/>
@@ -9044,10 +9044,10 @@
       </c>
     </row>
     <row r="32" spans="7:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="G32" s="87" t="s">
+      <c r="G32" s="39" t="s">
         <v>387</v>
       </c>
-      <c r="H32" s="87" t="s">
+      <c r="H32" s="39" t="s">
         <v>399</v>
       </c>
     </row>
@@ -9137,10 +9137,10 @@
       <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="85" t="s">
+      <c r="G2" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="H2" s="85" t="s">
+      <c r="H2" s="37" t="s">
         <v>69</v>
       </c>
       <c r="I2" s="8" t="s">
@@ -9159,10 +9159,10 @@
       <c r="F3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="85" t="s">
+      <c r="G3" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="H3" s="85" t="s">
+      <c r="H3" s="37" t="s">
         <v>83</v>
       </c>
       <c r="I3" s="8" t="s">
@@ -9181,10 +9181,10 @@
       <c r="F4" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="G4" s="85" t="s">
+      <c r="G4" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="85" t="s">
+      <c r="H4" s="37" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="8"/>
@@ -9197,10 +9197,10 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="85" t="s">
+      <c r="G5" s="37" t="s">
         <v>179</v>
       </c>
-      <c r="H5" s="85" t="s">
+      <c r="H5" s="37" t="s">
         <v>180</v>
       </c>
       <c r="I5" s="8"/>
@@ -9213,10 +9213,10 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="85" t="s">
+      <c r="G6" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="H6" s="85" t="s">
+      <c r="H6" s="37" t="s">
         <v>112</v>
       </c>
       <c r="I6" s="8"/>
@@ -9229,10 +9229,10 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="85" t="s">
+      <c r="G7" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="H7" s="85" t="s">
+      <c r="H7" s="37" t="s">
         <v>113</v>
       </c>
       <c r="I7" s="8"/>
@@ -9245,10 +9245,10 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="85" t="s">
+      <c r="G8" s="37" t="s">
         <v>374</v>
       </c>
-      <c r="H8" s="85" t="s">
+      <c r="H8" s="37" t="s">
         <v>376</v>
       </c>
       <c r="I8" s="8"/>
@@ -10113,10 +10113,10 @@
       <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="85" t="s">
+      <c r="G2" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="H2" s="85" t="s">
+      <c r="H2" s="37" t="s">
         <v>69</v>
       </c>
       <c r="I2" s="8" t="s">
@@ -10135,10 +10135,10 @@
       <c r="F3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="85" t="s">
+      <c r="G3" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="H3" s="85" t="s">
+      <c r="H3" s="37" t="s">
         <v>83</v>
       </c>
       <c r="I3" s="8" t="s">
@@ -10157,10 +10157,10 @@
       <c r="F4" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="G4" s="85" t="s">
+      <c r="G4" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="85" t="s">
+      <c r="H4" s="37" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="8" t="s">
@@ -10177,10 +10177,10 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="85" t="s">
+      <c r="G5" s="37" t="s">
         <v>179</v>
       </c>
-      <c r="H5" s="85" t="s">
+      <c r="H5" s="37" t="s">
         <v>180</v>
       </c>
       <c r="I5" s="8"/>
@@ -10193,10 +10193,10 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="85" t="s">
+      <c r="G6" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="H6" s="85" t="s">
+      <c r="H6" s="37" t="s">
         <v>112</v>
       </c>
       <c r="I6" s="8"/>
@@ -10209,10 +10209,10 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="85" t="s">
+      <c r="G7" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="H7" s="85" t="s">
+      <c r="H7" s="37" t="s">
         <v>113</v>
       </c>
       <c r="I7" s="8"/>
@@ -10225,10 +10225,10 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="85" t="s">
+      <c r="G8" s="37" t="s">
         <v>374</v>
       </c>
-      <c r="H8" s="85" t="s">
+      <c r="H8" s="37" t="s">
         <v>376</v>
       </c>
       <c r="I8" s="8"/>
@@ -10454,243 +10454,243 @@
       </c>
     </row>
     <row r="31" spans="6:10" ht="331.2" x14ac:dyDescent="0.3">
-      <c r="F31" s="72"/>
+      <c r="F31" s="24"/>
       <c r="G31" s="2" t="s">
         <v>396</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="I31" s="72"/>
-      <c r="J31" s="72"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
     </row>
     <row r="32" spans="6:10" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="F32" s="72"/>
-      <c r="G32" s="88" t="s">
+      <c r="F32" s="24"/>
+      <c r="G32" s="40" t="s">
         <v>393</v>
       </c>
-      <c r="H32" s="89" t="s">
+      <c r="H32" s="41" t="s">
         <v>394</v>
       </c>
-      <c r="I32" s="72"/>
-      <c r="J32" s="72"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
     </row>
     <row r="33" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F33" s="72"/>
-      <c r="G33" s="72"/>
-      <c r="H33" s="72"/>
-      <c r="I33" s="72"/>
-      <c r="J33" s="72"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="24"/>
     </row>
     <row r="34" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F34" s="72"/>
-      <c r="G34" s="72"/>
-      <c r="H34" s="72"/>
-      <c r="I34" s="72"/>
-      <c r="J34" s="72"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
     </row>
     <row r="35" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F35" s="72"/>
-      <c r="G35" s="72"/>
-      <c r="H35" s="72"/>
-      <c r="I35" s="72"/>
-      <c r="J35" s="72"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24"/>
     </row>
     <row r="36" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F36" s="72"/>
-      <c r="G36" s="72"/>
-      <c r="H36" s="72"/>
-      <c r="I36" s="72"/>
-      <c r="J36" s="72"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24"/>
     </row>
     <row r="37" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F37" s="72"/>
-      <c r="G37" s="72"/>
-      <c r="H37" s="72"/>
-      <c r="I37" s="72"/>
-      <c r="J37" s="72"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="24"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24"/>
     </row>
     <row r="38" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F38" s="72"/>
-      <c r="G38" s="72"/>
-      <c r="H38" s="72"/>
-      <c r="I38" s="72"/>
-      <c r="J38" s="72"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="24"/>
+      <c r="J38" s="24"/>
     </row>
     <row r="39" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F39" s="72"/>
-      <c r="G39" s="72"/>
-      <c r="H39" s="72"/>
-      <c r="I39" s="72"/>
-      <c r="J39" s="72"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="24"/>
+      <c r="J39" s="24"/>
     </row>
     <row r="40" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F40" s="72"/>
-      <c r="G40" s="72"/>
-      <c r="H40" s="72"/>
-      <c r="I40" s="72"/>
-      <c r="J40" s="72"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="24"/>
+      <c r="I40" s="24"/>
+      <c r="J40" s="24"/>
     </row>
     <row r="41" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F41" s="72"/>
-      <c r="G41" s="72"/>
-      <c r="H41" s="72"/>
-      <c r="I41" s="72"/>
-      <c r="J41" s="72"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="24"/>
+      <c r="J41" s="24"/>
     </row>
     <row r="42" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F42" s="72"/>
-      <c r="G42" s="72"/>
-      <c r="H42" s="72"/>
-      <c r="I42" s="72"/>
-      <c r="J42" s="72"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="24"/>
+      <c r="J42" s="24"/>
     </row>
     <row r="43" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F43" s="72"/>
-      <c r="G43" s="72"/>
-      <c r="H43" s="72"/>
-      <c r="I43" s="72"/>
-      <c r="J43" s="72"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="24"/>
+      <c r="H43" s="24"/>
+      <c r="I43" s="24"/>
+      <c r="J43" s="24"/>
     </row>
     <row r="44" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F44" s="72"/>
-      <c r="G44" s="72"/>
-      <c r="H44" s="72"/>
-      <c r="I44" s="72"/>
-      <c r="J44" s="72"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="24"/>
+      <c r="I44" s="24"/>
+      <c r="J44" s="24"/>
     </row>
     <row r="45" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F45" s="72"/>
-      <c r="G45" s="72"/>
-      <c r="H45" s="72"/>
-      <c r="I45" s="72"/>
-      <c r="J45" s="72"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="24"/>
+      <c r="H45" s="24"/>
+      <c r="I45" s="24"/>
+      <c r="J45" s="24"/>
     </row>
     <row r="46" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F46" s="72"/>
-      <c r="G46" s="72"/>
-      <c r="H46" s="72"/>
-      <c r="I46" s="72"/>
-      <c r="J46" s="72"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="24"/>
+      <c r="H46" s="24"/>
+      <c r="I46" s="24"/>
+      <c r="J46" s="24"/>
     </row>
     <row r="47" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F47" s="72"/>
-      <c r="G47" s="72"/>
-      <c r="H47" s="72"/>
-      <c r="I47" s="72"/>
-      <c r="J47" s="72"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="24"/>
+      <c r="H47" s="24"/>
+      <c r="I47" s="24"/>
+      <c r="J47" s="24"/>
     </row>
     <row r="48" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F48" s="72"/>
-      <c r="G48" s="72"/>
-      <c r="H48" s="72"/>
-      <c r="I48" s="72"/>
-      <c r="J48" s="72"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="24"/>
+      <c r="I48" s="24"/>
+      <c r="J48" s="24"/>
     </row>
     <row r="49" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F49" s="72"/>
-      <c r="G49" s="72"/>
-      <c r="H49" s="72"/>
-      <c r="I49" s="72"/>
-      <c r="J49" s="72"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="24"/>
+      <c r="H49" s="24"/>
+      <c r="I49" s="24"/>
+      <c r="J49" s="24"/>
     </row>
     <row r="50" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F50" s="72"/>
-      <c r="G50" s="72"/>
-      <c r="H50" s="72"/>
-      <c r="I50" s="72"/>
-      <c r="J50" s="72"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="24"/>
+      <c r="H50" s="24"/>
+      <c r="I50" s="24"/>
+      <c r="J50" s="24"/>
     </row>
     <row r="51" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F51" s="72"/>
-      <c r="G51" s="72"/>
-      <c r="H51" s="72"/>
-      <c r="I51" s="72"/>
-      <c r="J51" s="72"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="24"/>
+      <c r="H51" s="24"/>
+      <c r="I51" s="24"/>
+      <c r="J51" s="24"/>
     </row>
     <row r="52" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F52" s="72"/>
-      <c r="G52" s="72"/>
-      <c r="H52" s="72"/>
-      <c r="I52" s="72"/>
-      <c r="J52" s="72"/>
+      <c r="F52" s="24"/>
+      <c r="G52" s="24"/>
+      <c r="H52" s="24"/>
+      <c r="I52" s="24"/>
+      <c r="J52" s="24"/>
     </row>
     <row r="53" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F53" s="72"/>
-      <c r="G53" s="72"/>
-      <c r="H53" s="72"/>
-      <c r="I53" s="72"/>
-      <c r="J53" s="72"/>
+      <c r="F53" s="24"/>
+      <c r="G53" s="24"/>
+      <c r="H53" s="24"/>
+      <c r="I53" s="24"/>
+      <c r="J53" s="24"/>
     </row>
     <row r="54" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F54" s="72"/>
-      <c r="G54" s="72"/>
-      <c r="H54" s="72"/>
-      <c r="I54" s="72"/>
-      <c r="J54" s="72"/>
+      <c r="F54" s="24"/>
+      <c r="G54" s="24"/>
+      <c r="H54" s="24"/>
+      <c r="I54" s="24"/>
+      <c r="J54" s="24"/>
     </row>
     <row r="55" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F55" s="72"/>
-      <c r="G55" s="72"/>
-      <c r="H55" s="72"/>
-      <c r="I55" s="72"/>
-      <c r="J55" s="72"/>
+      <c r="F55" s="24"/>
+      <c r="G55" s="24"/>
+      <c r="H55" s="24"/>
+      <c r="I55" s="24"/>
+      <c r="J55" s="24"/>
     </row>
     <row r="56" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F56" s="72"/>
-      <c r="G56" s="72"/>
-      <c r="H56" s="72"/>
-      <c r="I56" s="72"/>
-      <c r="J56" s="72"/>
+      <c r="F56" s="24"/>
+      <c r="G56" s="24"/>
+      <c r="H56" s="24"/>
+      <c r="I56" s="24"/>
+      <c r="J56" s="24"/>
     </row>
     <row r="57" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F57" s="72"/>
-      <c r="G57" s="72"/>
-      <c r="H57" s="72"/>
-      <c r="I57" s="72"/>
-      <c r="J57" s="72"/>
+      <c r="F57" s="24"/>
+      <c r="G57" s="24"/>
+      <c r="H57" s="24"/>
+      <c r="I57" s="24"/>
+      <c r="J57" s="24"/>
     </row>
     <row r="58" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F58" s="72"/>
-      <c r="G58" s="72"/>
-      <c r="H58" s="72"/>
-      <c r="I58" s="72"/>
-      <c r="J58" s="72"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="24"/>
+      <c r="H58" s="24"/>
+      <c r="I58" s="24"/>
+      <c r="J58" s="24"/>
     </row>
     <row r="59" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F59" s="72"/>
-      <c r="G59" s="72"/>
-      <c r="H59" s="72"/>
-      <c r="I59" s="72"/>
-      <c r="J59" s="72"/>
+      <c r="F59" s="24"/>
+      <c r="G59" s="24"/>
+      <c r="H59" s="24"/>
+      <c r="I59" s="24"/>
+      <c r="J59" s="24"/>
     </row>
     <row r="60" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F60" s="72"/>
-      <c r="G60" s="72"/>
-      <c r="H60" s="72"/>
-      <c r="I60" s="72"/>
-      <c r="J60" s="72"/>
+      <c r="F60" s="24"/>
+      <c r="G60" s="24"/>
+      <c r="H60" s="24"/>
+      <c r="I60" s="24"/>
+      <c r="J60" s="24"/>
     </row>
     <row r="61" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F61" s="72"/>
-      <c r="G61" s="72"/>
-      <c r="H61" s="72"/>
-      <c r="I61" s="72"/>
-      <c r="J61" s="72"/>
+      <c r="F61" s="24"/>
+      <c r="G61" s="24"/>
+      <c r="H61" s="24"/>
+      <c r="I61" s="24"/>
+      <c r="J61" s="24"/>
     </row>
     <row r="62" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F62" s="72"/>
-      <c r="G62" s="72"/>
-      <c r="H62" s="72"/>
-      <c r="I62" s="72"/>
-      <c r="J62" s="72"/>
+      <c r="F62" s="24"/>
+      <c r="G62" s="24"/>
+      <c r="H62" s="24"/>
+      <c r="I62" s="24"/>
+      <c r="J62" s="24"/>
     </row>
     <row r="63" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F63" s="72"/>
-      <c r="G63" s="72"/>
-      <c r="H63" s="72"/>
-      <c r="I63" s="72"/>
-      <c r="J63" s="72"/>
+      <c r="F63" s="24"/>
+      <c r="G63" s="24"/>
+      <c r="H63" s="24"/>
+      <c r="I63" s="24"/>
+      <c r="J63" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10769,10 +10769,10 @@
       <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="85" t="s">
+      <c r="G2" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="H2" s="85" t="s">
+      <c r="H2" s="37" t="s">
         <v>69</v>
       </c>
       <c r="I2" s="8" t="s">
@@ -10791,10 +10791,10 @@
       <c r="F3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="85" t="s">
+      <c r="G3" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="H3" s="85" t="s">
+      <c r="H3" s="37" t="s">
         <v>83</v>
       </c>
       <c r="I3" s="8" t="s">
@@ -10813,10 +10813,10 @@
       <c r="F4" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="G4" s="85" t="s">
+      <c r="G4" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="85" t="s">
+      <c r="H4" s="37" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="8" t="s">
@@ -10833,10 +10833,10 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="85" t="s">
+      <c r="G5" s="37" t="s">
         <v>179</v>
       </c>
-      <c r="H5" s="85" t="s">
+      <c r="H5" s="37" t="s">
         <v>180</v>
       </c>
       <c r="I5" s="8"/>
@@ -10849,10 +10849,10 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="85" t="s">
+      <c r="G6" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="H6" s="85" t="s">
+      <c r="H6" s="37" t="s">
         <v>112</v>
       </c>
       <c r="I6" s="8"/>
@@ -10865,10 +10865,10 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="85" t="s">
+      <c r="G7" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="H7" s="85" t="s">
+      <c r="H7" s="37" t="s">
         <v>113</v>
       </c>
       <c r="I7" s="8"/>
@@ -10881,10 +10881,10 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="85" t="s">
+      <c r="G8" s="37" t="s">
         <v>374</v>
       </c>
-      <c r="H8" s="85" t="s">
+      <c r="H8" s="37" t="s">
         <v>376</v>
       </c>
       <c r="I8" s="8"/>
@@ -11118,10 +11118,10 @@
       </c>
     </row>
     <row r="32" spans="7:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="G32" s="88" t="s">
+      <c r="G32" s="40" t="s">
         <v>393</v>
       </c>
-      <c r="H32" s="89" t="s">
+      <c r="H32" s="41" t="s">
         <v>394</v>
       </c>
     </row>
@@ -11461,10 +11461,10 @@
       <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="85" t="s">
+      <c r="G2" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="H2" s="85" t="s">
+      <c r="H2" s="37" t="s">
         <v>69</v>
       </c>
       <c r="I2" s="8" t="s">
@@ -11483,10 +11483,10 @@
       <c r="F3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="85" t="s">
+      <c r="G3" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="H3" s="85" t="s">
+      <c r="H3" s="37" t="s">
         <v>83</v>
       </c>
       <c r="I3" s="8"/>
@@ -11501,10 +11501,10 @@
       <c r="F4" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="G4" s="85" t="s">
+      <c r="G4" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="85" t="s">
+      <c r="H4" s="37" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="8"/>
@@ -11517,10 +11517,10 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="85" t="s">
+      <c r="G5" s="37" t="s">
         <v>179</v>
       </c>
-      <c r="H5" s="85" t="s">
+      <c r="H5" s="37" t="s">
         <v>180</v>
       </c>
       <c r="I5" s="8"/>
@@ -11533,10 +11533,10 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="85" t="s">
+      <c r="G6" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="H6" s="85" t="s">
+      <c r="H6" s="37" t="s">
         <v>112</v>
       </c>
       <c r="I6" s="8"/>
@@ -11549,10 +11549,10 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="85" t="s">
+      <c r="G7" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="H7" s="85" t="s">
+      <c r="H7" s="37" t="s">
         <v>113</v>
       </c>
       <c r="I7" s="8"/>
@@ -11565,10 +11565,10 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="85" t="s">
+      <c r="G8" s="37" t="s">
         <v>374</v>
       </c>
-      <c r="H8" s="85" t="s">
+      <c r="H8" s="37" t="s">
         <v>376</v>
       </c>
       <c r="I8" s="8"/>
@@ -11875,10 +11875,10 @@
       <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="85" t="s">
+      <c r="G2" s="37" t="s">
         <v>409</v>
       </c>
-      <c r="H2" s="85" t="s">
+      <c r="H2" s="37" t="s">
         <v>410</v>
       </c>
       <c r="I2" s="8" t="s">
@@ -11900,7 +11900,7 @@
       <c r="G3" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="H3" s="85" t="s">
+      <c r="H3" s="37" t="s">
         <v>412</v>
       </c>
       <c r="I3" s="8"/>
@@ -11916,7 +11916,7 @@
       <c r="G4" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="H4" s="85" t="s">
+      <c r="H4" s="37" t="s">
         <v>414</v>
       </c>
       <c r="I4" s="8"/>
@@ -11930,7 +11930,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="85"/>
+      <c r="H5" s="37"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
     </row>
@@ -11942,7 +11942,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="85"/>
+      <c r="H6" s="37"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
     </row>
@@ -11954,7 +11954,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="85"/>
+      <c r="H7" s="37"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
     </row>
@@ -11966,7 +11966,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="85"/>
+      <c r="H8" s="37"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
     </row>
@@ -11978,7 +11978,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="85"/>
+      <c r="H9" s="37"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
     </row>
@@ -11990,7 +11990,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="85"/>
+      <c r="H10" s="37"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
     </row>

</xml_diff>

<commit_message>
Made changes towards Philippes comments.
</commit_message>
<xml_diff>
--- a/documentation/VD/source/procedures.xlsx
+++ b/documentation/VD/source/procedures.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74535761-68E5-4E07-803D-5F6136F62F83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D786534-CC1C-46B4-8DFA-6F61DB99F45C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14760" yWindow="4908" windowWidth="17280" windowHeight="11508" tabRatio="1000" firstSheet="20" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="852" windowWidth="17280" windowHeight="11508" tabRatio="1000" firstSheet="20" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="2" r:id="rId1"/>
@@ -1432,24 +1432,15 @@
     <t>**IntelliWave API** project is opened.</t>
   </si>
   <si>
-    <t>Click on **Wizards** on the target applicatio. Scroll down and click on **Radius of Curvature**.</t>
-  </si>
-  <si>
     <t>**Radius of Curvature** dialog is open.</t>
   </si>
   <si>
     <t>Click on the **Windows Search Bar**.Type **cmd** and press enter. Then, Click on the **Command Prompt** and type **python facile.py** in the **Command Prompt**</t>
   </si>
   <si>
-    <t>Click on **Add Behavior**. Then, click on 2 highlighted components that are shown in the view.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Visibility behavior is added. </t>
   </si>
   <si>
-    <t>Click on the arrow graphic and select **Select trigger action**.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Visibility behaviors  action is selected. </t>
   </si>
   <si>
@@ -1465,15 +1456,9 @@
     <t>Click on **Edit ports for:** and type as **measureRadiusOfCurvature**.</t>
   </si>
   <si>
-    <t>Click on **default** under **Input Ports** and type **diameter*. Click on **NoneType** under **Input Ports** and type the data structure to be float. Repeat this for an input named **tsf** with a float data type.</t>
-  </si>
-  <si>
     <t xml:space="preserve">All inputs are added. </t>
   </si>
   <si>
-    <t>Click on **default** under **Output Ports** and type **radiusOfCurvature*. Click on **NoneType** under **Output Ports** and type the data structure to be float.</t>
-  </si>
-  <si>
     <t>All outputs are added.</t>
   </si>
   <si>
@@ -1499,6 +1484,21 @@
   </si>
   <si>
     <t>Verify it returns a value that equals some predetermined value that we know is correct. Test case is complete.</t>
+  </si>
+  <si>
+    <t>Click on **Wizards** on the target application. Scroll down and click on **Radius of Curvature**.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on **Add Behavior**. Then, click on **wizard** component and then click on **Radius of Curvature** dialog in the target GUI view. </t>
+  </si>
+  <si>
+    <t>Click on the arrow graphic and click on  **Select trigger action**. Right after, click on **click** to be the trigger action.</t>
+  </si>
+  <si>
+    <t>Click on the add input port icon and scroll over  **default** under **Input Ports** and type **diameter*. Click on **NoneType** under **Input Ports** and type the data structure to be float. Repeat this for an input named **tsf** with a float data type.</t>
+  </si>
+  <si>
+    <t>Click on the add output port icon and scroll over **default** under **Output Ports** and type **radiusOfCurvature*. Click on **NoneType** under **Output Ports** and type the data structure to be float.</t>
   </si>
 </sst>
 </file>
@@ -1995,98 +1995,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2115,6 +2037,15 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2124,20 +2055,89 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2433,846 +2433,828 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="48" t="s">
         <v>305</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="76"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="50"/>
     </row>
     <row r="2" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="79"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="53"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="77"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="79"/>
+      <c r="A3" s="51"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="53"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="77"/>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="79"/>
+      <c r="A4" s="51"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="53"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="77"/>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="79"/>
+      <c r="A5" s="51"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="53"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="77"/>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="79"/>
+      <c r="A6" s="51"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="53"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="77"/>
-      <c r="B7" s="78"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78"/>
-      <c r="H7" s="78"/>
-      <c r="I7" s="79"/>
+      <c r="A7" s="51"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="53"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="77"/>
-      <c r="B8" s="78"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="78"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="79"/>
+      <c r="A8" s="51"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="53"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="77"/>
-      <c r="B9" s="78"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="79"/>
+      <c r="A9" s="51"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="53"/>
     </row>
     <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="80" t="s">
+      <c r="A10" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="81"/>
-      <c r="C10" s="81"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="81"/>
-      <c r="F10" s="81"/>
-      <c r="G10" s="81"/>
-      <c r="H10" s="81"/>
-      <c r="I10" s="82"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="56"/>
     </row>
     <row r="11" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="51"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="58"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="59"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="49"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="51"/>
+      <c r="A12" s="57"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="58"/>
+      <c r="H12" s="58"/>
+      <c r="I12" s="59"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="49"/>
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="51"/>
+      <c r="A13" s="57"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="59"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="49"/>
-      <c r="B14" s="50"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="51"/>
+      <c r="A14" s="57"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="59"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="49"/>
-      <c r="B15" s="50"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="51"/>
+      <c r="A15" s="57"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="58"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="58"/>
+      <c r="G15" s="58"/>
+      <c r="H15" s="58"/>
+      <c r="I15" s="59"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="49"/>
-      <c r="B16" s="50"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="51"/>
+      <c r="A16" s="57"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="59"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="49"/>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="51"/>
+      <c r="A17" s="57"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="59"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="49"/>
-      <c r="B18" s="50"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="50"/>
-      <c r="I18" s="51"/>
+      <c r="A18" s="57"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="58"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="58"/>
+      <c r="G18" s="58"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="59"/>
     </row>
     <row r="19" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="88">
+      <c r="A19" s="45">
         <v>1</v>
       </c>
-      <c r="B19" s="83" t="s">
+      <c r="B19" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="84"/>
-      <c r="D19" s="84"/>
-      <c r="E19" s="84"/>
-      <c r="F19" s="84"/>
-      <c r="G19" s="84"/>
-      <c r="H19" s="84"/>
-      <c r="I19" s="85"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="62"/>
     </row>
     <row r="20" spans="1:9" ht="20.7" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="89"/>
+      <c r="A20" s="46"/>
       <c r="B20" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="86" t="s">
+      <c r="C20" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="87"/>
-      <c r="E20" s="47" t="s">
+      <c r="D20" s="44"/>
+      <c r="E20" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="47"/>
-      <c r="G20" s="47"/>
-      <c r="H20" s="47"/>
-      <c r="I20" s="48"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="64"/>
     </row>
     <row r="21" spans="1:9" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="89"/>
+      <c r="A21" s="46"/>
       <c r="B21" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="86" t="s">
+      <c r="C21" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="87"/>
-      <c r="E21" s="47" t="s">
+      <c r="D21" s="44"/>
+      <c r="E21" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="48"/>
+      <c r="F21" s="63"/>
+      <c r="G21" s="63"/>
+      <c r="H21" s="63"/>
+      <c r="I21" s="64"/>
     </row>
     <row r="22" spans="1:9" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="89"/>
+      <c r="A22" s="46"/>
       <c r="B22" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="86" t="s">
+      <c r="C22" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="87"/>
-      <c r="E22" s="47" t="s">
+      <c r="D22" s="44"/>
+      <c r="E22" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="F22" s="47"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="47"/>
-      <c r="I22" s="48"/>
+      <c r="F22" s="63"/>
+      <c r="G22" s="63"/>
+      <c r="H22" s="63"/>
+      <c r="I22" s="64"/>
     </row>
     <row r="23" spans="1:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="89"/>
+      <c r="A23" s="46"/>
       <c r="B23" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="86" t="s">
+      <c r="C23" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="87"/>
-      <c r="E23" s="47" t="s">
+      <c r="D23" s="44"/>
+      <c r="E23" s="63" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="47"/>
-      <c r="I23" s="48"/>
+      <c r="F23" s="63"/>
+      <c r="G23" s="63"/>
+      <c r="H23" s="63"/>
+      <c r="I23" s="64"/>
     </row>
     <row r="24" spans="1:9" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="89"/>
+      <c r="A24" s="46"/>
       <c r="B24" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="86" t="s">
+      <c r="C24" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="87"/>
-      <c r="E24" s="47" t="s">
+      <c r="D24" s="44"/>
+      <c r="E24" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="F24" s="47"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="47"/>
-      <c r="I24" s="48"/>
+      <c r="F24" s="63"/>
+      <c r="G24" s="63"/>
+      <c r="H24" s="63"/>
+      <c r="I24" s="64"/>
     </row>
     <row r="25" spans="1:9" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="89"/>
+      <c r="A25" s="46"/>
       <c r="B25" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="86" t="s">
+      <c r="C25" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="87"/>
-      <c r="E25" s="47" t="s">
+      <c r="D25" s="44"/>
+      <c r="E25" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="F25" s="47"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="47"/>
-      <c r="I25" s="48"/>
+      <c r="F25" s="63"/>
+      <c r="G25" s="63"/>
+      <c r="H25" s="63"/>
+      <c r="I25" s="64"/>
     </row>
     <row r="26" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="89"/>
+      <c r="A26" s="46"/>
       <c r="B26" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C26" s="86" t="s">
+      <c r="C26" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="87"/>
-      <c r="E26" s="47" t="s">
+      <c r="D26" s="44"/>
+      <c r="E26" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="F26" s="47"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="47"/>
-      <c r="I26" s="48"/>
+      <c r="F26" s="63"/>
+      <c r="G26" s="63"/>
+      <c r="H26" s="63"/>
+      <c r="I26" s="64"/>
     </row>
     <row r="27" spans="1:9" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="89"/>
+      <c r="A27" s="46"/>
       <c r="B27" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="86" t="s">
+      <c r="C27" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="87"/>
-      <c r="E27" s="47" t="s">
+      <c r="D27" s="44"/>
+      <c r="E27" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="F27" s="47"/>
-      <c r="G27" s="47"/>
-      <c r="H27" s="47"/>
-      <c r="I27" s="48"/>
+      <c r="F27" s="63"/>
+      <c r="G27" s="63"/>
+      <c r="H27" s="63"/>
+      <c r="I27" s="64"/>
     </row>
     <row r="28" spans="1:9" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="89"/>
+      <c r="A28" s="46"/>
       <c r="B28" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="86" t="s">
+      <c r="C28" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="87"/>
-      <c r="E28" s="47" t="s">
+      <c r="D28" s="44"/>
+      <c r="E28" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="F28" s="70"/>
-      <c r="G28" s="70"/>
-      <c r="H28" s="70"/>
-      <c r="I28" s="71"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="65"/>
+      <c r="I28" s="66"/>
     </row>
     <row r="29" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="90"/>
+      <c r="A29" s="47"/>
       <c r="B29" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="86" t="s">
+      <c r="C29" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="87"/>
-      <c r="E29" s="62" t="s">
+      <c r="D29" s="44"/>
+      <c r="E29" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="F29" s="72"/>
-      <c r="G29" s="72"/>
-      <c r="H29" s="72"/>
-      <c r="I29" s="73"/>
+      <c r="F29" s="68"/>
+      <c r="G29" s="68"/>
+      <c r="H29" s="68"/>
+      <c r="I29" s="69"/>
     </row>
     <row r="30" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="55">
+      <c r="A30" s="70">
         <v>2</v>
       </c>
-      <c r="B30" s="44" t="s">
+      <c r="B30" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="45"/>
+      <c r="C30" s="74"/>
+      <c r="D30" s="74"/>
+      <c r="E30" s="74"/>
+      <c r="F30" s="74"/>
+      <c r="G30" s="74"/>
+      <c r="H30" s="74"/>
+      <c r="I30" s="75"/>
     </row>
     <row r="31" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="56"/>
+      <c r="A31" s="71"/>
       <c r="B31" s="9"/>
-      <c r="C31" s="46" t="s">
+      <c r="C31" s="76" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="48"/>
+      <c r="D31" s="63"/>
+      <c r="E31" s="63"/>
+      <c r="F31" s="63"/>
+      <c r="G31" s="63"/>
+      <c r="H31" s="63"/>
+      <c r="I31" s="64"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="56"/>
+      <c r="A32" s="71"/>
       <c r="B32" s="9"/>
-      <c r="C32" s="49"/>
-      <c r="D32" s="50"/>
-      <c r="E32" s="50"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="50"/>
-      <c r="H32" s="50"/>
-      <c r="I32" s="51"/>
+      <c r="C32" s="57"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="58"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="58"/>
+      <c r="H32" s="58"/>
+      <c r="I32" s="59"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="56"/>
+      <c r="A33" s="71"/>
       <c r="B33" s="9"/>
-      <c r="C33" s="49"/>
-      <c r="D33" s="50"/>
-      <c r="E33" s="50"/>
-      <c r="F33" s="50"/>
-      <c r="G33" s="50"/>
-      <c r="H33" s="50"/>
-      <c r="I33" s="51"/>
+      <c r="C33" s="57"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="58"/>
+      <c r="F33" s="58"/>
+      <c r="G33" s="58"/>
+      <c r="H33" s="58"/>
+      <c r="I33" s="59"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="56"/>
+      <c r="A34" s="71"/>
       <c r="B34" s="9"/>
-      <c r="C34" s="49"/>
-      <c r="D34" s="50"/>
-      <c r="E34" s="50"/>
-      <c r="F34" s="50"/>
-      <c r="G34" s="50"/>
-      <c r="H34" s="50"/>
-      <c r="I34" s="51"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="58"/>
+      <c r="E34" s="58"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="58"/>
+      <c r="I34" s="59"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="56"/>
+      <c r="A35" s="71"/>
       <c r="B35" s="9"/>
-      <c r="C35" s="49"/>
-      <c r="D35" s="50"/>
-      <c r="E35" s="50"/>
-      <c r="F35" s="50"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="50"/>
-      <c r="I35" s="51"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="58"/>
+      <c r="E35" s="58"/>
+      <c r="F35" s="58"/>
+      <c r="G35" s="58"/>
+      <c r="H35" s="58"/>
+      <c r="I35" s="59"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="56"/>
+      <c r="A36" s="71"/>
       <c r="B36" s="9"/>
-      <c r="C36" s="49"/>
-      <c r="D36" s="50"/>
-      <c r="E36" s="50"/>
-      <c r="F36" s="50"/>
-      <c r="G36" s="50"/>
-      <c r="H36" s="50"/>
-      <c r="I36" s="51"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="58"/>
+      <c r="E36" s="58"/>
+      <c r="F36" s="58"/>
+      <c r="G36" s="58"/>
+      <c r="H36" s="58"/>
+      <c r="I36" s="59"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="56"/>
+      <c r="A37" s="71"/>
       <c r="B37" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="67" t="s">
+      <c r="C37" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="D37" s="68"/>
-      <c r="E37" s="68"/>
-      <c r="F37" s="68"/>
-      <c r="G37" s="68"/>
-      <c r="H37" s="68"/>
-      <c r="I37" s="69"/>
+      <c r="D37" s="89"/>
+      <c r="E37" s="89"/>
+      <c r="F37" s="89"/>
+      <c r="G37" s="89"/>
+      <c r="H37" s="89"/>
+      <c r="I37" s="90"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="56"/>
+      <c r="A38" s="71"/>
       <c r="B38" s="11"/>
       <c r="C38" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D38" s="46" t="s">
+      <c r="D38" s="76" t="s">
         <v>54</v>
       </c>
-      <c r="E38" s="47"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="47"/>
-      <c r="H38" s="47"/>
-      <c r="I38" s="48"/>
+      <c r="E38" s="63"/>
+      <c r="F38" s="63"/>
+      <c r="G38" s="63"/>
+      <c r="H38" s="63"/>
+      <c r="I38" s="64"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="56"/>
+      <c r="A39" s="71"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
-      <c r="D39" s="49"/>
-      <c r="E39" s="50"/>
-      <c r="F39" s="50"/>
-      <c r="G39" s="50"/>
-      <c r="H39" s="50"/>
-      <c r="I39" s="51"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="58"/>
+      <c r="F39" s="58"/>
+      <c r="G39" s="58"/>
+      <c r="H39" s="58"/>
+      <c r="I39" s="59"/>
     </row>
     <row r="40" spans="1:9" ht="18.3" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="56"/>
+      <c r="A40" s="71"/>
       <c r="B40" s="11"/>
       <c r="C40" s="14"/>
-      <c r="D40" s="52"/>
-      <c r="E40" s="53"/>
-      <c r="F40" s="53"/>
-      <c r="G40" s="53"/>
-      <c r="H40" s="53"/>
-      <c r="I40" s="54"/>
+      <c r="D40" s="77"/>
+      <c r="E40" s="78"/>
+      <c r="F40" s="78"/>
+      <c r="G40" s="78"/>
+      <c r="H40" s="78"/>
+      <c r="I40" s="79"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="56"/>
+      <c r="A41" s="71"/>
       <c r="B41" s="11"/>
       <c r="C41" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D41" s="61" t="s">
+      <c r="D41" s="83" t="s">
         <v>56</v>
       </c>
-      <c r="E41" s="62"/>
-      <c r="F41" s="62"/>
-      <c r="G41" s="62"/>
-      <c r="H41" s="62"/>
-      <c r="I41" s="63"/>
+      <c r="E41" s="67"/>
+      <c r="F41" s="67"/>
+      <c r="G41" s="67"/>
+      <c r="H41" s="67"/>
+      <c r="I41" s="84"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="57"/>
+      <c r="A42" s="72"/>
       <c r="B42" s="14"/>
       <c r="C42" s="14"/>
-      <c r="D42" s="64"/>
-      <c r="E42" s="65"/>
-      <c r="F42" s="65"/>
-      <c r="G42" s="65"/>
-      <c r="H42" s="65"/>
-      <c r="I42" s="66"/>
+      <c r="D42" s="85"/>
+      <c r="E42" s="86"/>
+      <c r="F42" s="86"/>
+      <c r="G42" s="86"/>
+      <c r="H42" s="86"/>
+      <c r="I42" s="87"/>
     </row>
     <row r="43" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A43" s="55">
+      <c r="A43" s="70">
         <v>3</v>
       </c>
-      <c r="B43" s="43" t="s">
+      <c r="B43" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="44"/>
-      <c r="D43" s="44"/>
-      <c r="E43" s="44"/>
-      <c r="F43" s="44"/>
-      <c r="G43" s="44"/>
-      <c r="H43" s="44"/>
-      <c r="I43" s="45"/>
+      <c r="C43" s="74"/>
+      <c r="D43" s="74"/>
+      <c r="E43" s="74"/>
+      <c r="F43" s="74"/>
+      <c r="G43" s="74"/>
+      <c r="H43" s="74"/>
+      <c r="I43" s="75"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="56"/>
-      <c r="B44" s="58" t="s">
+      <c r="A44" s="71"/>
+      <c r="B44" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="C44" s="60" t="s">
+      <c r="C44" s="80" t="s">
         <v>57</v>
       </c>
-      <c r="D44" s="46" t="s">
+      <c r="D44" s="76" t="s">
         <v>60</v>
       </c>
-      <c r="E44" s="47"/>
-      <c r="F44" s="47"/>
-      <c r="G44" s="47"/>
-      <c r="H44" s="47"/>
-      <c r="I44" s="48"/>
+      <c r="E44" s="63"/>
+      <c r="F44" s="63"/>
+      <c r="G44" s="63"/>
+      <c r="H44" s="63"/>
+      <c r="I44" s="64"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="56"/>
-      <c r="B45" s="58"/>
-      <c r="C45" s="58"/>
-      <c r="D45" s="49"/>
-      <c r="E45" s="50"/>
-      <c r="F45" s="50"/>
-      <c r="G45" s="50"/>
-      <c r="H45" s="50"/>
-      <c r="I45" s="51"/>
+      <c r="A45" s="71"/>
+      <c r="B45" s="81"/>
+      <c r="C45" s="81"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="58"/>
+      <c r="F45" s="58"/>
+      <c r="G45" s="58"/>
+      <c r="H45" s="58"/>
+      <c r="I45" s="59"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="56"/>
-      <c r="B46" s="58"/>
-      <c r="C46" s="59"/>
-      <c r="D46" s="52"/>
-      <c r="E46" s="53"/>
-      <c r="F46" s="53"/>
-      <c r="G46" s="53"/>
-      <c r="H46" s="53"/>
-      <c r="I46" s="54"/>
+      <c r="A46" s="71"/>
+      <c r="B46" s="81"/>
+      <c r="C46" s="82"/>
+      <c r="D46" s="77"/>
+      <c r="E46" s="78"/>
+      <c r="F46" s="78"/>
+      <c r="G46" s="78"/>
+      <c r="H46" s="78"/>
+      <c r="I46" s="79"/>
     </row>
     <row r="47" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="56"/>
-      <c r="B47" s="58" t="s">
+      <c r="A47" s="71"/>
+      <c r="B47" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="C47" s="60" t="s">
+      <c r="C47" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="D47" s="46" t="s">
+      <c r="D47" s="76" t="s">
         <v>61</v>
       </c>
-      <c r="E47" s="47"/>
-      <c r="F47" s="47"/>
-      <c r="G47" s="47"/>
-      <c r="H47" s="47"/>
-      <c r="I47" s="48"/>
+      <c r="E47" s="63"/>
+      <c r="F47" s="63"/>
+      <c r="G47" s="63"/>
+      <c r="H47" s="63"/>
+      <c r="I47" s="64"/>
     </row>
     <row r="48" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="56"/>
-      <c r="B48" s="58"/>
-      <c r="C48" s="58"/>
-      <c r="D48" s="49"/>
-      <c r="E48" s="50"/>
-      <c r="F48" s="50"/>
-      <c r="G48" s="50"/>
-      <c r="H48" s="50"/>
-      <c r="I48" s="51"/>
+      <c r="A48" s="71"/>
+      <c r="B48" s="81"/>
+      <c r="C48" s="81"/>
+      <c r="D48" s="57"/>
+      <c r="E48" s="58"/>
+      <c r="F48" s="58"/>
+      <c r="G48" s="58"/>
+      <c r="H48" s="58"/>
+      <c r="I48" s="59"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="56"/>
-      <c r="B49" s="58"/>
-      <c r="C49" s="59"/>
-      <c r="D49" s="52"/>
-      <c r="E49" s="53"/>
-      <c r="F49" s="53"/>
-      <c r="G49" s="53"/>
-      <c r="H49" s="53"/>
-      <c r="I49" s="54"/>
+      <c r="A49" s="71"/>
+      <c r="B49" s="81"/>
+      <c r="C49" s="82"/>
+      <c r="D49" s="77"/>
+      <c r="E49" s="78"/>
+      <c r="F49" s="78"/>
+      <c r="G49" s="78"/>
+      <c r="H49" s="78"/>
+      <c r="I49" s="79"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="56"/>
-      <c r="B50" s="58" t="s">
+      <c r="A50" s="71"/>
+      <c r="B50" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="C50" s="58" t="s">
+      <c r="C50" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="D50" s="46" t="s">
+      <c r="D50" s="76" t="s">
         <v>63</v>
       </c>
-      <c r="E50" s="47"/>
-      <c r="F50" s="47"/>
-      <c r="G50" s="47"/>
-      <c r="H50" s="47"/>
-      <c r="I50" s="48"/>
+      <c r="E50" s="63"/>
+      <c r="F50" s="63"/>
+      <c r="G50" s="63"/>
+      <c r="H50" s="63"/>
+      <c r="I50" s="64"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="56"/>
-      <c r="B51" s="58"/>
-      <c r="C51" s="58"/>
-      <c r="D51" s="49"/>
-      <c r="E51" s="50"/>
-      <c r="F51" s="50"/>
-      <c r="G51" s="50"/>
-      <c r="H51" s="50"/>
-      <c r="I51" s="51"/>
+      <c r="A51" s="71"/>
+      <c r="B51" s="81"/>
+      <c r="C51" s="81"/>
+      <c r="D51" s="57"/>
+      <c r="E51" s="58"/>
+      <c r="F51" s="58"/>
+      <c r="G51" s="58"/>
+      <c r="H51" s="58"/>
+      <c r="I51" s="59"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="57"/>
-      <c r="B52" s="59"/>
-      <c r="C52" s="59"/>
-      <c r="D52" s="52"/>
-      <c r="E52" s="53"/>
-      <c r="F52" s="53"/>
-      <c r="G52" s="53"/>
-      <c r="H52" s="53"/>
-      <c r="I52" s="54"/>
+      <c r="A52" s="72"/>
+      <c r="B52" s="82"/>
+      <c r="C52" s="82"/>
+      <c r="D52" s="77"/>
+      <c r="E52" s="78"/>
+      <c r="F52" s="78"/>
+      <c r="G52" s="78"/>
+      <c r="H52" s="78"/>
+      <c r="I52" s="79"/>
     </row>
     <row r="53" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A53" s="55">
+      <c r="A53" s="70">
         <v>4</v>
       </c>
-      <c r="B53" s="43" t="s">
+      <c r="B53" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="C53" s="44"/>
-      <c r="D53" s="44"/>
-      <c r="E53" s="44"/>
-      <c r="F53" s="44"/>
-      <c r="G53" s="44"/>
-      <c r="H53" s="44"/>
-      <c r="I53" s="45"/>
+      <c r="C53" s="74"/>
+      <c r="D53" s="74"/>
+      <c r="E53" s="74"/>
+      <c r="F53" s="74"/>
+      <c r="G53" s="74"/>
+      <c r="H53" s="74"/>
+      <c r="I53" s="75"/>
     </row>
     <row r="54" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="56"/>
-      <c r="B54" s="56" t="s">
+      <c r="A54" s="71"/>
+      <c r="B54" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="C54" s="46" t="s">
+      <c r="C54" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="D54" s="47"/>
-      <c r="E54" s="47"/>
-      <c r="F54" s="47"/>
-      <c r="G54" s="47"/>
-      <c r="H54" s="47"/>
-      <c r="I54" s="48"/>
+      <c r="D54" s="63"/>
+      <c r="E54" s="63"/>
+      <c r="F54" s="63"/>
+      <c r="G54" s="63"/>
+      <c r="H54" s="63"/>
+      <c r="I54" s="64"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="56"/>
-      <c r="B55" s="56"/>
-      <c r="C55" s="49"/>
-      <c r="D55" s="50"/>
-      <c r="E55" s="50"/>
-      <c r="F55" s="50"/>
-      <c r="G55" s="50"/>
-      <c r="H55" s="50"/>
-      <c r="I55" s="51"/>
+      <c r="A55" s="71"/>
+      <c r="B55" s="71"/>
+      <c r="C55" s="57"/>
+      <c r="D55" s="58"/>
+      <c r="E55" s="58"/>
+      <c r="F55" s="58"/>
+      <c r="G55" s="58"/>
+      <c r="H55" s="58"/>
+      <c r="I55" s="59"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="56"/>
-      <c r="B56" s="56"/>
-      <c r="C56" s="49"/>
-      <c r="D56" s="50"/>
-      <c r="E56" s="50"/>
-      <c r="F56" s="50"/>
-      <c r="G56" s="50"/>
-      <c r="H56" s="50"/>
-      <c r="I56" s="51"/>
+      <c r="A56" s="71"/>
+      <c r="B56" s="71"/>
+      <c r="C56" s="57"/>
+      <c r="D56" s="58"/>
+      <c r="E56" s="58"/>
+      <c r="F56" s="58"/>
+      <c r="G56" s="58"/>
+      <c r="H56" s="58"/>
+      <c r="I56" s="59"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="56"/>
-      <c r="B57" s="56"/>
-      <c r="C57" s="49"/>
-      <c r="D57" s="50"/>
-      <c r="E57" s="50"/>
-      <c r="F57" s="50"/>
-      <c r="G57" s="50"/>
-      <c r="H57" s="50"/>
-      <c r="I57" s="51"/>
+      <c r="A57" s="71"/>
+      <c r="B57" s="71"/>
+      <c r="C57" s="57"/>
+      <c r="D57" s="58"/>
+      <c r="E57" s="58"/>
+      <c r="F57" s="58"/>
+      <c r="G57" s="58"/>
+      <c r="H57" s="58"/>
+      <c r="I57" s="59"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="56"/>
-      <c r="B58" s="56"/>
-      <c r="C58" s="49"/>
-      <c r="D58" s="50"/>
-      <c r="E58" s="50"/>
-      <c r="F58" s="50"/>
-      <c r="G58" s="50"/>
-      <c r="H58" s="50"/>
-      <c r="I58" s="51"/>
+      <c r="A58" s="71"/>
+      <c r="B58" s="71"/>
+      <c r="C58" s="57"/>
+      <c r="D58" s="58"/>
+      <c r="E58" s="58"/>
+      <c r="F58" s="58"/>
+      <c r="G58" s="58"/>
+      <c r="H58" s="58"/>
+      <c r="I58" s="59"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="56"/>
-      <c r="B59" s="56"/>
-      <c r="C59" s="49"/>
-      <c r="D59" s="50"/>
-      <c r="E59" s="50"/>
-      <c r="F59" s="50"/>
-      <c r="G59" s="50"/>
-      <c r="H59" s="50"/>
-      <c r="I59" s="51"/>
+      <c r="A59" s="71"/>
+      <c r="B59" s="71"/>
+      <c r="C59" s="57"/>
+      <c r="D59" s="58"/>
+      <c r="E59" s="58"/>
+      <c r="F59" s="58"/>
+      <c r="G59" s="58"/>
+      <c r="H59" s="58"/>
+      <c r="I59" s="59"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="56"/>
-      <c r="B60" s="56"/>
-      <c r="C60" s="49"/>
-      <c r="D60" s="50"/>
-      <c r="E60" s="50"/>
-      <c r="F60" s="50"/>
-      <c r="G60" s="50"/>
-      <c r="H60" s="50"/>
-      <c r="I60" s="51"/>
+      <c r="A60" s="71"/>
+      <c r="B60" s="71"/>
+      <c r="C60" s="57"/>
+      <c r="D60" s="58"/>
+      <c r="E60" s="58"/>
+      <c r="F60" s="58"/>
+      <c r="G60" s="58"/>
+      <c r="H60" s="58"/>
+      <c r="I60" s="59"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="56"/>
-      <c r="B61" s="56"/>
-      <c r="C61" s="49"/>
-      <c r="D61" s="50"/>
-      <c r="E61" s="50"/>
-      <c r="F61" s="50"/>
-      <c r="G61" s="50"/>
-      <c r="H61" s="50"/>
-      <c r="I61" s="51"/>
+      <c r="A61" s="71"/>
+      <c r="B61" s="71"/>
+      <c r="C61" s="57"/>
+      <c r="D61" s="58"/>
+      <c r="E61" s="58"/>
+      <c r="F61" s="58"/>
+      <c r="G61" s="58"/>
+      <c r="H61" s="58"/>
+      <c r="I61" s="59"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="56"/>
-      <c r="B62" s="56"/>
-      <c r="C62" s="49"/>
-      <c r="D62" s="50"/>
-      <c r="E62" s="50"/>
-      <c r="F62" s="50"/>
-      <c r="G62" s="50"/>
-      <c r="H62" s="50"/>
-      <c r="I62" s="51"/>
+      <c r="A62" s="71"/>
+      <c r="B62" s="71"/>
+      <c r="C62" s="57"/>
+      <c r="D62" s="58"/>
+      <c r="E62" s="58"/>
+      <c r="F62" s="58"/>
+      <c r="G62" s="58"/>
+      <c r="H62" s="58"/>
+      <c r="I62" s="59"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="57"/>
-      <c r="B63" s="57"/>
-      <c r="C63" s="52"/>
-      <c r="D63" s="53"/>
-      <c r="E63" s="53"/>
-      <c r="F63" s="53"/>
-      <c r="G63" s="53"/>
-      <c r="H63" s="53"/>
-      <c r="I63" s="54"/>
+      <c r="A63" s="72"/>
+      <c r="B63" s="72"/>
+      <c r="C63" s="77"/>
+      <c r="D63" s="78"/>
+      <c r="E63" s="78"/>
+      <c r="F63" s="78"/>
+      <c r="G63" s="78"/>
+      <c r="H63" s="78"/>
+      <c r="I63" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="A19:A29"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I9"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A11:I18"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="E28:I28"/>
-    <mergeCell ref="E29:I29"/>
+    <mergeCell ref="B53:I53"/>
+    <mergeCell ref="C54:I63"/>
+    <mergeCell ref="A53:A63"/>
+    <mergeCell ref="B54:B63"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="A43:A52"/>
     <mergeCell ref="A30:A42"/>
     <mergeCell ref="B43:I43"/>
     <mergeCell ref="D47:I49"/>
@@ -3286,14 +3268,32 @@
     <mergeCell ref="D44:I46"/>
     <mergeCell ref="B30:I30"/>
     <mergeCell ref="C37:I37"/>
-    <mergeCell ref="B53:I53"/>
-    <mergeCell ref="C54:I63"/>
-    <mergeCell ref="A53:A63"/>
-    <mergeCell ref="B54:B63"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="A43:A52"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="E29:I29"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I9"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A11:I18"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="A19:A29"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -8110,8 +8110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF3FB38F-39BD-477F-A58E-198477386216}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="E17" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8180,7 +8180,7 @@
         <v>12</v>
       </c>
       <c r="G2" s="37" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H2" s="37" t="s">
         <v>180</v>
@@ -8266,10 +8266,10 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="H7" s="8" t="s">
         <v>454</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>455</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
@@ -8290,7 +8290,7 @@
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -8298,15 +8298,15 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2" t="s">
-        <v>457</v>
+        <v>473</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -8314,10 +8314,10 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2" t="s">
-        <v>459</v>
+        <v>474</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -8330,10 +8330,10 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="8" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
@@ -8346,15 +8346,15 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="216" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -8362,15 +8362,15 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
-        <v>465</v>
+        <v>475</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -8378,10 +8378,10 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2" t="s">
-        <v>467</v>
+        <v>476</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
@@ -8407,20 +8407,20 @@
         <v>371</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
     </row>
     <row r="17" spans="7:8" ht="230.4" x14ac:dyDescent="0.3">
       <c r="G17" s="2" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
     </row>
     <row r="18" spans="7:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="G18" s="2" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>425</v>
@@ -8452,10 +8452,10 @@
     </row>
     <row r="22" spans="7:8" ht="144" x14ac:dyDescent="0.3">
       <c r="G22" s="2" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
     </row>
   </sheetData>
@@ -8538,7 +8538,7 @@
         <v>12</v>
       </c>
       <c r="G2" s="37" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H2" s="37" t="s">
         <v>180</v>
@@ -8868,7 +8868,7 @@
     </row>
     <row r="29" spans="7:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="G29" s="2" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>386</v>
@@ -8958,7 +8958,7 @@
         <v>12</v>
       </c>
       <c r="G2" s="37" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H2" s="37" t="s">
         <v>180</v>
@@ -9524,7 +9524,7 @@
         <v>149</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>

</xml_diff>